<commit_message>
Add admin dashboard and website router
Introduces website.js to provide an admin dashboard at /admin, displaying users.xlsx and logs.xlsx data after email authentication. Refactors server.js to mount the website router and exposes helpers for user and log data. Minor improvements and clarifications in comments and route lists.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/logs.xlsx
+++ b/Server/rfid-server-DBS-Http/logs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2921" uniqueCount="367">
   <si>
     <t>Timestamp</t>
   </si>
@@ -734,6 +734,384 @@
   </si>
   <si>
     <t>2025-11-24T21:16:30.521Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:17:52.871Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:17:52.921Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:18:04.077Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:18:04.140Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:39:54.732Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:39:54.758Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:44:58.360Z</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Health check</t>
+  </si>
+  <si>
+    <t>::1</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:44:58.567Z</t>
+  </si>
+  <si>
+    <t>/favicon.ico</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:45:27.788Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:45:37.629Z</t>
+  </si>
+  <si>
+    <t>/admin</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:45:44.108Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:45:53.343Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:46:52.289Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:46:52.335Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:46:56.715Z</t>
+  </si>
+  <si>
+    <t>/user/6BF02F00?roomID=104</t>
+  </si>
+  <si>
+    <t>Access denied for room 104</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:46:57.041Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:03.592Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:06.329Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:06.445Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:13.068Z</t>
+  </si>
+  <si>
+    <t>/user/835DF613?roomID=104</t>
+  </si>
+  <si>
+    <t>UID 835DF613 not found in /user</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:13.110Z</t>
+  </si>
+  <si>
+    <t>/uid-name/835DF613</t>
+  </si>
+  <si>
+    <t>UID 835DF613 not found in /uid-name</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:20.753Z</t>
+  </si>
+  <si>
+    <t>GGG</t>
+  </si>
+  <si>
+    <t>835DF613</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:22.927Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:23.422Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:27.560Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:30.011Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:30.060Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:36.960Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:37.009Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:39.187Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:39.246Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:49.558Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:49.606Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:55.231Z</t>
+  </si>
+  <si>
+    <t>/room/835DF613/104</t>
+  </si>
+  <si>
+    <t>User deleted because no rooms remain</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:47:58.345Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:04.120Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:10.895Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:14.064Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:14.100Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:22.754Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:25.689Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:30.430Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:30.596Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:32.719Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:34.152Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:34.175Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:35.100Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:35.173Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:35.839Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:35.886Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:37.143Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:37.170Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:37.594Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:37.622Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:37.989Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:38.078Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:40.038Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:41.854Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:41.896Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:42.738Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:42.777Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:43.241Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:43.301Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:43.885Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:44.046Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:45.029Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:47.752Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:47.835Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:49.184Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:49.226Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:53.378Z</t>
+  </si>
+  <si>
+    <t>/user/6BF02F00?roomID=103</t>
+  </si>
+  <si>
+    <t>Access denied for room 103</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:53.435Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:57.795Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:58.257Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:58.328Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:59.500Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:48:59.864Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:03.201Z</t>
+  </si>
+  <si>
+    <t>/user/6BF02F00?roomID=101</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>Access denied for room 101</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:03.367Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:06.684Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:07.875Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:08.066Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:08.291Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:08.334Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:10.383Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:15.308Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:15.346Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:23.898Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:26.537Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:28.654Z</t>
+  </si>
+  <si>
+    <t>/user/835DF613?roomID=101</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:28.685Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:30.902Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:31.554Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:31.602Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:32.024Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:32.062Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:32.515Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:32.555Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:32.889Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:32.954Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:33.503Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:33.573Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:33.892Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:34.088Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:49:34.960Z</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K187"/>
+  <dimension ref="A1:K292"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -7658,6 +8036,3681 @@
         <v>19</v>
       </c>
     </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>241</v>
+      </c>
+      <c r="B188" t="s">
+        <v>12</v>
+      </c>
+      <c r="C188" t="s">
+        <v>13</v>
+      </c>
+      <c r="D188" t="s">
+        <v>93</v>
+      </c>
+      <c r="E188">
+        <v>200</v>
+      </c>
+      <c r="F188" t="s">
+        <v>30</v>
+      </c>
+      <c r="G188" t="s">
+        <v>177</v>
+      </c>
+      <c r="H188" t="s">
+        <v>32</v>
+      </c>
+      <c r="I188" t="s">
+        <v>43</v>
+      </c>
+      <c r="J188" t="s">
+        <v>37</v>
+      </c>
+      <c r="K188" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>242</v>
+      </c>
+      <c r="B189" t="s">
+        <v>12</v>
+      </c>
+      <c r="C189" t="s">
+        <v>13</v>
+      </c>
+      <c r="D189" t="s">
+        <v>21</v>
+      </c>
+      <c r="E189">
+        <v>200</v>
+      </c>
+      <c r="F189" t="s">
+        <v>30</v>
+      </c>
+      <c r="G189" t="s">
+        <v>177</v>
+      </c>
+      <c r="H189" t="s">
+        <v>32</v>
+      </c>
+      <c r="I189" t="s">
+        <v>16</v>
+      </c>
+      <c r="J189" t="s">
+        <v>39</v>
+      </c>
+      <c r="K189" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>243</v>
+      </c>
+      <c r="B190" t="s">
+        <v>12</v>
+      </c>
+      <c r="C190" t="s">
+        <v>13</v>
+      </c>
+      <c r="D190" t="s">
+        <v>93</v>
+      </c>
+      <c r="E190">
+        <v>200</v>
+      </c>
+      <c r="F190" t="s">
+        <v>30</v>
+      </c>
+      <c r="G190" t="s">
+        <v>177</v>
+      </c>
+      <c r="H190" t="s">
+        <v>32</v>
+      </c>
+      <c r="I190" t="s">
+        <v>43</v>
+      </c>
+      <c r="J190" t="s">
+        <v>37</v>
+      </c>
+      <c r="K190" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>244</v>
+      </c>
+      <c r="B191" t="s">
+        <v>12</v>
+      </c>
+      <c r="C191" t="s">
+        <v>13</v>
+      </c>
+      <c r="D191" t="s">
+        <v>21</v>
+      </c>
+      <c r="E191">
+        <v>200</v>
+      </c>
+      <c r="F191" t="s">
+        <v>30</v>
+      </c>
+      <c r="G191" t="s">
+        <v>177</v>
+      </c>
+      <c r="H191" t="s">
+        <v>32</v>
+      </c>
+      <c r="I191" t="s">
+        <v>16</v>
+      </c>
+      <c r="J191" t="s">
+        <v>39</v>
+      </c>
+      <c r="K191" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>245</v>
+      </c>
+      <c r="B192" t="s">
+        <v>12</v>
+      </c>
+      <c r="C192" t="s">
+        <v>13</v>
+      </c>
+      <c r="D192" t="s">
+        <v>93</v>
+      </c>
+      <c r="E192">
+        <v>200</v>
+      </c>
+      <c r="F192" t="s">
+        <v>30</v>
+      </c>
+      <c r="G192" t="s">
+        <v>177</v>
+      </c>
+      <c r="H192" t="s">
+        <v>32</v>
+      </c>
+      <c r="I192" t="s">
+        <v>43</v>
+      </c>
+      <c r="J192" t="s">
+        <v>37</v>
+      </c>
+      <c r="K192" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>246</v>
+      </c>
+      <c r="B193" t="s">
+        <v>12</v>
+      </c>
+      <c r="C193" t="s">
+        <v>13</v>
+      </c>
+      <c r="D193" t="s">
+        <v>21</v>
+      </c>
+      <c r="E193">
+        <v>200</v>
+      </c>
+      <c r="F193" t="s">
+        <v>30</v>
+      </c>
+      <c r="G193" t="s">
+        <v>177</v>
+      </c>
+      <c r="H193" t="s">
+        <v>32</v>
+      </c>
+      <c r="I193" t="s">
+        <v>16</v>
+      </c>
+      <c r="J193" t="s">
+        <v>39</v>
+      </c>
+      <c r="K193" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>247</v>
+      </c>
+      <c r="B194" t="s">
+        <v>12</v>
+      </c>
+      <c r="C194" t="s">
+        <v>13</v>
+      </c>
+      <c r="D194" t="s">
+        <v>248</v>
+      </c>
+      <c r="E194">
+        <v>200</v>
+      </c>
+      <c r="F194" t="s">
+        <v>30</v>
+      </c>
+      <c r="G194" t="s">
+        <v>16</v>
+      </c>
+      <c r="H194" t="s">
+        <v>16</v>
+      </c>
+      <c r="I194" t="s">
+        <v>16</v>
+      </c>
+      <c r="J194" t="s">
+        <v>249</v>
+      </c>
+      <c r="K194" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>251</v>
+      </c>
+      <c r="B195" t="s">
+        <v>12</v>
+      </c>
+      <c r="C195" t="s">
+        <v>13</v>
+      </c>
+      <c r="D195" t="s">
+        <v>252</v>
+      </c>
+      <c r="E195">
+        <v>404</v>
+      </c>
+      <c r="F195" t="s">
+        <v>15</v>
+      </c>
+      <c r="G195" t="s">
+        <v>16</v>
+      </c>
+      <c r="H195" t="s">
+        <v>16</v>
+      </c>
+      <c r="I195" t="s">
+        <v>16</v>
+      </c>
+      <c r="J195" t="s">
+        <v>16</v>
+      </c>
+      <c r="K195" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>253</v>
+      </c>
+      <c r="B196" t="s">
+        <v>12</v>
+      </c>
+      <c r="C196" t="s">
+        <v>13</v>
+      </c>
+      <c r="D196" t="s">
+        <v>248</v>
+      </c>
+      <c r="E196">
+        <v>304</v>
+      </c>
+      <c r="F196" t="s">
+        <v>30</v>
+      </c>
+      <c r="G196" t="s">
+        <v>16</v>
+      </c>
+      <c r="H196" t="s">
+        <v>16</v>
+      </c>
+      <c r="I196" t="s">
+        <v>16</v>
+      </c>
+      <c r="J196" t="s">
+        <v>249</v>
+      </c>
+      <c r="K196" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>254</v>
+      </c>
+      <c r="B197" t="s">
+        <v>12</v>
+      </c>
+      <c r="C197" t="s">
+        <v>13</v>
+      </c>
+      <c r="D197" t="s">
+        <v>255</v>
+      </c>
+      <c r="E197">
+        <v>200</v>
+      </c>
+      <c r="F197" t="s">
+        <v>30</v>
+      </c>
+      <c r="G197" t="s">
+        <v>16</v>
+      </c>
+      <c r="H197" t="s">
+        <v>16</v>
+      </c>
+      <c r="I197" t="s">
+        <v>16</v>
+      </c>
+      <c r="J197" t="s">
+        <v>16</v>
+      </c>
+      <c r="K197" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>256</v>
+      </c>
+      <c r="B198" t="s">
+        <v>12</v>
+      </c>
+      <c r="C198" t="s">
+        <v>28</v>
+      </c>
+      <c r="D198" t="s">
+        <v>255</v>
+      </c>
+      <c r="E198">
+        <v>200</v>
+      </c>
+      <c r="F198" t="s">
+        <v>30</v>
+      </c>
+      <c r="G198" t="s">
+        <v>16</v>
+      </c>
+      <c r="H198" t="s">
+        <v>16</v>
+      </c>
+      <c r="I198" t="s">
+        <v>16</v>
+      </c>
+      <c r="J198" t="s">
+        <v>16</v>
+      </c>
+      <c r="K198" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>257</v>
+      </c>
+      <c r="B199" t="s">
+        <v>12</v>
+      </c>
+      <c r="C199" t="s">
+        <v>28</v>
+      </c>
+      <c r="D199" t="s">
+        <v>255</v>
+      </c>
+      <c r="E199">
+        <v>200</v>
+      </c>
+      <c r="F199" t="s">
+        <v>30</v>
+      </c>
+      <c r="G199" t="s">
+        <v>16</v>
+      </c>
+      <c r="H199" t="s">
+        <v>16</v>
+      </c>
+      <c r="I199" t="s">
+        <v>16</v>
+      </c>
+      <c r="J199" t="s">
+        <v>16</v>
+      </c>
+      <c r="K199" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>258</v>
+      </c>
+      <c r="B200" t="s">
+        <v>12</v>
+      </c>
+      <c r="C200" t="s">
+        <v>13</v>
+      </c>
+      <c r="D200" t="s">
+        <v>93</v>
+      </c>
+      <c r="E200">
+        <v>200</v>
+      </c>
+      <c r="F200" t="s">
+        <v>30</v>
+      </c>
+      <c r="G200" t="s">
+        <v>177</v>
+      </c>
+      <c r="H200" t="s">
+        <v>32</v>
+      </c>
+      <c r="I200" t="s">
+        <v>43</v>
+      </c>
+      <c r="J200" t="s">
+        <v>37</v>
+      </c>
+      <c r="K200" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>259</v>
+      </c>
+      <c r="B201" t="s">
+        <v>12</v>
+      </c>
+      <c r="C201" t="s">
+        <v>13</v>
+      </c>
+      <c r="D201" t="s">
+        <v>21</v>
+      </c>
+      <c r="E201">
+        <v>200</v>
+      </c>
+      <c r="F201" t="s">
+        <v>30</v>
+      </c>
+      <c r="G201" t="s">
+        <v>177</v>
+      </c>
+      <c r="H201" t="s">
+        <v>32</v>
+      </c>
+      <c r="I201" t="s">
+        <v>16</v>
+      </c>
+      <c r="J201" t="s">
+        <v>39</v>
+      </c>
+      <c r="K201" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>260</v>
+      </c>
+      <c r="B202" t="s">
+        <v>12</v>
+      </c>
+      <c r="C202" t="s">
+        <v>13</v>
+      </c>
+      <c r="D202" t="s">
+        <v>261</v>
+      </c>
+      <c r="E202">
+        <v>403</v>
+      </c>
+      <c r="F202" t="s">
+        <v>15</v>
+      </c>
+      <c r="G202" t="s">
+        <v>177</v>
+      </c>
+      <c r="H202" t="s">
+        <v>32</v>
+      </c>
+      <c r="I202" t="s">
+        <v>45</v>
+      </c>
+      <c r="J202" t="s">
+        <v>262</v>
+      </c>
+      <c r="K202" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>263</v>
+      </c>
+      <c r="B203" t="s">
+        <v>12</v>
+      </c>
+      <c r="C203" t="s">
+        <v>13</v>
+      </c>
+      <c r="D203" t="s">
+        <v>21</v>
+      </c>
+      <c r="E203">
+        <v>200</v>
+      </c>
+      <c r="F203" t="s">
+        <v>30</v>
+      </c>
+      <c r="G203" t="s">
+        <v>177</v>
+      </c>
+      <c r="H203" t="s">
+        <v>32</v>
+      </c>
+      <c r="I203" t="s">
+        <v>16</v>
+      </c>
+      <c r="J203" t="s">
+        <v>39</v>
+      </c>
+      <c r="K203" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>264</v>
+      </c>
+      <c r="B204" t="s">
+        <v>12</v>
+      </c>
+      <c r="C204" t="s">
+        <v>28</v>
+      </c>
+      <c r="D204" t="s">
+        <v>29</v>
+      </c>
+      <c r="E204">
+        <v>200</v>
+      </c>
+      <c r="F204" t="s">
+        <v>30</v>
+      </c>
+      <c r="G204" t="s">
+        <v>177</v>
+      </c>
+      <c r="H204" t="s">
+        <v>32</v>
+      </c>
+      <c r="I204" t="s">
+        <v>45</v>
+      </c>
+      <c r="J204" t="s">
+        <v>41</v>
+      </c>
+      <c r="K204" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>265</v>
+      </c>
+      <c r="B205" t="s">
+        <v>12</v>
+      </c>
+      <c r="C205" t="s">
+        <v>13</v>
+      </c>
+      <c r="D205" t="s">
+        <v>261</v>
+      </c>
+      <c r="E205">
+        <v>200</v>
+      </c>
+      <c r="F205" t="s">
+        <v>30</v>
+      </c>
+      <c r="G205" t="s">
+        <v>177</v>
+      </c>
+      <c r="H205" t="s">
+        <v>32</v>
+      </c>
+      <c r="I205" t="s">
+        <v>45</v>
+      </c>
+      <c r="J205" t="s">
+        <v>37</v>
+      </c>
+      <c r="K205" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>266</v>
+      </c>
+      <c r="B206" t="s">
+        <v>12</v>
+      </c>
+      <c r="C206" t="s">
+        <v>13</v>
+      </c>
+      <c r="D206" t="s">
+        <v>21</v>
+      </c>
+      <c r="E206">
+        <v>200</v>
+      </c>
+      <c r="F206" t="s">
+        <v>30</v>
+      </c>
+      <c r="G206" t="s">
+        <v>177</v>
+      </c>
+      <c r="H206" t="s">
+        <v>32</v>
+      </c>
+      <c r="I206" t="s">
+        <v>16</v>
+      </c>
+      <c r="J206" t="s">
+        <v>39</v>
+      </c>
+      <c r="K206" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>267</v>
+      </c>
+      <c r="B207" t="s">
+        <v>12</v>
+      </c>
+      <c r="C207" t="s">
+        <v>13</v>
+      </c>
+      <c r="D207" t="s">
+        <v>268</v>
+      </c>
+      <c r="E207">
+        <v>404</v>
+      </c>
+      <c r="F207" t="s">
+        <v>15</v>
+      </c>
+      <c r="G207" t="s">
+        <v>16</v>
+      </c>
+      <c r="H207" t="s">
+        <v>16</v>
+      </c>
+      <c r="I207" t="s">
+        <v>45</v>
+      </c>
+      <c r="J207" t="s">
+        <v>269</v>
+      </c>
+      <c r="K207" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>270</v>
+      </c>
+      <c r="B208" t="s">
+        <v>12</v>
+      </c>
+      <c r="C208" t="s">
+        <v>13</v>
+      </c>
+      <c r="D208" t="s">
+        <v>271</v>
+      </c>
+      <c r="E208">
+        <v>404</v>
+      </c>
+      <c r="F208" t="s">
+        <v>15</v>
+      </c>
+      <c r="G208" t="s">
+        <v>16</v>
+      </c>
+      <c r="H208" t="s">
+        <v>16</v>
+      </c>
+      <c r="I208" t="s">
+        <v>16</v>
+      </c>
+      <c r="J208" t="s">
+        <v>272</v>
+      </c>
+      <c r="K208" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>273</v>
+      </c>
+      <c r="B209" t="s">
+        <v>12</v>
+      </c>
+      <c r="C209" t="s">
+        <v>28</v>
+      </c>
+      <c r="D209" t="s">
+        <v>29</v>
+      </c>
+      <c r="E209">
+        <v>200</v>
+      </c>
+      <c r="F209" t="s">
+        <v>30</v>
+      </c>
+      <c r="G209" t="s">
+        <v>274</v>
+      </c>
+      <c r="H209" t="s">
+        <v>275</v>
+      </c>
+      <c r="I209" t="s">
+        <v>45</v>
+      </c>
+      <c r="J209" t="s">
+        <v>34</v>
+      </c>
+      <c r="K209" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>276</v>
+      </c>
+      <c r="B210" t="s">
+        <v>12</v>
+      </c>
+      <c r="C210" t="s">
+        <v>13</v>
+      </c>
+      <c r="D210" t="s">
+        <v>268</v>
+      </c>
+      <c r="E210">
+        <v>200</v>
+      </c>
+      <c r="F210" t="s">
+        <v>30</v>
+      </c>
+      <c r="G210" t="s">
+        <v>274</v>
+      </c>
+      <c r="H210" t="s">
+        <v>275</v>
+      </c>
+      <c r="I210" t="s">
+        <v>45</v>
+      </c>
+      <c r="J210" t="s">
+        <v>37</v>
+      </c>
+      <c r="K210" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>277</v>
+      </c>
+      <c r="B211" t="s">
+        <v>12</v>
+      </c>
+      <c r="C211" t="s">
+        <v>13</v>
+      </c>
+      <c r="D211" t="s">
+        <v>271</v>
+      </c>
+      <c r="E211">
+        <v>200</v>
+      </c>
+      <c r="F211" t="s">
+        <v>30</v>
+      </c>
+      <c r="G211" t="s">
+        <v>274</v>
+      </c>
+      <c r="H211" t="s">
+        <v>275</v>
+      </c>
+      <c r="I211" t="s">
+        <v>16</v>
+      </c>
+      <c r="J211" t="s">
+        <v>39</v>
+      </c>
+      <c r="K211" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>278</v>
+      </c>
+      <c r="B212" t="s">
+        <v>12</v>
+      </c>
+      <c r="C212" t="s">
+        <v>28</v>
+      </c>
+      <c r="D212" t="s">
+        <v>255</v>
+      </c>
+      <c r="E212">
+        <v>200</v>
+      </c>
+      <c r="F212" t="s">
+        <v>30</v>
+      </c>
+      <c r="G212" t="s">
+        <v>16</v>
+      </c>
+      <c r="H212" t="s">
+        <v>16</v>
+      </c>
+      <c r="I212" t="s">
+        <v>16</v>
+      </c>
+      <c r="J212" t="s">
+        <v>16</v>
+      </c>
+      <c r="K212" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>279</v>
+      </c>
+      <c r="B213" t="s">
+        <v>12</v>
+      </c>
+      <c r="C213" t="s">
+        <v>13</v>
+      </c>
+      <c r="D213" t="s">
+        <v>268</v>
+      </c>
+      <c r="E213">
+        <v>200</v>
+      </c>
+      <c r="F213" t="s">
+        <v>30</v>
+      </c>
+      <c r="G213" t="s">
+        <v>274</v>
+      </c>
+      <c r="H213" t="s">
+        <v>275</v>
+      </c>
+      <c r="I213" t="s">
+        <v>45</v>
+      </c>
+      <c r="J213" t="s">
+        <v>37</v>
+      </c>
+      <c r="K213" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>280</v>
+      </c>
+      <c r="B214" t="s">
+        <v>12</v>
+      </c>
+      <c r="C214" t="s">
+        <v>13</v>
+      </c>
+      <c r="D214" t="s">
+        <v>271</v>
+      </c>
+      <c r="E214">
+        <v>200</v>
+      </c>
+      <c r="F214" t="s">
+        <v>30</v>
+      </c>
+      <c r="G214" t="s">
+        <v>274</v>
+      </c>
+      <c r="H214" t="s">
+        <v>275</v>
+      </c>
+      <c r="I214" t="s">
+        <v>16</v>
+      </c>
+      <c r="J214" t="s">
+        <v>39</v>
+      </c>
+      <c r="K214" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>281</v>
+      </c>
+      <c r="B215" t="s">
+        <v>12</v>
+      </c>
+      <c r="C215" t="s">
+        <v>13</v>
+      </c>
+      <c r="D215" t="s">
+        <v>268</v>
+      </c>
+      <c r="E215">
+        <v>200</v>
+      </c>
+      <c r="F215" t="s">
+        <v>30</v>
+      </c>
+      <c r="G215" t="s">
+        <v>274</v>
+      </c>
+      <c r="H215" t="s">
+        <v>275</v>
+      </c>
+      <c r="I215" t="s">
+        <v>45</v>
+      </c>
+      <c r="J215" t="s">
+        <v>37</v>
+      </c>
+      <c r="K215" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>282</v>
+      </c>
+      <c r="B216" t="s">
+        <v>12</v>
+      </c>
+      <c r="C216" t="s">
+        <v>13</v>
+      </c>
+      <c r="D216" t="s">
+        <v>271</v>
+      </c>
+      <c r="E216">
+        <v>200</v>
+      </c>
+      <c r="F216" t="s">
+        <v>30</v>
+      </c>
+      <c r="G216" t="s">
+        <v>274</v>
+      </c>
+      <c r="H216" t="s">
+        <v>275</v>
+      </c>
+      <c r="I216" t="s">
+        <v>16</v>
+      </c>
+      <c r="J216" t="s">
+        <v>39</v>
+      </c>
+      <c r="K216" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>283</v>
+      </c>
+      <c r="B217" t="s">
+        <v>12</v>
+      </c>
+      <c r="C217" t="s">
+        <v>13</v>
+      </c>
+      <c r="D217" t="s">
+        <v>268</v>
+      </c>
+      <c r="E217">
+        <v>200</v>
+      </c>
+      <c r="F217" t="s">
+        <v>30</v>
+      </c>
+      <c r="G217" t="s">
+        <v>274</v>
+      </c>
+      <c r="H217" t="s">
+        <v>275</v>
+      </c>
+      <c r="I217" t="s">
+        <v>45</v>
+      </c>
+      <c r="J217" t="s">
+        <v>37</v>
+      </c>
+      <c r="K217" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>284</v>
+      </c>
+      <c r="B218" t="s">
+        <v>12</v>
+      </c>
+      <c r="C218" t="s">
+        <v>13</v>
+      </c>
+      <c r="D218" t="s">
+        <v>271</v>
+      </c>
+      <c r="E218">
+        <v>200</v>
+      </c>
+      <c r="F218" t="s">
+        <v>30</v>
+      </c>
+      <c r="G218" t="s">
+        <v>274</v>
+      </c>
+      <c r="H218" t="s">
+        <v>275</v>
+      </c>
+      <c r="I218" t="s">
+        <v>16</v>
+      </c>
+      <c r="J218" t="s">
+        <v>39</v>
+      </c>
+      <c r="K218" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>285</v>
+      </c>
+      <c r="B219" t="s">
+        <v>12</v>
+      </c>
+      <c r="C219" t="s">
+        <v>13</v>
+      </c>
+      <c r="D219" t="s">
+        <v>268</v>
+      </c>
+      <c r="E219">
+        <v>200</v>
+      </c>
+      <c r="F219" t="s">
+        <v>30</v>
+      </c>
+      <c r="G219" t="s">
+        <v>274</v>
+      </c>
+      <c r="H219" t="s">
+        <v>275</v>
+      </c>
+      <c r="I219" t="s">
+        <v>45</v>
+      </c>
+      <c r="J219" t="s">
+        <v>37</v>
+      </c>
+      <c r="K219" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>286</v>
+      </c>
+      <c r="B220" t="s">
+        <v>12</v>
+      </c>
+      <c r="C220" t="s">
+        <v>13</v>
+      </c>
+      <c r="D220" t="s">
+        <v>271</v>
+      </c>
+      <c r="E220">
+        <v>200</v>
+      </c>
+      <c r="F220" t="s">
+        <v>30</v>
+      </c>
+      <c r="G220" t="s">
+        <v>274</v>
+      </c>
+      <c r="H220" t="s">
+        <v>275</v>
+      </c>
+      <c r="I220" t="s">
+        <v>16</v>
+      </c>
+      <c r="J220" t="s">
+        <v>39</v>
+      </c>
+      <c r="K220" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>287</v>
+      </c>
+      <c r="B221" t="s">
+        <v>12</v>
+      </c>
+      <c r="C221" t="s">
+        <v>70</v>
+      </c>
+      <c r="D221" t="s">
+        <v>288</v>
+      </c>
+      <c r="E221">
+        <v>200</v>
+      </c>
+      <c r="F221" t="s">
+        <v>30</v>
+      </c>
+      <c r="G221" t="s">
+        <v>274</v>
+      </c>
+      <c r="H221" t="s">
+        <v>275</v>
+      </c>
+      <c r="I221" t="s">
+        <v>45</v>
+      </c>
+      <c r="J221" t="s">
+        <v>289</v>
+      </c>
+      <c r="K221" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>290</v>
+      </c>
+      <c r="B222" t="s">
+        <v>12</v>
+      </c>
+      <c r="C222" t="s">
+        <v>28</v>
+      </c>
+      <c r="D222" t="s">
+        <v>255</v>
+      </c>
+      <c r="E222">
+        <v>200</v>
+      </c>
+      <c r="F222" t="s">
+        <v>30</v>
+      </c>
+      <c r="G222" t="s">
+        <v>16</v>
+      </c>
+      <c r="H222" t="s">
+        <v>16</v>
+      </c>
+      <c r="I222" t="s">
+        <v>16</v>
+      </c>
+      <c r="J222" t="s">
+        <v>16</v>
+      </c>
+      <c r="K222" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>291</v>
+      </c>
+      <c r="B223" t="s">
+        <v>12</v>
+      </c>
+      <c r="C223" t="s">
+        <v>13</v>
+      </c>
+      <c r="D223" t="s">
+        <v>255</v>
+      </c>
+      <c r="E223">
+        <v>200</v>
+      </c>
+      <c r="F223" t="s">
+        <v>30</v>
+      </c>
+      <c r="G223" t="s">
+        <v>16</v>
+      </c>
+      <c r="H223" t="s">
+        <v>16</v>
+      </c>
+      <c r="I223" t="s">
+        <v>16</v>
+      </c>
+      <c r="J223" t="s">
+        <v>16</v>
+      </c>
+      <c r="K223" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>292</v>
+      </c>
+      <c r="B224" t="s">
+        <v>12</v>
+      </c>
+      <c r="C224" t="s">
+        <v>28</v>
+      </c>
+      <c r="D224" t="s">
+        <v>255</v>
+      </c>
+      <c r="E224">
+        <v>200</v>
+      </c>
+      <c r="F224" t="s">
+        <v>30</v>
+      </c>
+      <c r="G224" t="s">
+        <v>16</v>
+      </c>
+      <c r="H224" t="s">
+        <v>16</v>
+      </c>
+      <c r="I224" t="s">
+        <v>16</v>
+      </c>
+      <c r="J224" t="s">
+        <v>16</v>
+      </c>
+      <c r="K224" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>293</v>
+      </c>
+      <c r="B225" t="s">
+        <v>12</v>
+      </c>
+      <c r="C225" t="s">
+        <v>13</v>
+      </c>
+      <c r="D225" t="s">
+        <v>268</v>
+      </c>
+      <c r="E225">
+        <v>404</v>
+      </c>
+      <c r="F225" t="s">
+        <v>15</v>
+      </c>
+      <c r="G225" t="s">
+        <v>16</v>
+      </c>
+      <c r="H225" t="s">
+        <v>16</v>
+      </c>
+      <c r="I225" t="s">
+        <v>45</v>
+      </c>
+      <c r="J225" t="s">
+        <v>269</v>
+      </c>
+      <c r="K225" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>294</v>
+      </c>
+      <c r="B226" t="s">
+        <v>12</v>
+      </c>
+      <c r="C226" t="s">
+        <v>13</v>
+      </c>
+      <c r="D226" t="s">
+        <v>271</v>
+      </c>
+      <c r="E226">
+        <v>404</v>
+      </c>
+      <c r="F226" t="s">
+        <v>15</v>
+      </c>
+      <c r="G226" t="s">
+        <v>16</v>
+      </c>
+      <c r="H226" t="s">
+        <v>16</v>
+      </c>
+      <c r="I226" t="s">
+        <v>16</v>
+      </c>
+      <c r="J226" t="s">
+        <v>272</v>
+      </c>
+      <c r="K226" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>295</v>
+      </c>
+      <c r="B227" t="s">
+        <v>12</v>
+      </c>
+      <c r="C227" t="s">
+        <v>28</v>
+      </c>
+      <c r="D227" t="s">
+        <v>29</v>
+      </c>
+      <c r="E227">
+        <v>200</v>
+      </c>
+      <c r="F227" t="s">
+        <v>30</v>
+      </c>
+      <c r="G227" t="s">
+        <v>274</v>
+      </c>
+      <c r="H227" t="s">
+        <v>275</v>
+      </c>
+      <c r="I227" t="s">
+        <v>45</v>
+      </c>
+      <c r="J227" t="s">
+        <v>34</v>
+      </c>
+      <c r="K227" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>296</v>
+      </c>
+      <c r="B228" t="s">
+        <v>12</v>
+      </c>
+      <c r="C228" t="s">
+        <v>28</v>
+      </c>
+      <c r="D228" t="s">
+        <v>255</v>
+      </c>
+      <c r="E228">
+        <v>200</v>
+      </c>
+      <c r="F228" t="s">
+        <v>30</v>
+      </c>
+      <c r="G228" t="s">
+        <v>16</v>
+      </c>
+      <c r="H228" t="s">
+        <v>16</v>
+      </c>
+      <c r="I228" t="s">
+        <v>16</v>
+      </c>
+      <c r="J228" t="s">
+        <v>16</v>
+      </c>
+      <c r="K228" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>297</v>
+      </c>
+      <c r="B229" t="s">
+        <v>12</v>
+      </c>
+      <c r="C229" t="s">
+        <v>13</v>
+      </c>
+      <c r="D229" t="s">
+        <v>268</v>
+      </c>
+      <c r="E229">
+        <v>200</v>
+      </c>
+      <c r="F229" t="s">
+        <v>30</v>
+      </c>
+      <c r="G229" t="s">
+        <v>274</v>
+      </c>
+      <c r="H229" t="s">
+        <v>275</v>
+      </c>
+      <c r="I229" t="s">
+        <v>45</v>
+      </c>
+      <c r="J229" t="s">
+        <v>37</v>
+      </c>
+      <c r="K229" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>298</v>
+      </c>
+      <c r="B230" t="s">
+        <v>12</v>
+      </c>
+      <c r="C230" t="s">
+        <v>13</v>
+      </c>
+      <c r="D230" t="s">
+        <v>271</v>
+      </c>
+      <c r="E230">
+        <v>200</v>
+      </c>
+      <c r="F230" t="s">
+        <v>30</v>
+      </c>
+      <c r="G230" t="s">
+        <v>274</v>
+      </c>
+      <c r="H230" t="s">
+        <v>275</v>
+      </c>
+      <c r="I230" t="s">
+        <v>16</v>
+      </c>
+      <c r="J230" t="s">
+        <v>39</v>
+      </c>
+      <c r="K230" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>299</v>
+      </c>
+      <c r="B231" t="s">
+        <v>12</v>
+      </c>
+      <c r="C231" t="s">
+        <v>28</v>
+      </c>
+      <c r="D231" t="s">
+        <v>255</v>
+      </c>
+      <c r="E231">
+        <v>200</v>
+      </c>
+      <c r="F231" t="s">
+        <v>30</v>
+      </c>
+      <c r="G231" t="s">
+        <v>16</v>
+      </c>
+      <c r="H231" t="s">
+        <v>16</v>
+      </c>
+      <c r="I231" t="s">
+        <v>16</v>
+      </c>
+      <c r="J231" t="s">
+        <v>16</v>
+      </c>
+      <c r="K231" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>300</v>
+      </c>
+      <c r="B232" t="s">
+        <v>12</v>
+      </c>
+      <c r="C232" t="s">
+        <v>13</v>
+      </c>
+      <c r="D232" t="s">
+        <v>268</v>
+      </c>
+      <c r="E232">
+        <v>200</v>
+      </c>
+      <c r="F232" t="s">
+        <v>30</v>
+      </c>
+      <c r="G232" t="s">
+        <v>274</v>
+      </c>
+      <c r="H232" t="s">
+        <v>275</v>
+      </c>
+      <c r="I232" t="s">
+        <v>45</v>
+      </c>
+      <c r="J232" t="s">
+        <v>37</v>
+      </c>
+      <c r="K232" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>301</v>
+      </c>
+      <c r="B233" t="s">
+        <v>12</v>
+      </c>
+      <c r="C233" t="s">
+        <v>13</v>
+      </c>
+      <c r="D233" t="s">
+        <v>271</v>
+      </c>
+      <c r="E233">
+        <v>200</v>
+      </c>
+      <c r="F233" t="s">
+        <v>30</v>
+      </c>
+      <c r="G233" t="s">
+        <v>274</v>
+      </c>
+      <c r="H233" t="s">
+        <v>275</v>
+      </c>
+      <c r="I233" t="s">
+        <v>16</v>
+      </c>
+      <c r="J233" t="s">
+        <v>39</v>
+      </c>
+      <c r="K233" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>302</v>
+      </c>
+      <c r="B234" t="s">
+        <v>12</v>
+      </c>
+      <c r="C234" t="s">
+        <v>13</v>
+      </c>
+      <c r="D234" t="s">
+        <v>268</v>
+      </c>
+      <c r="E234">
+        <v>200</v>
+      </c>
+      <c r="F234" t="s">
+        <v>30</v>
+      </c>
+      <c r="G234" t="s">
+        <v>274</v>
+      </c>
+      <c r="H234" t="s">
+        <v>275</v>
+      </c>
+      <c r="I234" t="s">
+        <v>45</v>
+      </c>
+      <c r="J234" t="s">
+        <v>37</v>
+      </c>
+      <c r="K234" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>303</v>
+      </c>
+      <c r="B235" t="s">
+        <v>12</v>
+      </c>
+      <c r="C235" t="s">
+        <v>13</v>
+      </c>
+      <c r="D235" t="s">
+        <v>271</v>
+      </c>
+      <c r="E235">
+        <v>200</v>
+      </c>
+      <c r="F235" t="s">
+        <v>30</v>
+      </c>
+      <c r="G235" t="s">
+        <v>274</v>
+      </c>
+      <c r="H235" t="s">
+        <v>275</v>
+      </c>
+      <c r="I235" t="s">
+        <v>16</v>
+      </c>
+      <c r="J235" t="s">
+        <v>39</v>
+      </c>
+      <c r="K235" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>304</v>
+      </c>
+      <c r="B236" t="s">
+        <v>12</v>
+      </c>
+      <c r="C236" t="s">
+        <v>13</v>
+      </c>
+      <c r="D236" t="s">
+        <v>268</v>
+      </c>
+      <c r="E236">
+        <v>200</v>
+      </c>
+      <c r="F236" t="s">
+        <v>30</v>
+      </c>
+      <c r="G236" t="s">
+        <v>274</v>
+      </c>
+      <c r="H236" t="s">
+        <v>275</v>
+      </c>
+      <c r="I236" t="s">
+        <v>45</v>
+      </c>
+      <c r="J236" t="s">
+        <v>37</v>
+      </c>
+      <c r="K236" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>305</v>
+      </c>
+      <c r="B237" t="s">
+        <v>12</v>
+      </c>
+      <c r="C237" t="s">
+        <v>13</v>
+      </c>
+      <c r="D237" t="s">
+        <v>271</v>
+      </c>
+      <c r="E237">
+        <v>200</v>
+      </c>
+      <c r="F237" t="s">
+        <v>30</v>
+      </c>
+      <c r="G237" t="s">
+        <v>274</v>
+      </c>
+      <c r="H237" t="s">
+        <v>275</v>
+      </c>
+      <c r="I237" t="s">
+        <v>16</v>
+      </c>
+      <c r="J237" t="s">
+        <v>39</v>
+      </c>
+      <c r="K237" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>306</v>
+      </c>
+      <c r="B238" t="s">
+        <v>12</v>
+      </c>
+      <c r="C238" t="s">
+        <v>13</v>
+      </c>
+      <c r="D238" t="s">
+        <v>268</v>
+      </c>
+      <c r="E238">
+        <v>200</v>
+      </c>
+      <c r="F238" t="s">
+        <v>30</v>
+      </c>
+      <c r="G238" t="s">
+        <v>274</v>
+      </c>
+      <c r="H238" t="s">
+        <v>275</v>
+      </c>
+      <c r="I238" t="s">
+        <v>45</v>
+      </c>
+      <c r="J238" t="s">
+        <v>37</v>
+      </c>
+      <c r="K238" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>307</v>
+      </c>
+      <c r="B239" t="s">
+        <v>12</v>
+      </c>
+      <c r="C239" t="s">
+        <v>13</v>
+      </c>
+      <c r="D239" t="s">
+        <v>271</v>
+      </c>
+      <c r="E239">
+        <v>200</v>
+      </c>
+      <c r="F239" t="s">
+        <v>30</v>
+      </c>
+      <c r="G239" t="s">
+        <v>274</v>
+      </c>
+      <c r="H239" t="s">
+        <v>275</v>
+      </c>
+      <c r="I239" t="s">
+        <v>16</v>
+      </c>
+      <c r="J239" t="s">
+        <v>39</v>
+      </c>
+      <c r="K239" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>308</v>
+      </c>
+      <c r="B240" t="s">
+        <v>12</v>
+      </c>
+      <c r="C240" t="s">
+        <v>13</v>
+      </c>
+      <c r="D240" t="s">
+        <v>268</v>
+      </c>
+      <c r="E240">
+        <v>200</v>
+      </c>
+      <c r="F240" t="s">
+        <v>30</v>
+      </c>
+      <c r="G240" t="s">
+        <v>274</v>
+      </c>
+      <c r="H240" t="s">
+        <v>275</v>
+      </c>
+      <c r="I240" t="s">
+        <v>45</v>
+      </c>
+      <c r="J240" t="s">
+        <v>37</v>
+      </c>
+      <c r="K240" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>309</v>
+      </c>
+      <c r="B241" t="s">
+        <v>12</v>
+      </c>
+      <c r="C241" t="s">
+        <v>13</v>
+      </c>
+      <c r="D241" t="s">
+        <v>271</v>
+      </c>
+      <c r="E241">
+        <v>200</v>
+      </c>
+      <c r="F241" t="s">
+        <v>30</v>
+      </c>
+      <c r="G241" t="s">
+        <v>274</v>
+      </c>
+      <c r="H241" t="s">
+        <v>275</v>
+      </c>
+      <c r="I241" t="s">
+        <v>16</v>
+      </c>
+      <c r="J241" t="s">
+        <v>39</v>
+      </c>
+      <c r="K241" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>310</v>
+      </c>
+      <c r="B242" t="s">
+        <v>12</v>
+      </c>
+      <c r="C242" t="s">
+        <v>13</v>
+      </c>
+      <c r="D242" t="s">
+        <v>268</v>
+      </c>
+      <c r="E242">
+        <v>200</v>
+      </c>
+      <c r="F242" t="s">
+        <v>30</v>
+      </c>
+      <c r="G242" t="s">
+        <v>274</v>
+      </c>
+      <c r="H242" t="s">
+        <v>275</v>
+      </c>
+      <c r="I242" t="s">
+        <v>45</v>
+      </c>
+      <c r="J242" t="s">
+        <v>37</v>
+      </c>
+      <c r="K242" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>311</v>
+      </c>
+      <c r="B243" t="s">
+        <v>12</v>
+      </c>
+      <c r="C243" t="s">
+        <v>13</v>
+      </c>
+      <c r="D243" t="s">
+        <v>271</v>
+      </c>
+      <c r="E243">
+        <v>200</v>
+      </c>
+      <c r="F243" t="s">
+        <v>30</v>
+      </c>
+      <c r="G243" t="s">
+        <v>274</v>
+      </c>
+      <c r="H243" t="s">
+        <v>275</v>
+      </c>
+      <c r="I243" t="s">
+        <v>16</v>
+      </c>
+      <c r="J243" t="s">
+        <v>39</v>
+      </c>
+      <c r="K243" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>312</v>
+      </c>
+      <c r="B244" t="s">
+        <v>12</v>
+      </c>
+      <c r="C244" t="s">
+        <v>28</v>
+      </c>
+      <c r="D244" t="s">
+        <v>255</v>
+      </c>
+      <c r="E244">
+        <v>200</v>
+      </c>
+      <c r="F244" t="s">
+        <v>30</v>
+      </c>
+      <c r="G244" t="s">
+        <v>16</v>
+      </c>
+      <c r="H244" t="s">
+        <v>16</v>
+      </c>
+      <c r="I244" t="s">
+        <v>16</v>
+      </c>
+      <c r="J244" t="s">
+        <v>16</v>
+      </c>
+      <c r="K244" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>313</v>
+      </c>
+      <c r="B245" t="s">
+        <v>12</v>
+      </c>
+      <c r="C245" t="s">
+        <v>13</v>
+      </c>
+      <c r="D245" t="s">
+        <v>268</v>
+      </c>
+      <c r="E245">
+        <v>200</v>
+      </c>
+      <c r="F245" t="s">
+        <v>30</v>
+      </c>
+      <c r="G245" t="s">
+        <v>274</v>
+      </c>
+      <c r="H245" t="s">
+        <v>275</v>
+      </c>
+      <c r="I245" t="s">
+        <v>45</v>
+      </c>
+      <c r="J245" t="s">
+        <v>37</v>
+      </c>
+      <c r="K245" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>314</v>
+      </c>
+      <c r="B246" t="s">
+        <v>12</v>
+      </c>
+      <c r="C246" t="s">
+        <v>13</v>
+      </c>
+      <c r="D246" t="s">
+        <v>271</v>
+      </c>
+      <c r="E246">
+        <v>200</v>
+      </c>
+      <c r="F246" t="s">
+        <v>30</v>
+      </c>
+      <c r="G246" t="s">
+        <v>274</v>
+      </c>
+      <c r="H246" t="s">
+        <v>275</v>
+      </c>
+      <c r="I246" t="s">
+        <v>16</v>
+      </c>
+      <c r="J246" t="s">
+        <v>39</v>
+      </c>
+      <c r="K246" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>315</v>
+      </c>
+      <c r="B247" t="s">
+        <v>12</v>
+      </c>
+      <c r="C247" t="s">
+        <v>13</v>
+      </c>
+      <c r="D247" t="s">
+        <v>268</v>
+      </c>
+      <c r="E247">
+        <v>200</v>
+      </c>
+      <c r="F247" t="s">
+        <v>30</v>
+      </c>
+      <c r="G247" t="s">
+        <v>274</v>
+      </c>
+      <c r="H247" t="s">
+        <v>275</v>
+      </c>
+      <c r="I247" t="s">
+        <v>45</v>
+      </c>
+      <c r="J247" t="s">
+        <v>37</v>
+      </c>
+      <c r="K247" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>316</v>
+      </c>
+      <c r="B248" t="s">
+        <v>12</v>
+      </c>
+      <c r="C248" t="s">
+        <v>13</v>
+      </c>
+      <c r="D248" t="s">
+        <v>271</v>
+      </c>
+      <c r="E248">
+        <v>200</v>
+      </c>
+      <c r="F248" t="s">
+        <v>30</v>
+      </c>
+      <c r="G248" t="s">
+        <v>274</v>
+      </c>
+      <c r="H248" t="s">
+        <v>275</v>
+      </c>
+      <c r="I248" t="s">
+        <v>16</v>
+      </c>
+      <c r="J248" t="s">
+        <v>39</v>
+      </c>
+      <c r="K248" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>317</v>
+      </c>
+      <c r="B249" t="s">
+        <v>12</v>
+      </c>
+      <c r="C249" t="s">
+        <v>13</v>
+      </c>
+      <c r="D249" t="s">
+        <v>268</v>
+      </c>
+      <c r="E249">
+        <v>200</v>
+      </c>
+      <c r="F249" t="s">
+        <v>30</v>
+      </c>
+      <c r="G249" t="s">
+        <v>274</v>
+      </c>
+      <c r="H249" t="s">
+        <v>275</v>
+      </c>
+      <c r="I249" t="s">
+        <v>45</v>
+      </c>
+      <c r="J249" t="s">
+        <v>37</v>
+      </c>
+      <c r="K249" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>318</v>
+      </c>
+      <c r="B250" t="s">
+        <v>12</v>
+      </c>
+      <c r="C250" t="s">
+        <v>13</v>
+      </c>
+      <c r="D250" t="s">
+        <v>271</v>
+      </c>
+      <c r="E250">
+        <v>200</v>
+      </c>
+      <c r="F250" t="s">
+        <v>30</v>
+      </c>
+      <c r="G250" t="s">
+        <v>274</v>
+      </c>
+      <c r="H250" t="s">
+        <v>275</v>
+      </c>
+      <c r="I250" t="s">
+        <v>16</v>
+      </c>
+      <c r="J250" t="s">
+        <v>39</v>
+      </c>
+      <c r="K250" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>319</v>
+      </c>
+      <c r="B251" t="s">
+        <v>12</v>
+      </c>
+      <c r="C251" t="s">
+        <v>13</v>
+      </c>
+      <c r="D251" t="s">
+        <v>268</v>
+      </c>
+      <c r="E251">
+        <v>200</v>
+      </c>
+      <c r="F251" t="s">
+        <v>30</v>
+      </c>
+      <c r="G251" t="s">
+        <v>274</v>
+      </c>
+      <c r="H251" t="s">
+        <v>275</v>
+      </c>
+      <c r="I251" t="s">
+        <v>45</v>
+      </c>
+      <c r="J251" t="s">
+        <v>37</v>
+      </c>
+      <c r="K251" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>320</v>
+      </c>
+      <c r="B252" t="s">
+        <v>12</v>
+      </c>
+      <c r="C252" t="s">
+        <v>13</v>
+      </c>
+      <c r="D252" t="s">
+        <v>271</v>
+      </c>
+      <c r="E252">
+        <v>200</v>
+      </c>
+      <c r="F252" t="s">
+        <v>30</v>
+      </c>
+      <c r="G252" t="s">
+        <v>274</v>
+      </c>
+      <c r="H252" t="s">
+        <v>275</v>
+      </c>
+      <c r="I252" t="s">
+        <v>16</v>
+      </c>
+      <c r="J252" t="s">
+        <v>39</v>
+      </c>
+      <c r="K252" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>321</v>
+      </c>
+      <c r="B253" t="s">
+        <v>12</v>
+      </c>
+      <c r="C253" t="s">
+        <v>28</v>
+      </c>
+      <c r="D253" t="s">
+        <v>255</v>
+      </c>
+      <c r="E253">
+        <v>200</v>
+      </c>
+      <c r="F253" t="s">
+        <v>30</v>
+      </c>
+      <c r="G253" t="s">
+        <v>16</v>
+      </c>
+      <c r="H253" t="s">
+        <v>16</v>
+      </c>
+      <c r="I253" t="s">
+        <v>16</v>
+      </c>
+      <c r="J253" t="s">
+        <v>16</v>
+      </c>
+      <c r="K253" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>322</v>
+      </c>
+      <c r="B254" t="s">
+        <v>12</v>
+      </c>
+      <c r="C254" t="s">
+        <v>13</v>
+      </c>
+      <c r="D254" t="s">
+        <v>261</v>
+      </c>
+      <c r="E254">
+        <v>200</v>
+      </c>
+      <c r="F254" t="s">
+        <v>30</v>
+      </c>
+      <c r="G254" t="s">
+        <v>177</v>
+      </c>
+      <c r="H254" t="s">
+        <v>32</v>
+      </c>
+      <c r="I254" t="s">
+        <v>45</v>
+      </c>
+      <c r="J254" t="s">
+        <v>37</v>
+      </c>
+      <c r="K254" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>323</v>
+      </c>
+      <c r="B255" t="s">
+        <v>12</v>
+      </c>
+      <c r="C255" t="s">
+        <v>13</v>
+      </c>
+      <c r="D255" t="s">
+        <v>21</v>
+      </c>
+      <c r="E255">
+        <v>200</v>
+      </c>
+      <c r="F255" t="s">
+        <v>30</v>
+      </c>
+      <c r="G255" t="s">
+        <v>177</v>
+      </c>
+      <c r="H255" t="s">
+        <v>32</v>
+      </c>
+      <c r="I255" t="s">
+        <v>16</v>
+      </c>
+      <c r="J255" t="s">
+        <v>39</v>
+      </c>
+      <c r="K255" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>324</v>
+      </c>
+      <c r="B256" t="s">
+        <v>12</v>
+      </c>
+      <c r="C256" t="s">
+        <v>13</v>
+      </c>
+      <c r="D256" t="s">
+        <v>261</v>
+      </c>
+      <c r="E256">
+        <v>200</v>
+      </c>
+      <c r="F256" t="s">
+        <v>30</v>
+      </c>
+      <c r="G256" t="s">
+        <v>177</v>
+      </c>
+      <c r="H256" t="s">
+        <v>32</v>
+      </c>
+      <c r="I256" t="s">
+        <v>45</v>
+      </c>
+      <c r="J256" t="s">
+        <v>37</v>
+      </c>
+      <c r="K256" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>325</v>
+      </c>
+      <c r="B257" t="s">
+        <v>12</v>
+      </c>
+      <c r="C257" t="s">
+        <v>13</v>
+      </c>
+      <c r="D257" t="s">
+        <v>21</v>
+      </c>
+      <c r="E257">
+        <v>200</v>
+      </c>
+      <c r="F257" t="s">
+        <v>30</v>
+      </c>
+      <c r="G257" t="s">
+        <v>177</v>
+      </c>
+      <c r="H257" t="s">
+        <v>32</v>
+      </c>
+      <c r="I257" t="s">
+        <v>16</v>
+      </c>
+      <c r="J257" t="s">
+        <v>39</v>
+      </c>
+      <c r="K257" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>326</v>
+      </c>
+      <c r="B258" t="s">
+        <v>12</v>
+      </c>
+      <c r="C258" t="s">
+        <v>13</v>
+      </c>
+      <c r="D258" t="s">
+        <v>327</v>
+      </c>
+      <c r="E258">
+        <v>403</v>
+      </c>
+      <c r="F258" t="s">
+        <v>15</v>
+      </c>
+      <c r="G258" t="s">
+        <v>177</v>
+      </c>
+      <c r="H258" t="s">
+        <v>32</v>
+      </c>
+      <c r="I258" t="s">
+        <v>79</v>
+      </c>
+      <c r="J258" t="s">
+        <v>328</v>
+      </c>
+      <c r="K258" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>329</v>
+      </c>
+      <c r="B259" t="s">
+        <v>12</v>
+      </c>
+      <c r="C259" t="s">
+        <v>13</v>
+      </c>
+      <c r="D259" t="s">
+        <v>21</v>
+      </c>
+      <c r="E259">
+        <v>200</v>
+      </c>
+      <c r="F259" t="s">
+        <v>30</v>
+      </c>
+      <c r="G259" t="s">
+        <v>177</v>
+      </c>
+      <c r="H259" t="s">
+        <v>32</v>
+      </c>
+      <c r="I259" t="s">
+        <v>16</v>
+      </c>
+      <c r="J259" t="s">
+        <v>39</v>
+      </c>
+      <c r="K259" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>330</v>
+      </c>
+      <c r="B260" t="s">
+        <v>12</v>
+      </c>
+      <c r="C260" t="s">
+        <v>28</v>
+      </c>
+      <c r="D260" t="s">
+        <v>29</v>
+      </c>
+      <c r="E260">
+        <v>200</v>
+      </c>
+      <c r="F260" t="s">
+        <v>30</v>
+      </c>
+      <c r="G260" t="s">
+        <v>177</v>
+      </c>
+      <c r="H260" t="s">
+        <v>32</v>
+      </c>
+      <c r="I260" t="s">
+        <v>79</v>
+      </c>
+      <c r="J260" t="s">
+        <v>41</v>
+      </c>
+      <c r="K260" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>331</v>
+      </c>
+      <c r="B261" t="s">
+        <v>12</v>
+      </c>
+      <c r="C261" t="s">
+        <v>13</v>
+      </c>
+      <c r="D261" t="s">
+        <v>327</v>
+      </c>
+      <c r="E261">
+        <v>200</v>
+      </c>
+      <c r="F261" t="s">
+        <v>30</v>
+      </c>
+      <c r="G261" t="s">
+        <v>177</v>
+      </c>
+      <c r="H261" t="s">
+        <v>32</v>
+      </c>
+      <c r="I261" t="s">
+        <v>79</v>
+      </c>
+      <c r="J261" t="s">
+        <v>37</v>
+      </c>
+      <c r="K261" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>332</v>
+      </c>
+      <c r="B262" t="s">
+        <v>12</v>
+      </c>
+      <c r="C262" t="s">
+        <v>13</v>
+      </c>
+      <c r="D262" t="s">
+        <v>21</v>
+      </c>
+      <c r="E262">
+        <v>200</v>
+      </c>
+      <c r="F262" t="s">
+        <v>30</v>
+      </c>
+      <c r="G262" t="s">
+        <v>177</v>
+      </c>
+      <c r="H262" t="s">
+        <v>32</v>
+      </c>
+      <c r="I262" t="s">
+        <v>16</v>
+      </c>
+      <c r="J262" t="s">
+        <v>39</v>
+      </c>
+      <c r="K262" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>333</v>
+      </c>
+      <c r="B263" t="s">
+        <v>12</v>
+      </c>
+      <c r="C263" t="s">
+        <v>13</v>
+      </c>
+      <c r="D263" t="s">
+        <v>327</v>
+      </c>
+      <c r="E263">
+        <v>200</v>
+      </c>
+      <c r="F263" t="s">
+        <v>30</v>
+      </c>
+      <c r="G263" t="s">
+        <v>177</v>
+      </c>
+      <c r="H263" t="s">
+        <v>32</v>
+      </c>
+      <c r="I263" t="s">
+        <v>79</v>
+      </c>
+      <c r="J263" t="s">
+        <v>37</v>
+      </c>
+      <c r="K263" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>334</v>
+      </c>
+      <c r="B264" t="s">
+        <v>12</v>
+      </c>
+      <c r="C264" t="s">
+        <v>13</v>
+      </c>
+      <c r="D264" t="s">
+        <v>21</v>
+      </c>
+      <c r="E264">
+        <v>200</v>
+      </c>
+      <c r="F264" t="s">
+        <v>30</v>
+      </c>
+      <c r="G264" t="s">
+        <v>177</v>
+      </c>
+      <c r="H264" t="s">
+        <v>32</v>
+      </c>
+      <c r="I264" t="s">
+        <v>16</v>
+      </c>
+      <c r="J264" t="s">
+        <v>39</v>
+      </c>
+      <c r="K264" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>335</v>
+      </c>
+      <c r="B265" t="s">
+        <v>12</v>
+      </c>
+      <c r="C265" t="s">
+        <v>13</v>
+      </c>
+      <c r="D265" t="s">
+        <v>336</v>
+      </c>
+      <c r="E265">
+        <v>403</v>
+      </c>
+      <c r="F265" t="s">
+        <v>15</v>
+      </c>
+      <c r="G265" t="s">
+        <v>177</v>
+      </c>
+      <c r="H265" t="s">
+        <v>32</v>
+      </c>
+      <c r="I265" t="s">
+        <v>337</v>
+      </c>
+      <c r="J265" t="s">
+        <v>338</v>
+      </c>
+      <c r="K265" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>339</v>
+      </c>
+      <c r="B266" t="s">
+        <v>12</v>
+      </c>
+      <c r="C266" t="s">
+        <v>13</v>
+      </c>
+      <c r="D266" t="s">
+        <v>21</v>
+      </c>
+      <c r="E266">
+        <v>200</v>
+      </c>
+      <c r="F266" t="s">
+        <v>30</v>
+      </c>
+      <c r="G266" t="s">
+        <v>177</v>
+      </c>
+      <c r="H266" t="s">
+        <v>32</v>
+      </c>
+      <c r="I266" t="s">
+        <v>16</v>
+      </c>
+      <c r="J266" t="s">
+        <v>39</v>
+      </c>
+      <c r="K266" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>340</v>
+      </c>
+      <c r="B267" t="s">
+        <v>12</v>
+      </c>
+      <c r="C267" t="s">
+        <v>28</v>
+      </c>
+      <c r="D267" t="s">
+        <v>29</v>
+      </c>
+      <c r="E267">
+        <v>200</v>
+      </c>
+      <c r="F267" t="s">
+        <v>30</v>
+      </c>
+      <c r="G267" t="s">
+        <v>177</v>
+      </c>
+      <c r="H267" t="s">
+        <v>32</v>
+      </c>
+      <c r="I267" t="s">
+        <v>337</v>
+      </c>
+      <c r="J267" t="s">
+        <v>41</v>
+      </c>
+      <c r="K267" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>341</v>
+      </c>
+      <c r="B268" t="s">
+        <v>12</v>
+      </c>
+      <c r="C268" t="s">
+        <v>13</v>
+      </c>
+      <c r="D268" t="s">
+        <v>336</v>
+      </c>
+      <c r="E268">
+        <v>200</v>
+      </c>
+      <c r="F268" t="s">
+        <v>30</v>
+      </c>
+      <c r="G268" t="s">
+        <v>177</v>
+      </c>
+      <c r="H268" t="s">
+        <v>32</v>
+      </c>
+      <c r="I268" t="s">
+        <v>337</v>
+      </c>
+      <c r="J268" t="s">
+        <v>37</v>
+      </c>
+      <c r="K268" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>342</v>
+      </c>
+      <c r="B269" t="s">
+        <v>12</v>
+      </c>
+      <c r="C269" t="s">
+        <v>13</v>
+      </c>
+      <c r="D269" t="s">
+        <v>21</v>
+      </c>
+      <c r="E269">
+        <v>200</v>
+      </c>
+      <c r="F269" t="s">
+        <v>30</v>
+      </c>
+      <c r="G269" t="s">
+        <v>177</v>
+      </c>
+      <c r="H269" t="s">
+        <v>32</v>
+      </c>
+      <c r="I269" t="s">
+        <v>16</v>
+      </c>
+      <c r="J269" t="s">
+        <v>39</v>
+      </c>
+      <c r="K269" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>343</v>
+      </c>
+      <c r="B270" t="s">
+        <v>12</v>
+      </c>
+      <c r="C270" t="s">
+        <v>13</v>
+      </c>
+      <c r="D270" t="s">
+        <v>336</v>
+      </c>
+      <c r="E270">
+        <v>200</v>
+      </c>
+      <c r="F270" t="s">
+        <v>30</v>
+      </c>
+      <c r="G270" t="s">
+        <v>177</v>
+      </c>
+      <c r="H270" t="s">
+        <v>32</v>
+      </c>
+      <c r="I270" t="s">
+        <v>337</v>
+      </c>
+      <c r="J270" t="s">
+        <v>37</v>
+      </c>
+      <c r="K270" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>344</v>
+      </c>
+      <c r="B271" t="s">
+        <v>12</v>
+      </c>
+      <c r="C271" t="s">
+        <v>13</v>
+      </c>
+      <c r="D271" t="s">
+        <v>21</v>
+      </c>
+      <c r="E271">
+        <v>200</v>
+      </c>
+      <c r="F271" t="s">
+        <v>30</v>
+      </c>
+      <c r="G271" t="s">
+        <v>177</v>
+      </c>
+      <c r="H271" t="s">
+        <v>32</v>
+      </c>
+      <c r="I271" t="s">
+        <v>16</v>
+      </c>
+      <c r="J271" t="s">
+        <v>39</v>
+      </c>
+      <c r="K271" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>345</v>
+      </c>
+      <c r="B272" t="s">
+        <v>12</v>
+      </c>
+      <c r="C272" t="s">
+        <v>28</v>
+      </c>
+      <c r="D272" t="s">
+        <v>255</v>
+      </c>
+      <c r="E272">
+        <v>200</v>
+      </c>
+      <c r="F272" t="s">
+        <v>30</v>
+      </c>
+      <c r="G272" t="s">
+        <v>16</v>
+      </c>
+      <c r="H272" t="s">
+        <v>16</v>
+      </c>
+      <c r="I272" t="s">
+        <v>16</v>
+      </c>
+      <c r="J272" t="s">
+        <v>16</v>
+      </c>
+      <c r="K272" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>346</v>
+      </c>
+      <c r="B273" t="s">
+        <v>12</v>
+      </c>
+      <c r="C273" t="s">
+        <v>13</v>
+      </c>
+      <c r="D273" t="s">
+        <v>336</v>
+      </c>
+      <c r="E273">
+        <v>200</v>
+      </c>
+      <c r="F273" t="s">
+        <v>30</v>
+      </c>
+      <c r="G273" t="s">
+        <v>177</v>
+      </c>
+      <c r="H273" t="s">
+        <v>32</v>
+      </c>
+      <c r="I273" t="s">
+        <v>337</v>
+      </c>
+      <c r="J273" t="s">
+        <v>37</v>
+      </c>
+      <c r="K273" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>347</v>
+      </c>
+      <c r="B274" t="s">
+        <v>12</v>
+      </c>
+      <c r="C274" t="s">
+        <v>13</v>
+      </c>
+      <c r="D274" t="s">
+        <v>21</v>
+      </c>
+      <c r="E274">
+        <v>200</v>
+      </c>
+      <c r="F274" t="s">
+        <v>30</v>
+      </c>
+      <c r="G274" t="s">
+        <v>177</v>
+      </c>
+      <c r="H274" t="s">
+        <v>32</v>
+      </c>
+      <c r="I274" t="s">
+        <v>16</v>
+      </c>
+      <c r="J274" t="s">
+        <v>39</v>
+      </c>
+      <c r="K274" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>348</v>
+      </c>
+      <c r="B275" t="s">
+        <v>12</v>
+      </c>
+      <c r="C275" t="s">
+        <v>28</v>
+      </c>
+      <c r="D275" t="s">
+        <v>29</v>
+      </c>
+      <c r="E275">
+        <v>200</v>
+      </c>
+      <c r="F275" t="s">
+        <v>30</v>
+      </c>
+      <c r="G275" t="s">
+        <v>274</v>
+      </c>
+      <c r="H275" t="s">
+        <v>275</v>
+      </c>
+      <c r="I275" t="s">
+        <v>337</v>
+      </c>
+      <c r="J275" t="s">
+        <v>41</v>
+      </c>
+      <c r="K275" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>349</v>
+      </c>
+      <c r="B276" t="s">
+        <v>12</v>
+      </c>
+      <c r="C276" t="s">
+        <v>28</v>
+      </c>
+      <c r="D276" t="s">
+        <v>255</v>
+      </c>
+      <c r="E276">
+        <v>200</v>
+      </c>
+      <c r="F276" t="s">
+        <v>30</v>
+      </c>
+      <c r="G276" t="s">
+        <v>16</v>
+      </c>
+      <c r="H276" t="s">
+        <v>16</v>
+      </c>
+      <c r="I276" t="s">
+        <v>16</v>
+      </c>
+      <c r="J276" t="s">
+        <v>16</v>
+      </c>
+      <c r="K276" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>350</v>
+      </c>
+      <c r="B277" t="s">
+        <v>12</v>
+      </c>
+      <c r="C277" t="s">
+        <v>13</v>
+      </c>
+      <c r="D277" t="s">
+        <v>351</v>
+      </c>
+      <c r="E277">
+        <v>200</v>
+      </c>
+      <c r="F277" t="s">
+        <v>30</v>
+      </c>
+      <c r="G277" t="s">
+        <v>274</v>
+      </c>
+      <c r="H277" t="s">
+        <v>275</v>
+      </c>
+      <c r="I277" t="s">
+        <v>337</v>
+      </c>
+      <c r="J277" t="s">
+        <v>37</v>
+      </c>
+      <c r="K277" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>352</v>
+      </c>
+      <c r="B278" t="s">
+        <v>12</v>
+      </c>
+      <c r="C278" t="s">
+        <v>13</v>
+      </c>
+      <c r="D278" t="s">
+        <v>271</v>
+      </c>
+      <c r="E278">
+        <v>200</v>
+      </c>
+      <c r="F278" t="s">
+        <v>30</v>
+      </c>
+      <c r="G278" t="s">
+        <v>274</v>
+      </c>
+      <c r="H278" t="s">
+        <v>275</v>
+      </c>
+      <c r="I278" t="s">
+        <v>16</v>
+      </c>
+      <c r="J278" t="s">
+        <v>39</v>
+      </c>
+      <c r="K278" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>353</v>
+      </c>
+      <c r="B279" t="s">
+        <v>12</v>
+      </c>
+      <c r="C279" t="s">
+        <v>28</v>
+      </c>
+      <c r="D279" t="s">
+        <v>255</v>
+      </c>
+      <c r="E279">
+        <v>200</v>
+      </c>
+      <c r="F279" t="s">
+        <v>30</v>
+      </c>
+      <c r="G279" t="s">
+        <v>16</v>
+      </c>
+      <c r="H279" t="s">
+        <v>16</v>
+      </c>
+      <c r="I279" t="s">
+        <v>16</v>
+      </c>
+      <c r="J279" t="s">
+        <v>16</v>
+      </c>
+      <c r="K279" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>354</v>
+      </c>
+      <c r="B280" t="s">
+        <v>12</v>
+      </c>
+      <c r="C280" t="s">
+        <v>13</v>
+      </c>
+      <c r="D280" t="s">
+        <v>351</v>
+      </c>
+      <c r="E280">
+        <v>200</v>
+      </c>
+      <c r="F280" t="s">
+        <v>30</v>
+      </c>
+      <c r="G280" t="s">
+        <v>274</v>
+      </c>
+      <c r="H280" t="s">
+        <v>275</v>
+      </c>
+      <c r="I280" t="s">
+        <v>337</v>
+      </c>
+      <c r="J280" t="s">
+        <v>37</v>
+      </c>
+      <c r="K280" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>355</v>
+      </c>
+      <c r="B281" t="s">
+        <v>12</v>
+      </c>
+      <c r="C281" t="s">
+        <v>13</v>
+      </c>
+      <c r="D281" t="s">
+        <v>271</v>
+      </c>
+      <c r="E281">
+        <v>200</v>
+      </c>
+      <c r="F281" t="s">
+        <v>30</v>
+      </c>
+      <c r="G281" t="s">
+        <v>274</v>
+      </c>
+      <c r="H281" t="s">
+        <v>275</v>
+      </c>
+      <c r="I281" t="s">
+        <v>16</v>
+      </c>
+      <c r="J281" t="s">
+        <v>39</v>
+      </c>
+      <c r="K281" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>356</v>
+      </c>
+      <c r="B282" t="s">
+        <v>12</v>
+      </c>
+      <c r="C282" t="s">
+        <v>13</v>
+      </c>
+      <c r="D282" t="s">
+        <v>351</v>
+      </c>
+      <c r="E282">
+        <v>200</v>
+      </c>
+      <c r="F282" t="s">
+        <v>30</v>
+      </c>
+      <c r="G282" t="s">
+        <v>274</v>
+      </c>
+      <c r="H282" t="s">
+        <v>275</v>
+      </c>
+      <c r="I282" t="s">
+        <v>337</v>
+      </c>
+      <c r="J282" t="s">
+        <v>37</v>
+      </c>
+      <c r="K282" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>357</v>
+      </c>
+      <c r="B283" t="s">
+        <v>12</v>
+      </c>
+      <c r="C283" t="s">
+        <v>13</v>
+      </c>
+      <c r="D283" t="s">
+        <v>271</v>
+      </c>
+      <c r="E283">
+        <v>200</v>
+      </c>
+      <c r="F283" t="s">
+        <v>30</v>
+      </c>
+      <c r="G283" t="s">
+        <v>274</v>
+      </c>
+      <c r="H283" t="s">
+        <v>275</v>
+      </c>
+      <c r="I283" t="s">
+        <v>16</v>
+      </c>
+      <c r="J283" t="s">
+        <v>39</v>
+      </c>
+      <c r="K283" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>358</v>
+      </c>
+      <c r="B284" t="s">
+        <v>12</v>
+      </c>
+      <c r="C284" t="s">
+        <v>13</v>
+      </c>
+      <c r="D284" t="s">
+        <v>351</v>
+      </c>
+      <c r="E284">
+        <v>200</v>
+      </c>
+      <c r="F284" t="s">
+        <v>30</v>
+      </c>
+      <c r="G284" t="s">
+        <v>274</v>
+      </c>
+      <c r="H284" t="s">
+        <v>275</v>
+      </c>
+      <c r="I284" t="s">
+        <v>337</v>
+      </c>
+      <c r="J284" t="s">
+        <v>37</v>
+      </c>
+      <c r="K284" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>359</v>
+      </c>
+      <c r="B285" t="s">
+        <v>12</v>
+      </c>
+      <c r="C285" t="s">
+        <v>13</v>
+      </c>
+      <c r="D285" t="s">
+        <v>271</v>
+      </c>
+      <c r="E285">
+        <v>200</v>
+      </c>
+      <c r="F285" t="s">
+        <v>30</v>
+      </c>
+      <c r="G285" t="s">
+        <v>274</v>
+      </c>
+      <c r="H285" t="s">
+        <v>275</v>
+      </c>
+      <c r="I285" t="s">
+        <v>16</v>
+      </c>
+      <c r="J285" t="s">
+        <v>39</v>
+      </c>
+      <c r="K285" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>360</v>
+      </c>
+      <c r="B286" t="s">
+        <v>12</v>
+      </c>
+      <c r="C286" t="s">
+        <v>13</v>
+      </c>
+      <c r="D286" t="s">
+        <v>351</v>
+      </c>
+      <c r="E286">
+        <v>200</v>
+      </c>
+      <c r="F286" t="s">
+        <v>30</v>
+      </c>
+      <c r="G286" t="s">
+        <v>274</v>
+      </c>
+      <c r="H286" t="s">
+        <v>275</v>
+      </c>
+      <c r="I286" t="s">
+        <v>337</v>
+      </c>
+      <c r="J286" t="s">
+        <v>37</v>
+      </c>
+      <c r="K286" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>361</v>
+      </c>
+      <c r="B287" t="s">
+        <v>12</v>
+      </c>
+      <c r="C287" t="s">
+        <v>13</v>
+      </c>
+      <c r="D287" t="s">
+        <v>271</v>
+      </c>
+      <c r="E287">
+        <v>200</v>
+      </c>
+      <c r="F287" t="s">
+        <v>30</v>
+      </c>
+      <c r="G287" t="s">
+        <v>274</v>
+      </c>
+      <c r="H287" t="s">
+        <v>275</v>
+      </c>
+      <c r="I287" t="s">
+        <v>16</v>
+      </c>
+      <c r="J287" t="s">
+        <v>39</v>
+      </c>
+      <c r="K287" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>362</v>
+      </c>
+      <c r="B288" t="s">
+        <v>12</v>
+      </c>
+      <c r="C288" t="s">
+        <v>13</v>
+      </c>
+      <c r="D288" t="s">
+        <v>351</v>
+      </c>
+      <c r="E288">
+        <v>200</v>
+      </c>
+      <c r="F288" t="s">
+        <v>30</v>
+      </c>
+      <c r="G288" t="s">
+        <v>274</v>
+      </c>
+      <c r="H288" t="s">
+        <v>275</v>
+      </c>
+      <c r="I288" t="s">
+        <v>337</v>
+      </c>
+      <c r="J288" t="s">
+        <v>37</v>
+      </c>
+      <c r="K288" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>363</v>
+      </c>
+      <c r="B289" t="s">
+        <v>12</v>
+      </c>
+      <c r="C289" t="s">
+        <v>13</v>
+      </c>
+      <c r="D289" t="s">
+        <v>271</v>
+      </c>
+      <c r="E289">
+        <v>200</v>
+      </c>
+      <c r="F289" t="s">
+        <v>30</v>
+      </c>
+      <c r="G289" t="s">
+        <v>274</v>
+      </c>
+      <c r="H289" t="s">
+        <v>275</v>
+      </c>
+      <c r="I289" t="s">
+        <v>16</v>
+      </c>
+      <c r="J289" t="s">
+        <v>39</v>
+      </c>
+      <c r="K289" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>364</v>
+      </c>
+      <c r="B290" t="s">
+        <v>12</v>
+      </c>
+      <c r="C290" t="s">
+        <v>13</v>
+      </c>
+      <c r="D290" t="s">
+        <v>351</v>
+      </c>
+      <c r="E290">
+        <v>200</v>
+      </c>
+      <c r="F290" t="s">
+        <v>30</v>
+      </c>
+      <c r="G290" t="s">
+        <v>274</v>
+      </c>
+      <c r="H290" t="s">
+        <v>275</v>
+      </c>
+      <c r="I290" t="s">
+        <v>337</v>
+      </c>
+      <c r="J290" t="s">
+        <v>37</v>
+      </c>
+      <c r="K290" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>365</v>
+      </c>
+      <c r="B291" t="s">
+        <v>12</v>
+      </c>
+      <c r="C291" t="s">
+        <v>13</v>
+      </c>
+      <c r="D291" t="s">
+        <v>271</v>
+      </c>
+      <c r="E291">
+        <v>200</v>
+      </c>
+      <c r="F291" t="s">
+        <v>30</v>
+      </c>
+      <c r="G291" t="s">
+        <v>274</v>
+      </c>
+      <c r="H291" t="s">
+        <v>275</v>
+      </c>
+      <c r="I291" t="s">
+        <v>16</v>
+      </c>
+      <c r="J291" t="s">
+        <v>39</v>
+      </c>
+      <c r="K291" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>366</v>
+      </c>
+      <c r="B292" t="s">
+        <v>12</v>
+      </c>
+      <c r="C292" t="s">
+        <v>28</v>
+      </c>
+      <c r="D292" t="s">
+        <v>255</v>
+      </c>
+      <c r="E292">
+        <v>200</v>
+      </c>
+      <c r="F292" t="s">
+        <v>30</v>
+      </c>
+      <c r="G292" t="s">
+        <v>16</v>
+      </c>
+      <c r="H292" t="s">
+        <v>16</v>
+      </c>
+      <c r="I292" t="s">
+        <v>16</v>
+      </c>
+      <c r="J292" t="s">
+        <v>16</v>
+      </c>
+      <c r="K292" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update logs and users Excel files
Refreshed logs.xlsx and users.xlsx with new data. These updates may include recent log entries and user information changes.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/logs.xlsx
+++ b/Server/rfid-server-DBS-Http/logs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2921" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2981" uniqueCount="373">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1112,6 +1112,24 @@
   </si>
   <si>
     <t>2025-11-24T21:49:34.960Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:52:47.234Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:52:47.272Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:52:52.655Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:52:52.682Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:54:22.333Z</t>
+  </si>
+  <si>
+    <t>2025-11-24T21:54:22.372Z</t>
   </si>
 </sst>
 </file>
@@ -1488,7 +1506,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K292"/>
+  <dimension ref="A1:K298"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -11711,6 +11729,216 @@
         <v>250</v>
       </c>
     </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>367</v>
+      </c>
+      <c r="B293" t="s">
+        <v>12</v>
+      </c>
+      <c r="C293" t="s">
+        <v>13</v>
+      </c>
+      <c r="D293" t="s">
+        <v>336</v>
+      </c>
+      <c r="E293">
+        <v>200</v>
+      </c>
+      <c r="F293" t="s">
+        <v>30</v>
+      </c>
+      <c r="G293" t="s">
+        <v>177</v>
+      </c>
+      <c r="H293" t="s">
+        <v>32</v>
+      </c>
+      <c r="I293" t="s">
+        <v>337</v>
+      </c>
+      <c r="J293" t="s">
+        <v>37</v>
+      </c>
+      <c r="K293" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>368</v>
+      </c>
+      <c r="B294" t="s">
+        <v>12</v>
+      </c>
+      <c r="C294" t="s">
+        <v>13</v>
+      </c>
+      <c r="D294" t="s">
+        <v>21</v>
+      </c>
+      <c r="E294">
+        <v>200</v>
+      </c>
+      <c r="F294" t="s">
+        <v>30</v>
+      </c>
+      <c r="G294" t="s">
+        <v>177</v>
+      </c>
+      <c r="H294" t="s">
+        <v>32</v>
+      </c>
+      <c r="I294" t="s">
+        <v>16</v>
+      </c>
+      <c r="J294" t="s">
+        <v>39</v>
+      </c>
+      <c r="K294" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>369</v>
+      </c>
+      <c r="B295" t="s">
+        <v>12</v>
+      </c>
+      <c r="C295" t="s">
+        <v>13</v>
+      </c>
+      <c r="D295" t="s">
+        <v>351</v>
+      </c>
+      <c r="E295">
+        <v>200</v>
+      </c>
+      <c r="F295" t="s">
+        <v>30</v>
+      </c>
+      <c r="G295" t="s">
+        <v>274</v>
+      </c>
+      <c r="H295" t="s">
+        <v>275</v>
+      </c>
+      <c r="I295" t="s">
+        <v>337</v>
+      </c>
+      <c r="J295" t="s">
+        <v>37</v>
+      </c>
+      <c r="K295" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>370</v>
+      </c>
+      <c r="B296" t="s">
+        <v>12</v>
+      </c>
+      <c r="C296" t="s">
+        <v>13</v>
+      </c>
+      <c r="D296" t="s">
+        <v>271</v>
+      </c>
+      <c r="E296">
+        <v>200</v>
+      </c>
+      <c r="F296" t="s">
+        <v>30</v>
+      </c>
+      <c r="G296" t="s">
+        <v>274</v>
+      </c>
+      <c r="H296" t="s">
+        <v>275</v>
+      </c>
+      <c r="I296" t="s">
+        <v>16</v>
+      </c>
+      <c r="J296" t="s">
+        <v>39</v>
+      </c>
+      <c r="K296" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>371</v>
+      </c>
+      <c r="B297" t="s">
+        <v>12</v>
+      </c>
+      <c r="C297" t="s">
+        <v>13</v>
+      </c>
+      <c r="D297" t="s">
+        <v>351</v>
+      </c>
+      <c r="E297">
+        <v>200</v>
+      </c>
+      <c r="F297" t="s">
+        <v>30</v>
+      </c>
+      <c r="G297" t="s">
+        <v>274</v>
+      </c>
+      <c r="H297" t="s">
+        <v>275</v>
+      </c>
+      <c r="I297" t="s">
+        <v>337</v>
+      </c>
+      <c r="J297" t="s">
+        <v>37</v>
+      </c>
+      <c r="K297" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>372</v>
+      </c>
+      <c r="B298" t="s">
+        <v>12</v>
+      </c>
+      <c r="C298" t="s">
+        <v>13</v>
+      </c>
+      <c r="D298" t="s">
+        <v>271</v>
+      </c>
+      <c r="E298">
+        <v>200</v>
+      </c>
+      <c r="F298" t="s">
+        <v>30</v>
+      </c>
+      <c r="G298" t="s">
+        <v>274</v>
+      </c>
+      <c r="H298" t="s">
+        <v>275</v>
+      </c>
+      <c r="I298" t="s">
+        <v>16</v>
+      </c>
+      <c r="J298" t="s">
+        <v>39</v>
+      </c>
+      <c r="K298" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Add EJS templating and related dependencies
Integrated EJS for server-side templating, including new views for dashboard and login. Updated package.json and lock files to include ejs, jake, filelist, and picocolors dependencies. Added admin.css for styling and modified server.js and website.js to support new functionality.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/logs.xlsx
+++ b/Server/rfid-server-DBS-Http/logs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2981" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3821" uniqueCount="479">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1130,6 +1130,324 @@
   </si>
   <si>
     <t>2025-11-24T21:54:22.372Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:23:57.207Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:23:57.276Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:25:12.819Z</t>
+  </si>
+  <si>
+    <t>/user/EA4C7814?roomID=103</t>
+  </si>
+  <si>
+    <t>UID EA4C7814 not found in /user</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:25:12.859Z</t>
+  </si>
+  <si>
+    <t>/uid-name/EA4C7814</t>
+  </si>
+  <si>
+    <t>UID EA4C7814 not found in /uid-name</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:25:32.661Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:25:32.923Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:25:38.571Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:25:38.627Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:25:43.152Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:25:43.197Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:29:42.434Z</t>
+  </si>
+  <si>
+    <t>/user/EA4C7814?roomID=105</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:29:42.498Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:29:46.213Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:29:46.655Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:29:57.793Z</t>
+  </si>
+  <si>
+    <t>/user/E9956AF6?roomID=105</t>
+  </si>
+  <si>
+    <t>UID E9956AF6 not found in /user</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:29:57.912Z</t>
+  </si>
+  <si>
+    <t>/uid-name/E9956AF6</t>
+  </si>
+  <si>
+    <t>UID E9956AF6 not found in /uid-name</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:12.498Z</t>
+  </si>
+  <si>
+    <t>gggggg</t>
+  </si>
+  <si>
+    <t>E9956AF6</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:16.343Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:16.383Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:20.695Z</t>
+  </si>
+  <si>
+    <t>/room/E9956AF6/105</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:23.338Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:23.396Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:27.645Z</t>
+  </si>
+  <si>
+    <t>/user/E9956AF6</t>
+  </si>
+  <si>
+    <t>UID E9956AF6 not found in DELETE /user</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:31.914Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:32.128Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:32.963Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:33.024Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:37.111Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:37.167Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:37.891Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:37.977Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:41.384Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:41.433Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:53.002Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:55.918Z</t>
+  </si>
+  <si>
+    <t>/user/835DF613?roomID=106</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:30:56.042Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:11.550Z</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:24.525Z</t>
+  </si>
+  <si>
+    <t>/user/835DF613?roomID=108</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:24.566Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:28.208Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:28.509Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:30.376Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:30.419Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:32.069Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:32.094Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:35.037Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:35.133Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:40.765Z</t>
+  </si>
+  <si>
+    <t>/room/835DF613/108</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:40.894Z</t>
+  </si>
+  <si>
+    <t>Access denied for room 108</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:40.930Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:42.381Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:42.421Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:42.514Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:42.594Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:43.318Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:43.370Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:49.425Z</t>
+  </si>
+  <si>
+    <t>/user/835DF613</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:49.826Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:31:50.076Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:32:50.909Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:32:51.076Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:32:58.434Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:34:09.830Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:34:13.153Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:35:28.509Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:35:29.788Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:35:31.664Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:35:34.704Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:41:31.941Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:41:32.016Z</t>
+  </si>
+  <si>
+    <t>/admin.css</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:41:33.692Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:41:33.749Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:41:37.221Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:41:37.265Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:42:07.109Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:42:08.712Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:42:11.276Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:43:29.120Z</t>
+  </si>
+  <si>
+    <t>/dashboard</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:45:59.921Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:46:01.808Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:47:47.702Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:47:54.059Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:47:57.689Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T04:48:07.957Z</t>
   </si>
 </sst>
 </file>
@@ -1506,7 +1824,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K298"/>
+  <dimension ref="A1:K382"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -11939,6 +12257,2946 @@
         <v>19</v>
       </c>
     </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>373</v>
+      </c>
+      <c r="B299" t="s">
+        <v>12</v>
+      </c>
+      <c r="C299" t="s">
+        <v>13</v>
+      </c>
+      <c r="D299" t="s">
+        <v>327</v>
+      </c>
+      <c r="E299">
+        <v>200</v>
+      </c>
+      <c r="F299" t="s">
+        <v>30</v>
+      </c>
+      <c r="G299" t="s">
+        <v>177</v>
+      </c>
+      <c r="H299" t="s">
+        <v>32</v>
+      </c>
+      <c r="I299" t="s">
+        <v>79</v>
+      </c>
+      <c r="J299" t="s">
+        <v>37</v>
+      </c>
+      <c r="K299" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>374</v>
+      </c>
+      <c r="B300" t="s">
+        <v>12</v>
+      </c>
+      <c r="C300" t="s">
+        <v>13</v>
+      </c>
+      <c r="D300" t="s">
+        <v>21</v>
+      </c>
+      <c r="E300">
+        <v>200</v>
+      </c>
+      <c r="F300" t="s">
+        <v>30</v>
+      </c>
+      <c r="G300" t="s">
+        <v>177</v>
+      </c>
+      <c r="H300" t="s">
+        <v>32</v>
+      </c>
+      <c r="I300" t="s">
+        <v>16</v>
+      </c>
+      <c r="J300" t="s">
+        <v>39</v>
+      </c>
+      <c r="K300" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>375</v>
+      </c>
+      <c r="B301" t="s">
+        <v>12</v>
+      </c>
+      <c r="C301" t="s">
+        <v>13</v>
+      </c>
+      <c r="D301" t="s">
+        <v>376</v>
+      </c>
+      <c r="E301">
+        <v>404</v>
+      </c>
+      <c r="F301" t="s">
+        <v>15</v>
+      </c>
+      <c r="G301" t="s">
+        <v>16</v>
+      </c>
+      <c r="H301" t="s">
+        <v>16</v>
+      </c>
+      <c r="I301" t="s">
+        <v>79</v>
+      </c>
+      <c r="J301" t="s">
+        <v>377</v>
+      </c>
+      <c r="K301" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>378</v>
+      </c>
+      <c r="B302" t="s">
+        <v>12</v>
+      </c>
+      <c r="C302" t="s">
+        <v>13</v>
+      </c>
+      <c r="D302" t="s">
+        <v>379</v>
+      </c>
+      <c r="E302">
+        <v>404</v>
+      </c>
+      <c r="F302" t="s">
+        <v>15</v>
+      </c>
+      <c r="G302" t="s">
+        <v>16</v>
+      </c>
+      <c r="H302" t="s">
+        <v>16</v>
+      </c>
+      <c r="I302" t="s">
+        <v>16</v>
+      </c>
+      <c r="J302" t="s">
+        <v>380</v>
+      </c>
+      <c r="K302" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>381</v>
+      </c>
+      <c r="B303" t="s">
+        <v>12</v>
+      </c>
+      <c r="C303" t="s">
+        <v>13</v>
+      </c>
+      <c r="D303" t="s">
+        <v>327</v>
+      </c>
+      <c r="E303">
+        <v>200</v>
+      </c>
+      <c r="F303" t="s">
+        <v>30</v>
+      </c>
+      <c r="G303" t="s">
+        <v>177</v>
+      </c>
+      <c r="H303" t="s">
+        <v>32</v>
+      </c>
+      <c r="I303" t="s">
+        <v>79</v>
+      </c>
+      <c r="J303" t="s">
+        <v>37</v>
+      </c>
+      <c r="K303" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>382</v>
+      </c>
+      <c r="B304" t="s">
+        <v>12</v>
+      </c>
+      <c r="C304" t="s">
+        <v>13</v>
+      </c>
+      <c r="D304" t="s">
+        <v>21</v>
+      </c>
+      <c r="E304">
+        <v>200</v>
+      </c>
+      <c r="F304" t="s">
+        <v>30</v>
+      </c>
+      <c r="G304" t="s">
+        <v>177</v>
+      </c>
+      <c r="H304" t="s">
+        <v>32</v>
+      </c>
+      <c r="I304" t="s">
+        <v>16</v>
+      </c>
+      <c r="J304" t="s">
+        <v>39</v>
+      </c>
+      <c r="K304" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>383</v>
+      </c>
+      <c r="B305" t="s">
+        <v>12</v>
+      </c>
+      <c r="C305" t="s">
+        <v>13</v>
+      </c>
+      <c r="D305" t="s">
+        <v>376</v>
+      </c>
+      <c r="E305">
+        <v>404</v>
+      </c>
+      <c r="F305" t="s">
+        <v>15</v>
+      </c>
+      <c r="G305" t="s">
+        <v>16</v>
+      </c>
+      <c r="H305" t="s">
+        <v>16</v>
+      </c>
+      <c r="I305" t="s">
+        <v>79</v>
+      </c>
+      <c r="J305" t="s">
+        <v>377</v>
+      </c>
+      <c r="K305" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>384</v>
+      </c>
+      <c r="B306" t="s">
+        <v>12</v>
+      </c>
+      <c r="C306" t="s">
+        <v>13</v>
+      </c>
+      <c r="D306" t="s">
+        <v>379</v>
+      </c>
+      <c r="E306">
+        <v>404</v>
+      </c>
+      <c r="F306" t="s">
+        <v>15</v>
+      </c>
+      <c r="G306" t="s">
+        <v>16</v>
+      </c>
+      <c r="H306" t="s">
+        <v>16</v>
+      </c>
+      <c r="I306" t="s">
+        <v>16</v>
+      </c>
+      <c r="J306" t="s">
+        <v>380</v>
+      </c>
+      <c r="K306" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>385</v>
+      </c>
+      <c r="B307" t="s">
+        <v>12</v>
+      </c>
+      <c r="C307" t="s">
+        <v>13</v>
+      </c>
+      <c r="D307" t="s">
+        <v>327</v>
+      </c>
+      <c r="E307">
+        <v>200</v>
+      </c>
+      <c r="F307" t="s">
+        <v>30</v>
+      </c>
+      <c r="G307" t="s">
+        <v>177</v>
+      </c>
+      <c r="H307" t="s">
+        <v>32</v>
+      </c>
+      <c r="I307" t="s">
+        <v>79</v>
+      </c>
+      <c r="J307" t="s">
+        <v>37</v>
+      </c>
+      <c r="K307" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>386</v>
+      </c>
+      <c r="B308" t="s">
+        <v>12</v>
+      </c>
+      <c r="C308" t="s">
+        <v>13</v>
+      </c>
+      <c r="D308" t="s">
+        <v>21</v>
+      </c>
+      <c r="E308">
+        <v>200</v>
+      </c>
+      <c r="F308" t="s">
+        <v>30</v>
+      </c>
+      <c r="G308" t="s">
+        <v>177</v>
+      </c>
+      <c r="H308" t="s">
+        <v>32</v>
+      </c>
+      <c r="I308" t="s">
+        <v>16</v>
+      </c>
+      <c r="J308" t="s">
+        <v>39</v>
+      </c>
+      <c r="K308" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>387</v>
+      </c>
+      <c r="B309" t="s">
+        <v>12</v>
+      </c>
+      <c r="C309" t="s">
+        <v>13</v>
+      </c>
+      <c r="D309" t="s">
+        <v>388</v>
+      </c>
+      <c r="E309">
+        <v>404</v>
+      </c>
+      <c r="F309" t="s">
+        <v>15</v>
+      </c>
+      <c r="G309" t="s">
+        <v>16</v>
+      </c>
+      <c r="H309" t="s">
+        <v>16</v>
+      </c>
+      <c r="I309" t="s">
+        <v>43</v>
+      </c>
+      <c r="J309" t="s">
+        <v>377</v>
+      </c>
+      <c r="K309" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>389</v>
+      </c>
+      <c r="B310" t="s">
+        <v>12</v>
+      </c>
+      <c r="C310" t="s">
+        <v>13</v>
+      </c>
+      <c r="D310" t="s">
+        <v>379</v>
+      </c>
+      <c r="E310">
+        <v>404</v>
+      </c>
+      <c r="F310" t="s">
+        <v>15</v>
+      </c>
+      <c r="G310" t="s">
+        <v>16</v>
+      </c>
+      <c r="H310" t="s">
+        <v>16</v>
+      </c>
+      <c r="I310" t="s">
+        <v>16</v>
+      </c>
+      <c r="J310" t="s">
+        <v>380</v>
+      </c>
+      <c r="K310" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>390</v>
+      </c>
+      <c r="B311" t="s">
+        <v>12</v>
+      </c>
+      <c r="C311" t="s">
+        <v>13</v>
+      </c>
+      <c r="D311" t="s">
+        <v>93</v>
+      </c>
+      <c r="E311">
+        <v>200</v>
+      </c>
+      <c r="F311" t="s">
+        <v>30</v>
+      </c>
+      <c r="G311" t="s">
+        <v>177</v>
+      </c>
+      <c r="H311" t="s">
+        <v>32</v>
+      </c>
+      <c r="I311" t="s">
+        <v>43</v>
+      </c>
+      <c r="J311" t="s">
+        <v>37</v>
+      </c>
+      <c r="K311" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>391</v>
+      </c>
+      <c r="B312" t="s">
+        <v>12</v>
+      </c>
+      <c r="C312" t="s">
+        <v>13</v>
+      </c>
+      <c r="D312" t="s">
+        <v>21</v>
+      </c>
+      <c r="E312">
+        <v>200</v>
+      </c>
+      <c r="F312" t="s">
+        <v>30</v>
+      </c>
+      <c r="G312" t="s">
+        <v>177</v>
+      </c>
+      <c r="H312" t="s">
+        <v>32</v>
+      </c>
+      <c r="I312" t="s">
+        <v>16</v>
+      </c>
+      <c r="J312" t="s">
+        <v>39</v>
+      </c>
+      <c r="K312" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>392</v>
+      </c>
+      <c r="B313" t="s">
+        <v>12</v>
+      </c>
+      <c r="C313" t="s">
+        <v>13</v>
+      </c>
+      <c r="D313" t="s">
+        <v>393</v>
+      </c>
+      <c r="E313">
+        <v>404</v>
+      </c>
+      <c r="F313" t="s">
+        <v>15</v>
+      </c>
+      <c r="G313" t="s">
+        <v>16</v>
+      </c>
+      <c r="H313" t="s">
+        <v>16</v>
+      </c>
+      <c r="I313" t="s">
+        <v>43</v>
+      </c>
+      <c r="J313" t="s">
+        <v>394</v>
+      </c>
+      <c r="K313" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>395</v>
+      </c>
+      <c r="B314" t="s">
+        <v>12</v>
+      </c>
+      <c r="C314" t="s">
+        <v>13</v>
+      </c>
+      <c r="D314" t="s">
+        <v>396</v>
+      </c>
+      <c r="E314">
+        <v>404</v>
+      </c>
+      <c r="F314" t="s">
+        <v>15</v>
+      </c>
+      <c r="G314" t="s">
+        <v>16</v>
+      </c>
+      <c r="H314" t="s">
+        <v>16</v>
+      </c>
+      <c r="I314" t="s">
+        <v>16</v>
+      </c>
+      <c r="J314" t="s">
+        <v>397</v>
+      </c>
+      <c r="K314" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>398</v>
+      </c>
+      <c r="B315" t="s">
+        <v>12</v>
+      </c>
+      <c r="C315" t="s">
+        <v>28</v>
+      </c>
+      <c r="D315" t="s">
+        <v>29</v>
+      </c>
+      <c r="E315">
+        <v>200</v>
+      </c>
+      <c r="F315" t="s">
+        <v>30</v>
+      </c>
+      <c r="G315" t="s">
+        <v>399</v>
+      </c>
+      <c r="H315" t="s">
+        <v>400</v>
+      </c>
+      <c r="I315" t="s">
+        <v>43</v>
+      </c>
+      <c r="J315" t="s">
+        <v>34</v>
+      </c>
+      <c r="K315" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>401</v>
+      </c>
+      <c r="B316" t="s">
+        <v>12</v>
+      </c>
+      <c r="C316" t="s">
+        <v>13</v>
+      </c>
+      <c r="D316" t="s">
+        <v>393</v>
+      </c>
+      <c r="E316">
+        <v>200</v>
+      </c>
+      <c r="F316" t="s">
+        <v>30</v>
+      </c>
+      <c r="G316" t="s">
+        <v>399</v>
+      </c>
+      <c r="H316" t="s">
+        <v>400</v>
+      </c>
+      <c r="I316" t="s">
+        <v>43</v>
+      </c>
+      <c r="J316" t="s">
+        <v>37</v>
+      </c>
+      <c r="K316" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>402</v>
+      </c>
+      <c r="B317" t="s">
+        <v>12</v>
+      </c>
+      <c r="C317" t="s">
+        <v>13</v>
+      </c>
+      <c r="D317" t="s">
+        <v>396</v>
+      </c>
+      <c r="E317">
+        <v>200</v>
+      </c>
+      <c r="F317" t="s">
+        <v>30</v>
+      </c>
+      <c r="G317" t="s">
+        <v>399</v>
+      </c>
+      <c r="H317" t="s">
+        <v>400</v>
+      </c>
+      <c r="I317" t="s">
+        <v>16</v>
+      </c>
+      <c r="J317" t="s">
+        <v>39</v>
+      </c>
+      <c r="K317" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>403</v>
+      </c>
+      <c r="B318" t="s">
+        <v>12</v>
+      </c>
+      <c r="C318" t="s">
+        <v>70</v>
+      </c>
+      <c r="D318" t="s">
+        <v>404</v>
+      </c>
+      <c r="E318">
+        <v>200</v>
+      </c>
+      <c r="F318" t="s">
+        <v>30</v>
+      </c>
+      <c r="G318" t="s">
+        <v>399</v>
+      </c>
+      <c r="H318" t="s">
+        <v>400</v>
+      </c>
+      <c r="I318" t="s">
+        <v>43</v>
+      </c>
+      <c r="J318" t="s">
+        <v>289</v>
+      </c>
+      <c r="K318" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>405</v>
+      </c>
+      <c r="B319" t="s">
+        <v>12</v>
+      </c>
+      <c r="C319" t="s">
+        <v>13</v>
+      </c>
+      <c r="D319" t="s">
+        <v>393</v>
+      </c>
+      <c r="E319">
+        <v>404</v>
+      </c>
+      <c r="F319" t="s">
+        <v>15</v>
+      </c>
+      <c r="G319" t="s">
+        <v>16</v>
+      </c>
+      <c r="H319" t="s">
+        <v>16</v>
+      </c>
+      <c r="I319" t="s">
+        <v>43</v>
+      </c>
+      <c r="J319" t="s">
+        <v>394</v>
+      </c>
+      <c r="K319" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>406</v>
+      </c>
+      <c r="B320" t="s">
+        <v>12</v>
+      </c>
+      <c r="C320" t="s">
+        <v>13</v>
+      </c>
+      <c r="D320" t="s">
+        <v>396</v>
+      </c>
+      <c r="E320">
+        <v>404</v>
+      </c>
+      <c r="F320" t="s">
+        <v>15</v>
+      </c>
+      <c r="G320" t="s">
+        <v>16</v>
+      </c>
+      <c r="H320" t="s">
+        <v>16</v>
+      </c>
+      <c r="I320" t="s">
+        <v>16</v>
+      </c>
+      <c r="J320" t="s">
+        <v>397</v>
+      </c>
+      <c r="K320" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>407</v>
+      </c>
+      <c r="B321" t="s">
+        <v>12</v>
+      </c>
+      <c r="C321" t="s">
+        <v>70</v>
+      </c>
+      <c r="D321" t="s">
+        <v>408</v>
+      </c>
+      <c r="E321">
+        <v>404</v>
+      </c>
+      <c r="F321" t="s">
+        <v>15</v>
+      </c>
+      <c r="G321" t="s">
+        <v>16</v>
+      </c>
+      <c r="H321" t="s">
+        <v>16</v>
+      </c>
+      <c r="I321" t="s">
+        <v>16</v>
+      </c>
+      <c r="J321" t="s">
+        <v>409</v>
+      </c>
+      <c r="K321" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>410</v>
+      </c>
+      <c r="B322" t="s">
+        <v>12</v>
+      </c>
+      <c r="C322" t="s">
+        <v>13</v>
+      </c>
+      <c r="D322" t="s">
+        <v>393</v>
+      </c>
+      <c r="E322">
+        <v>404</v>
+      </c>
+      <c r="F322" t="s">
+        <v>15</v>
+      </c>
+      <c r="G322" t="s">
+        <v>16</v>
+      </c>
+      <c r="H322" t="s">
+        <v>16</v>
+      </c>
+      <c r="I322" t="s">
+        <v>43</v>
+      </c>
+      <c r="J322" t="s">
+        <v>394</v>
+      </c>
+      <c r="K322" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>411</v>
+      </c>
+      <c r="B323" t="s">
+        <v>12</v>
+      </c>
+      <c r="C323" t="s">
+        <v>13</v>
+      </c>
+      <c r="D323" t="s">
+        <v>396</v>
+      </c>
+      <c r="E323">
+        <v>404</v>
+      </c>
+      <c r="F323" t="s">
+        <v>15</v>
+      </c>
+      <c r="G323" t="s">
+        <v>16</v>
+      </c>
+      <c r="H323" t="s">
+        <v>16</v>
+      </c>
+      <c r="I323" t="s">
+        <v>16</v>
+      </c>
+      <c r="J323" t="s">
+        <v>397</v>
+      </c>
+      <c r="K323" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>412</v>
+      </c>
+      <c r="B324" t="s">
+        <v>12</v>
+      </c>
+      <c r="C324" t="s">
+        <v>13</v>
+      </c>
+      <c r="D324" t="s">
+        <v>393</v>
+      </c>
+      <c r="E324">
+        <v>404</v>
+      </c>
+      <c r="F324" t="s">
+        <v>15</v>
+      </c>
+      <c r="G324" t="s">
+        <v>16</v>
+      </c>
+      <c r="H324" t="s">
+        <v>16</v>
+      </c>
+      <c r="I324" t="s">
+        <v>43</v>
+      </c>
+      <c r="J324" t="s">
+        <v>394</v>
+      </c>
+      <c r="K324" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>413</v>
+      </c>
+      <c r="B325" t="s">
+        <v>12</v>
+      </c>
+      <c r="C325" t="s">
+        <v>13</v>
+      </c>
+      <c r="D325" t="s">
+        <v>396</v>
+      </c>
+      <c r="E325">
+        <v>404</v>
+      </c>
+      <c r="F325" t="s">
+        <v>15</v>
+      </c>
+      <c r="G325" t="s">
+        <v>16</v>
+      </c>
+      <c r="H325" t="s">
+        <v>16</v>
+      </c>
+      <c r="I325" t="s">
+        <v>16</v>
+      </c>
+      <c r="J325" t="s">
+        <v>397</v>
+      </c>
+      <c r="K325" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>414</v>
+      </c>
+      <c r="B326" t="s">
+        <v>12</v>
+      </c>
+      <c r="C326" t="s">
+        <v>13</v>
+      </c>
+      <c r="D326" t="s">
+        <v>393</v>
+      </c>
+      <c r="E326">
+        <v>404</v>
+      </c>
+      <c r="F326" t="s">
+        <v>15</v>
+      </c>
+      <c r="G326" t="s">
+        <v>16</v>
+      </c>
+      <c r="H326" t="s">
+        <v>16</v>
+      </c>
+      <c r="I326" t="s">
+        <v>43</v>
+      </c>
+      <c r="J326" t="s">
+        <v>394</v>
+      </c>
+      <c r="K326" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>415</v>
+      </c>
+      <c r="B327" t="s">
+        <v>12</v>
+      </c>
+      <c r="C327" t="s">
+        <v>13</v>
+      </c>
+      <c r="D327" t="s">
+        <v>396</v>
+      </c>
+      <c r="E327">
+        <v>404</v>
+      </c>
+      <c r="F327" t="s">
+        <v>15</v>
+      </c>
+      <c r="G327" t="s">
+        <v>16</v>
+      </c>
+      <c r="H327" t="s">
+        <v>16</v>
+      </c>
+      <c r="I327" t="s">
+        <v>16</v>
+      </c>
+      <c r="J327" t="s">
+        <v>397</v>
+      </c>
+      <c r="K327" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>416</v>
+      </c>
+      <c r="B328" t="s">
+        <v>12</v>
+      </c>
+      <c r="C328" t="s">
+        <v>13</v>
+      </c>
+      <c r="D328" t="s">
+        <v>393</v>
+      </c>
+      <c r="E328">
+        <v>404</v>
+      </c>
+      <c r="F328" t="s">
+        <v>15</v>
+      </c>
+      <c r="G328" t="s">
+        <v>16</v>
+      </c>
+      <c r="H328" t="s">
+        <v>16</v>
+      </c>
+      <c r="I328" t="s">
+        <v>43</v>
+      </c>
+      <c r="J328" t="s">
+        <v>394</v>
+      </c>
+      <c r="K328" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>417</v>
+      </c>
+      <c r="B329" t="s">
+        <v>12</v>
+      </c>
+      <c r="C329" t="s">
+        <v>13</v>
+      </c>
+      <c r="D329" t="s">
+        <v>396</v>
+      </c>
+      <c r="E329">
+        <v>404</v>
+      </c>
+      <c r="F329" t="s">
+        <v>15</v>
+      </c>
+      <c r="G329" t="s">
+        <v>16</v>
+      </c>
+      <c r="H329" t="s">
+        <v>16</v>
+      </c>
+      <c r="I329" t="s">
+        <v>16</v>
+      </c>
+      <c r="J329" t="s">
+        <v>397</v>
+      </c>
+      <c r="K329" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>418</v>
+      </c>
+      <c r="B330" t="s">
+        <v>12</v>
+      </c>
+      <c r="C330" t="s">
+        <v>13</v>
+      </c>
+      <c r="D330" t="s">
+        <v>393</v>
+      </c>
+      <c r="E330">
+        <v>404</v>
+      </c>
+      <c r="F330" t="s">
+        <v>15</v>
+      </c>
+      <c r="G330" t="s">
+        <v>16</v>
+      </c>
+      <c r="H330" t="s">
+        <v>16</v>
+      </c>
+      <c r="I330" t="s">
+        <v>43</v>
+      </c>
+      <c r="J330" t="s">
+        <v>394</v>
+      </c>
+      <c r="K330" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>419</v>
+      </c>
+      <c r="B331" t="s">
+        <v>12</v>
+      </c>
+      <c r="C331" t="s">
+        <v>13</v>
+      </c>
+      <c r="D331" t="s">
+        <v>396</v>
+      </c>
+      <c r="E331">
+        <v>404</v>
+      </c>
+      <c r="F331" t="s">
+        <v>15</v>
+      </c>
+      <c r="G331" t="s">
+        <v>16</v>
+      </c>
+      <c r="H331" t="s">
+        <v>16</v>
+      </c>
+      <c r="I331" t="s">
+        <v>16</v>
+      </c>
+      <c r="J331" t="s">
+        <v>397</v>
+      </c>
+      <c r="K331" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>420</v>
+      </c>
+      <c r="B332" t="s">
+        <v>12</v>
+      </c>
+      <c r="C332" t="s">
+        <v>28</v>
+      </c>
+      <c r="D332" t="s">
+        <v>29</v>
+      </c>
+      <c r="E332">
+        <v>200</v>
+      </c>
+      <c r="F332" t="s">
+        <v>30</v>
+      </c>
+      <c r="G332" t="s">
+        <v>274</v>
+      </c>
+      <c r="H332" t="s">
+        <v>275</v>
+      </c>
+      <c r="I332" t="s">
+        <v>33</v>
+      </c>
+      <c r="J332" t="s">
+        <v>41</v>
+      </c>
+      <c r="K332" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>421</v>
+      </c>
+      <c r="B333" t="s">
+        <v>12</v>
+      </c>
+      <c r="C333" t="s">
+        <v>13</v>
+      </c>
+      <c r="D333" t="s">
+        <v>422</v>
+      </c>
+      <c r="E333">
+        <v>200</v>
+      </c>
+      <c r="F333" t="s">
+        <v>30</v>
+      </c>
+      <c r="G333" t="s">
+        <v>274</v>
+      </c>
+      <c r="H333" t="s">
+        <v>275</v>
+      </c>
+      <c r="I333" t="s">
+        <v>33</v>
+      </c>
+      <c r="J333" t="s">
+        <v>37</v>
+      </c>
+      <c r="K333" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>423</v>
+      </c>
+      <c r="B334" t="s">
+        <v>12</v>
+      </c>
+      <c r="C334" t="s">
+        <v>13</v>
+      </c>
+      <c r="D334" t="s">
+        <v>271</v>
+      </c>
+      <c r="E334">
+        <v>200</v>
+      </c>
+      <c r="F334" t="s">
+        <v>30</v>
+      </c>
+      <c r="G334" t="s">
+        <v>274</v>
+      </c>
+      <c r="H334" t="s">
+        <v>275</v>
+      </c>
+      <c r="I334" t="s">
+        <v>16</v>
+      </c>
+      <c r="J334" t="s">
+        <v>39</v>
+      </c>
+      <c r="K334" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>424</v>
+      </c>
+      <c r="B335" t="s">
+        <v>12</v>
+      </c>
+      <c r="C335" t="s">
+        <v>28</v>
+      </c>
+      <c r="D335" t="s">
+        <v>29</v>
+      </c>
+      <c r="E335">
+        <v>200</v>
+      </c>
+      <c r="F335" t="s">
+        <v>30</v>
+      </c>
+      <c r="G335" t="s">
+        <v>274</v>
+      </c>
+      <c r="H335" t="s">
+        <v>275</v>
+      </c>
+      <c r="I335" t="s">
+        <v>425</v>
+      </c>
+      <c r="J335" t="s">
+        <v>41</v>
+      </c>
+      <c r="K335" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>426</v>
+      </c>
+      <c r="B336" t="s">
+        <v>12</v>
+      </c>
+      <c r="C336" t="s">
+        <v>13</v>
+      </c>
+      <c r="D336" t="s">
+        <v>427</v>
+      </c>
+      <c r="E336">
+        <v>200</v>
+      </c>
+      <c r="F336" t="s">
+        <v>30</v>
+      </c>
+      <c r="G336" t="s">
+        <v>274</v>
+      </c>
+      <c r="H336" t="s">
+        <v>275</v>
+      </c>
+      <c r="I336" t="s">
+        <v>425</v>
+      </c>
+      <c r="J336" t="s">
+        <v>37</v>
+      </c>
+      <c r="K336" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>428</v>
+      </c>
+      <c r="B337" t="s">
+        <v>12</v>
+      </c>
+      <c r="C337" t="s">
+        <v>13</v>
+      </c>
+      <c r="D337" t="s">
+        <v>271</v>
+      </c>
+      <c r="E337">
+        <v>200</v>
+      </c>
+      <c r="F337" t="s">
+        <v>30</v>
+      </c>
+      <c r="G337" t="s">
+        <v>274</v>
+      </c>
+      <c r="H337" t="s">
+        <v>275</v>
+      </c>
+      <c r="I337" t="s">
+        <v>16</v>
+      </c>
+      <c r="J337" t="s">
+        <v>39</v>
+      </c>
+      <c r="K337" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>429</v>
+      </c>
+      <c r="B338" t="s">
+        <v>12</v>
+      </c>
+      <c r="C338" t="s">
+        <v>13</v>
+      </c>
+      <c r="D338" t="s">
+        <v>427</v>
+      </c>
+      <c r="E338">
+        <v>200</v>
+      </c>
+      <c r="F338" t="s">
+        <v>30</v>
+      </c>
+      <c r="G338" t="s">
+        <v>274</v>
+      </c>
+      <c r="H338" t="s">
+        <v>275</v>
+      </c>
+      <c r="I338" t="s">
+        <v>425</v>
+      </c>
+      <c r="J338" t="s">
+        <v>37</v>
+      </c>
+      <c r="K338" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>430</v>
+      </c>
+      <c r="B339" t="s">
+        <v>12</v>
+      </c>
+      <c r="C339" t="s">
+        <v>13</v>
+      </c>
+      <c r="D339" t="s">
+        <v>271</v>
+      </c>
+      <c r="E339">
+        <v>200</v>
+      </c>
+      <c r="F339" t="s">
+        <v>30</v>
+      </c>
+      <c r="G339" t="s">
+        <v>274</v>
+      </c>
+      <c r="H339" t="s">
+        <v>275</v>
+      </c>
+      <c r="I339" t="s">
+        <v>16</v>
+      </c>
+      <c r="J339" t="s">
+        <v>39</v>
+      </c>
+      <c r="K339" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>431</v>
+      </c>
+      <c r="B340" t="s">
+        <v>12</v>
+      </c>
+      <c r="C340" t="s">
+        <v>13</v>
+      </c>
+      <c r="D340" t="s">
+        <v>427</v>
+      </c>
+      <c r="E340">
+        <v>200</v>
+      </c>
+      <c r="F340" t="s">
+        <v>30</v>
+      </c>
+      <c r="G340" t="s">
+        <v>274</v>
+      </c>
+      <c r="H340" t="s">
+        <v>275</v>
+      </c>
+      <c r="I340" t="s">
+        <v>425</v>
+      </c>
+      <c r="J340" t="s">
+        <v>37</v>
+      </c>
+      <c r="K340" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>432</v>
+      </c>
+      <c r="B341" t="s">
+        <v>12</v>
+      </c>
+      <c r="C341" t="s">
+        <v>13</v>
+      </c>
+      <c r="D341" t="s">
+        <v>271</v>
+      </c>
+      <c r="E341">
+        <v>200</v>
+      </c>
+      <c r="F341" t="s">
+        <v>30</v>
+      </c>
+      <c r="G341" t="s">
+        <v>274</v>
+      </c>
+      <c r="H341" t="s">
+        <v>275</v>
+      </c>
+      <c r="I341" t="s">
+        <v>16</v>
+      </c>
+      <c r="J341" t="s">
+        <v>39</v>
+      </c>
+      <c r="K341" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>433</v>
+      </c>
+      <c r="B342" t="s">
+        <v>12</v>
+      </c>
+      <c r="C342" t="s">
+        <v>13</v>
+      </c>
+      <c r="D342" t="s">
+        <v>427</v>
+      </c>
+      <c r="E342">
+        <v>200</v>
+      </c>
+      <c r="F342" t="s">
+        <v>30</v>
+      </c>
+      <c r="G342" t="s">
+        <v>274</v>
+      </c>
+      <c r="H342" t="s">
+        <v>275</v>
+      </c>
+      <c r="I342" t="s">
+        <v>425</v>
+      </c>
+      <c r="J342" t="s">
+        <v>37</v>
+      </c>
+      <c r="K342" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>434</v>
+      </c>
+      <c r="B343" t="s">
+        <v>12</v>
+      </c>
+      <c r="C343" t="s">
+        <v>13</v>
+      </c>
+      <c r="D343" t="s">
+        <v>271</v>
+      </c>
+      <c r="E343">
+        <v>200</v>
+      </c>
+      <c r="F343" t="s">
+        <v>30</v>
+      </c>
+      <c r="G343" t="s">
+        <v>274</v>
+      </c>
+      <c r="H343" t="s">
+        <v>275</v>
+      </c>
+      <c r="I343" t="s">
+        <v>16</v>
+      </c>
+      <c r="J343" t="s">
+        <v>39</v>
+      </c>
+      <c r="K343" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>435</v>
+      </c>
+      <c r="B344" t="s">
+        <v>12</v>
+      </c>
+      <c r="C344" t="s">
+        <v>13</v>
+      </c>
+      <c r="D344" t="s">
+        <v>427</v>
+      </c>
+      <c r="E344">
+        <v>200</v>
+      </c>
+      <c r="F344" t="s">
+        <v>30</v>
+      </c>
+      <c r="G344" t="s">
+        <v>274</v>
+      </c>
+      <c r="H344" t="s">
+        <v>275</v>
+      </c>
+      <c r="I344" t="s">
+        <v>425</v>
+      </c>
+      <c r="J344" t="s">
+        <v>37</v>
+      </c>
+      <c r="K344" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>436</v>
+      </c>
+      <c r="B345" t="s">
+        <v>12</v>
+      </c>
+      <c r="C345" t="s">
+        <v>13</v>
+      </c>
+      <c r="D345" t="s">
+        <v>271</v>
+      </c>
+      <c r="E345">
+        <v>200</v>
+      </c>
+      <c r="F345" t="s">
+        <v>30</v>
+      </c>
+      <c r="G345" t="s">
+        <v>274</v>
+      </c>
+      <c r="H345" t="s">
+        <v>275</v>
+      </c>
+      <c r="I345" t="s">
+        <v>16</v>
+      </c>
+      <c r="J345" t="s">
+        <v>39</v>
+      </c>
+      <c r="K345" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>437</v>
+      </c>
+      <c r="B346" t="s">
+        <v>12</v>
+      </c>
+      <c r="C346" t="s">
+        <v>70</v>
+      </c>
+      <c r="D346" t="s">
+        <v>438</v>
+      </c>
+      <c r="E346">
+        <v>200</v>
+      </c>
+      <c r="F346" t="s">
+        <v>30</v>
+      </c>
+      <c r="G346" t="s">
+        <v>274</v>
+      </c>
+      <c r="H346" t="s">
+        <v>275</v>
+      </c>
+      <c r="I346" t="s">
+        <v>425</v>
+      </c>
+      <c r="J346" t="s">
+        <v>72</v>
+      </c>
+      <c r="K346" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>439</v>
+      </c>
+      <c r="B347" t="s">
+        <v>12</v>
+      </c>
+      <c r="C347" t="s">
+        <v>13</v>
+      </c>
+      <c r="D347" t="s">
+        <v>427</v>
+      </c>
+      <c r="E347">
+        <v>403</v>
+      </c>
+      <c r="F347" t="s">
+        <v>15</v>
+      </c>
+      <c r="G347" t="s">
+        <v>274</v>
+      </c>
+      <c r="H347" t="s">
+        <v>275</v>
+      </c>
+      <c r="I347" t="s">
+        <v>425</v>
+      </c>
+      <c r="J347" t="s">
+        <v>440</v>
+      </c>
+      <c r="K347" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>441</v>
+      </c>
+      <c r="B348" t="s">
+        <v>12</v>
+      </c>
+      <c r="C348" t="s">
+        <v>13</v>
+      </c>
+      <c r="D348" t="s">
+        <v>271</v>
+      </c>
+      <c r="E348">
+        <v>200</v>
+      </c>
+      <c r="F348" t="s">
+        <v>30</v>
+      </c>
+      <c r="G348" t="s">
+        <v>274</v>
+      </c>
+      <c r="H348" t="s">
+        <v>275</v>
+      </c>
+      <c r="I348" t="s">
+        <v>16</v>
+      </c>
+      <c r="J348" t="s">
+        <v>39</v>
+      </c>
+      <c r="K348" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>442</v>
+      </c>
+      <c r="B349" t="s">
+        <v>12</v>
+      </c>
+      <c r="C349" t="s">
+        <v>13</v>
+      </c>
+      <c r="D349" t="s">
+        <v>427</v>
+      </c>
+      <c r="E349">
+        <v>403</v>
+      </c>
+      <c r="F349" t="s">
+        <v>15</v>
+      </c>
+      <c r="G349" t="s">
+        <v>274</v>
+      </c>
+      <c r="H349" t="s">
+        <v>275</v>
+      </c>
+      <c r="I349" t="s">
+        <v>425</v>
+      </c>
+      <c r="J349" t="s">
+        <v>440</v>
+      </c>
+      <c r="K349" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>443</v>
+      </c>
+      <c r="B350" t="s">
+        <v>12</v>
+      </c>
+      <c r="C350" t="s">
+        <v>13</v>
+      </c>
+      <c r="D350" t="s">
+        <v>271</v>
+      </c>
+      <c r="E350">
+        <v>200</v>
+      </c>
+      <c r="F350" t="s">
+        <v>30</v>
+      </c>
+      <c r="G350" t="s">
+        <v>274</v>
+      </c>
+      <c r="H350" t="s">
+        <v>275</v>
+      </c>
+      <c r="I350" t="s">
+        <v>16</v>
+      </c>
+      <c r="J350" t="s">
+        <v>39</v>
+      </c>
+      <c r="K350" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>444</v>
+      </c>
+      <c r="B351" t="s">
+        <v>12</v>
+      </c>
+      <c r="C351" t="s">
+        <v>13</v>
+      </c>
+      <c r="D351" t="s">
+        <v>427</v>
+      </c>
+      <c r="E351">
+        <v>403</v>
+      </c>
+      <c r="F351" t="s">
+        <v>15</v>
+      </c>
+      <c r="G351" t="s">
+        <v>274</v>
+      </c>
+      <c r="H351" t="s">
+        <v>275</v>
+      </c>
+      <c r="I351" t="s">
+        <v>425</v>
+      </c>
+      <c r="J351" t="s">
+        <v>440</v>
+      </c>
+      <c r="K351" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>445</v>
+      </c>
+      <c r="B352" t="s">
+        <v>12</v>
+      </c>
+      <c r="C352" t="s">
+        <v>13</v>
+      </c>
+      <c r="D352" t="s">
+        <v>271</v>
+      </c>
+      <c r="E352">
+        <v>200</v>
+      </c>
+      <c r="F352" t="s">
+        <v>30</v>
+      </c>
+      <c r="G352" t="s">
+        <v>274</v>
+      </c>
+      <c r="H352" t="s">
+        <v>275</v>
+      </c>
+      <c r="I352" t="s">
+        <v>16</v>
+      </c>
+      <c r="J352" t="s">
+        <v>39</v>
+      </c>
+      <c r="K352" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>446</v>
+      </c>
+      <c r="B353" t="s">
+        <v>12</v>
+      </c>
+      <c r="C353" t="s">
+        <v>13</v>
+      </c>
+      <c r="D353" t="s">
+        <v>427</v>
+      </c>
+      <c r="E353">
+        <v>403</v>
+      </c>
+      <c r="F353" t="s">
+        <v>15</v>
+      </c>
+      <c r="G353" t="s">
+        <v>274</v>
+      </c>
+      <c r="H353" t="s">
+        <v>275</v>
+      </c>
+      <c r="I353" t="s">
+        <v>425</v>
+      </c>
+      <c r="J353" t="s">
+        <v>440</v>
+      </c>
+      <c r="K353" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>447</v>
+      </c>
+      <c r="B354" t="s">
+        <v>12</v>
+      </c>
+      <c r="C354" t="s">
+        <v>13</v>
+      </c>
+      <c r="D354" t="s">
+        <v>271</v>
+      </c>
+      <c r="E354">
+        <v>200</v>
+      </c>
+      <c r="F354" t="s">
+        <v>30</v>
+      </c>
+      <c r="G354" t="s">
+        <v>274</v>
+      </c>
+      <c r="H354" t="s">
+        <v>275</v>
+      </c>
+      <c r="I354" t="s">
+        <v>16</v>
+      </c>
+      <c r="J354" t="s">
+        <v>39</v>
+      </c>
+      <c r="K354" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>448</v>
+      </c>
+      <c r="B355" t="s">
+        <v>12</v>
+      </c>
+      <c r="C355" t="s">
+        <v>70</v>
+      </c>
+      <c r="D355" t="s">
+        <v>449</v>
+      </c>
+      <c r="E355">
+        <v>200</v>
+      </c>
+      <c r="F355" t="s">
+        <v>30</v>
+      </c>
+      <c r="G355" t="s">
+        <v>274</v>
+      </c>
+      <c r="H355" t="s">
+        <v>275</v>
+      </c>
+      <c r="I355" t="s">
+        <v>16</v>
+      </c>
+      <c r="J355" t="s">
+        <v>77</v>
+      </c>
+      <c r="K355" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>450</v>
+      </c>
+      <c r="B356" t="s">
+        <v>12</v>
+      </c>
+      <c r="C356" t="s">
+        <v>13</v>
+      </c>
+      <c r="D356" t="s">
+        <v>427</v>
+      </c>
+      <c r="E356">
+        <v>404</v>
+      </c>
+      <c r="F356" t="s">
+        <v>15</v>
+      </c>
+      <c r="G356" t="s">
+        <v>16</v>
+      </c>
+      <c r="H356" t="s">
+        <v>16</v>
+      </c>
+      <c r="I356" t="s">
+        <v>425</v>
+      </c>
+      <c r="J356" t="s">
+        <v>269</v>
+      </c>
+      <c r="K356" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>451</v>
+      </c>
+      <c r="B357" t="s">
+        <v>12</v>
+      </c>
+      <c r="C357" t="s">
+        <v>13</v>
+      </c>
+      <c r="D357" t="s">
+        <v>271</v>
+      </c>
+      <c r="E357">
+        <v>404</v>
+      </c>
+      <c r="F357" t="s">
+        <v>15</v>
+      </c>
+      <c r="G357" t="s">
+        <v>16</v>
+      </c>
+      <c r="H357" t="s">
+        <v>16</v>
+      </c>
+      <c r="I357" t="s">
+        <v>16</v>
+      </c>
+      <c r="J357" t="s">
+        <v>272</v>
+      </c>
+      <c r="K357" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>452</v>
+      </c>
+      <c r="B358" t="s">
+        <v>12</v>
+      </c>
+      <c r="C358" t="s">
+        <v>13</v>
+      </c>
+      <c r="D358" t="s">
+        <v>248</v>
+      </c>
+      <c r="E358">
+        <v>200</v>
+      </c>
+      <c r="F358" t="s">
+        <v>30</v>
+      </c>
+      <c r="G358" t="s">
+        <v>16</v>
+      </c>
+      <c r="H358" t="s">
+        <v>16</v>
+      </c>
+      <c r="I358" t="s">
+        <v>16</v>
+      </c>
+      <c r="J358" t="s">
+        <v>249</v>
+      </c>
+      <c r="K358" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>453</v>
+      </c>
+      <c r="B359" t="s">
+        <v>12</v>
+      </c>
+      <c r="C359" t="s">
+        <v>13</v>
+      </c>
+      <c r="D359" t="s">
+        <v>252</v>
+      </c>
+      <c r="E359">
+        <v>404</v>
+      </c>
+      <c r="F359" t="s">
+        <v>15</v>
+      </c>
+      <c r="G359" t="s">
+        <v>16</v>
+      </c>
+      <c r="H359" t="s">
+        <v>16</v>
+      </c>
+      <c r="I359" t="s">
+        <v>16</v>
+      </c>
+      <c r="J359" t="s">
+        <v>16</v>
+      </c>
+      <c r="K359" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>454</v>
+      </c>
+      <c r="B360" t="s">
+        <v>12</v>
+      </c>
+      <c r="C360" t="s">
+        <v>13</v>
+      </c>
+      <c r="D360" t="s">
+        <v>255</v>
+      </c>
+      <c r="E360">
+        <v>200</v>
+      </c>
+      <c r="F360" t="s">
+        <v>30</v>
+      </c>
+      <c r="G360" t="s">
+        <v>16</v>
+      </c>
+      <c r="H360" t="s">
+        <v>16</v>
+      </c>
+      <c r="I360" t="s">
+        <v>16</v>
+      </c>
+      <c r="J360" t="s">
+        <v>16</v>
+      </c>
+      <c r="K360" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>455</v>
+      </c>
+      <c r="B361" t="s">
+        <v>12</v>
+      </c>
+      <c r="C361" t="s">
+        <v>13</v>
+      </c>
+      <c r="D361" t="s">
+        <v>255</v>
+      </c>
+      <c r="E361">
+        <v>200</v>
+      </c>
+      <c r="F361" t="s">
+        <v>30</v>
+      </c>
+      <c r="G361" t="s">
+        <v>16</v>
+      </c>
+      <c r="H361" t="s">
+        <v>16</v>
+      </c>
+      <c r="I361" t="s">
+        <v>16</v>
+      </c>
+      <c r="J361" t="s">
+        <v>16</v>
+      </c>
+      <c r="K361" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>456</v>
+      </c>
+      <c r="B362" t="s">
+        <v>12</v>
+      </c>
+      <c r="C362" t="s">
+        <v>28</v>
+      </c>
+      <c r="D362" t="s">
+        <v>255</v>
+      </c>
+      <c r="E362">
+        <v>200</v>
+      </c>
+      <c r="F362" t="s">
+        <v>30</v>
+      </c>
+      <c r="G362" t="s">
+        <v>16</v>
+      </c>
+      <c r="H362" t="s">
+        <v>16</v>
+      </c>
+      <c r="I362" t="s">
+        <v>16</v>
+      </c>
+      <c r="J362" t="s">
+        <v>16</v>
+      </c>
+      <c r="K362" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>457</v>
+      </c>
+      <c r="B363" t="s">
+        <v>12</v>
+      </c>
+      <c r="C363" t="s">
+        <v>28</v>
+      </c>
+      <c r="D363" t="s">
+        <v>255</v>
+      </c>
+      <c r="E363">
+        <v>200</v>
+      </c>
+      <c r="F363" t="s">
+        <v>30</v>
+      </c>
+      <c r="G363" t="s">
+        <v>16</v>
+      </c>
+      <c r="H363" t="s">
+        <v>16</v>
+      </c>
+      <c r="I363" t="s">
+        <v>16</v>
+      </c>
+      <c r="J363" t="s">
+        <v>16</v>
+      </c>
+      <c r="K363" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>458</v>
+      </c>
+      <c r="B364" t="s">
+        <v>12</v>
+      </c>
+      <c r="C364" t="s">
+        <v>13</v>
+      </c>
+      <c r="D364" t="s">
+        <v>255</v>
+      </c>
+      <c r="E364">
+        <v>200</v>
+      </c>
+      <c r="F364" t="s">
+        <v>30</v>
+      </c>
+      <c r="G364" t="s">
+        <v>16</v>
+      </c>
+      <c r="H364" t="s">
+        <v>16</v>
+      </c>
+      <c r="I364" t="s">
+        <v>16</v>
+      </c>
+      <c r="J364" t="s">
+        <v>16</v>
+      </c>
+      <c r="K364" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>459</v>
+      </c>
+      <c r="B365" t="s">
+        <v>12</v>
+      </c>
+      <c r="C365" t="s">
+        <v>13</v>
+      </c>
+      <c r="D365" t="s">
+        <v>255</v>
+      </c>
+      <c r="E365">
+        <v>304</v>
+      </c>
+      <c r="F365" t="s">
+        <v>30</v>
+      </c>
+      <c r="G365" t="s">
+        <v>16</v>
+      </c>
+      <c r="H365" t="s">
+        <v>16</v>
+      </c>
+      <c r="I365" t="s">
+        <v>16</v>
+      </c>
+      <c r="J365" t="s">
+        <v>16</v>
+      </c>
+      <c r="K365" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>460</v>
+      </c>
+      <c r="B366" t="s">
+        <v>12</v>
+      </c>
+      <c r="C366" t="s">
+        <v>28</v>
+      </c>
+      <c r="D366" t="s">
+        <v>255</v>
+      </c>
+      <c r="E366">
+        <v>200</v>
+      </c>
+      <c r="F366" t="s">
+        <v>30</v>
+      </c>
+      <c r="G366" t="s">
+        <v>16</v>
+      </c>
+      <c r="H366" t="s">
+        <v>16</v>
+      </c>
+      <c r="I366" t="s">
+        <v>16</v>
+      </c>
+      <c r="J366" t="s">
+        <v>16</v>
+      </c>
+      <c r="K366" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>461</v>
+      </c>
+      <c r="B367" t="s">
+        <v>12</v>
+      </c>
+      <c r="C367" t="s">
+        <v>13</v>
+      </c>
+      <c r="D367" t="s">
+        <v>255</v>
+      </c>
+      <c r="E367">
+        <v>200</v>
+      </c>
+      <c r="F367" t="s">
+        <v>30</v>
+      </c>
+      <c r="G367" t="s">
+        <v>16</v>
+      </c>
+      <c r="H367" t="s">
+        <v>16</v>
+      </c>
+      <c r="I367" t="s">
+        <v>16</v>
+      </c>
+      <c r="J367" t="s">
+        <v>16</v>
+      </c>
+      <c r="K367" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>462</v>
+      </c>
+      <c r="B368" t="s">
+        <v>12</v>
+      </c>
+      <c r="C368" t="s">
+        <v>13</v>
+      </c>
+      <c r="D368" t="s">
+        <v>463</v>
+      </c>
+      <c r="E368">
+        <v>404</v>
+      </c>
+      <c r="F368" t="s">
+        <v>15</v>
+      </c>
+      <c r="G368" t="s">
+        <v>16</v>
+      </c>
+      <c r="H368" t="s">
+        <v>16</v>
+      </c>
+      <c r="I368" t="s">
+        <v>16</v>
+      </c>
+      <c r="J368" t="s">
+        <v>16</v>
+      </c>
+      <c r="K368" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>464</v>
+      </c>
+      <c r="B369" t="s">
+        <v>12</v>
+      </c>
+      <c r="C369" t="s">
+        <v>13</v>
+      </c>
+      <c r="D369" t="s">
+        <v>255</v>
+      </c>
+      <c r="E369">
+        <v>304</v>
+      </c>
+      <c r="F369" t="s">
+        <v>30</v>
+      </c>
+      <c r="G369" t="s">
+        <v>16</v>
+      </c>
+      <c r="H369" t="s">
+        <v>16</v>
+      </c>
+      <c r="I369" t="s">
+        <v>16</v>
+      </c>
+      <c r="J369" t="s">
+        <v>16</v>
+      </c>
+      <c r="K369" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>465</v>
+      </c>
+      <c r="B370" t="s">
+        <v>12</v>
+      </c>
+      <c r="C370" t="s">
+        <v>13</v>
+      </c>
+      <c r="D370" t="s">
+        <v>463</v>
+      </c>
+      <c r="E370">
+        <v>404</v>
+      </c>
+      <c r="F370" t="s">
+        <v>15</v>
+      </c>
+      <c r="G370" t="s">
+        <v>16</v>
+      </c>
+      <c r="H370" t="s">
+        <v>16</v>
+      </c>
+      <c r="I370" t="s">
+        <v>16</v>
+      </c>
+      <c r="J370" t="s">
+        <v>16</v>
+      </c>
+      <c r="K370" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>466</v>
+      </c>
+      <c r="B371" t="s">
+        <v>12</v>
+      </c>
+      <c r="C371" t="s">
+        <v>28</v>
+      </c>
+      <c r="D371" t="s">
+        <v>255</v>
+      </c>
+      <c r="E371">
+        <v>200</v>
+      </c>
+      <c r="F371" t="s">
+        <v>30</v>
+      </c>
+      <c r="G371" t="s">
+        <v>16</v>
+      </c>
+      <c r="H371" t="s">
+        <v>16</v>
+      </c>
+      <c r="I371" t="s">
+        <v>16</v>
+      </c>
+      <c r="J371" t="s">
+        <v>16</v>
+      </c>
+      <c r="K371" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>467</v>
+      </c>
+      <c r="B372" t="s">
+        <v>12</v>
+      </c>
+      <c r="C372" t="s">
+        <v>13</v>
+      </c>
+      <c r="D372" t="s">
+        <v>463</v>
+      </c>
+      <c r="E372">
+        <v>404</v>
+      </c>
+      <c r="F372" t="s">
+        <v>15</v>
+      </c>
+      <c r="G372" t="s">
+        <v>16</v>
+      </c>
+      <c r="H372" t="s">
+        <v>16</v>
+      </c>
+      <c r="I372" t="s">
+        <v>16</v>
+      </c>
+      <c r="J372" t="s">
+        <v>16</v>
+      </c>
+      <c r="K372" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>468</v>
+      </c>
+      <c r="B373" t="s">
+        <v>12</v>
+      </c>
+      <c r="C373" t="s">
+        <v>13</v>
+      </c>
+      <c r="D373" t="s">
+        <v>255</v>
+      </c>
+      <c r="E373">
+        <v>200</v>
+      </c>
+      <c r="F373" t="s">
+        <v>30</v>
+      </c>
+      <c r="G373" t="s">
+        <v>16</v>
+      </c>
+      <c r="H373" t="s">
+        <v>16</v>
+      </c>
+      <c r="I373" t="s">
+        <v>16</v>
+      </c>
+      <c r="J373" t="s">
+        <v>16</v>
+      </c>
+      <c r="K373" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>469</v>
+      </c>
+      <c r="B374" t="s">
+        <v>12</v>
+      </c>
+      <c r="C374" t="s">
+        <v>13</v>
+      </c>
+      <c r="D374" t="s">
+        <v>255</v>
+      </c>
+      <c r="E374">
+        <v>304</v>
+      </c>
+      <c r="F374" t="s">
+        <v>30</v>
+      </c>
+      <c r="G374" t="s">
+        <v>16</v>
+      </c>
+      <c r="H374" t="s">
+        <v>16</v>
+      </c>
+      <c r="I374" t="s">
+        <v>16</v>
+      </c>
+      <c r="J374" t="s">
+        <v>16</v>
+      </c>
+      <c r="K374" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>470</v>
+      </c>
+      <c r="B375" t="s">
+        <v>12</v>
+      </c>
+      <c r="C375" t="s">
+        <v>28</v>
+      </c>
+      <c r="D375" t="s">
+        <v>255</v>
+      </c>
+      <c r="E375">
+        <v>200</v>
+      </c>
+      <c r="F375" t="s">
+        <v>30</v>
+      </c>
+      <c r="G375" t="s">
+        <v>16</v>
+      </c>
+      <c r="H375" t="s">
+        <v>16</v>
+      </c>
+      <c r="I375" t="s">
+        <v>16</v>
+      </c>
+      <c r="J375" t="s">
+        <v>16</v>
+      </c>
+      <c r="K375" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>471</v>
+      </c>
+      <c r="B376" t="s">
+        <v>12</v>
+      </c>
+      <c r="C376" t="s">
+        <v>13</v>
+      </c>
+      <c r="D376" t="s">
+        <v>472</v>
+      </c>
+      <c r="E376">
+        <v>404</v>
+      </c>
+      <c r="F376" t="s">
+        <v>15</v>
+      </c>
+      <c r="G376" t="s">
+        <v>16</v>
+      </c>
+      <c r="H376" t="s">
+        <v>16</v>
+      </c>
+      <c r="I376" t="s">
+        <v>16</v>
+      </c>
+      <c r="J376" t="s">
+        <v>16</v>
+      </c>
+      <c r="K376" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>473</v>
+      </c>
+      <c r="B377" t="s">
+        <v>12</v>
+      </c>
+      <c r="C377" t="s">
+        <v>13</v>
+      </c>
+      <c r="D377" t="s">
+        <v>472</v>
+      </c>
+      <c r="E377">
+        <v>404</v>
+      </c>
+      <c r="F377" t="s">
+        <v>15</v>
+      </c>
+      <c r="G377" t="s">
+        <v>16</v>
+      </c>
+      <c r="H377" t="s">
+        <v>16</v>
+      </c>
+      <c r="I377" t="s">
+        <v>16</v>
+      </c>
+      <c r="J377" t="s">
+        <v>16</v>
+      </c>
+      <c r="K377" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>474</v>
+      </c>
+      <c r="B378" t="s">
+        <v>12</v>
+      </c>
+      <c r="C378" t="s">
+        <v>13</v>
+      </c>
+      <c r="D378" t="s">
+        <v>255</v>
+      </c>
+      <c r="E378">
+        <v>200</v>
+      </c>
+      <c r="F378" t="s">
+        <v>30</v>
+      </c>
+      <c r="G378" t="s">
+        <v>16</v>
+      </c>
+      <c r="H378" t="s">
+        <v>16</v>
+      </c>
+      <c r="I378" t="s">
+        <v>16</v>
+      </c>
+      <c r="J378" t="s">
+        <v>16</v>
+      </c>
+      <c r="K378" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>475</v>
+      </c>
+      <c r="B379" t="s">
+        <v>12</v>
+      </c>
+      <c r="C379" t="s">
+        <v>13</v>
+      </c>
+      <c r="D379" t="s">
+        <v>248</v>
+      </c>
+      <c r="E379">
+        <v>304</v>
+      </c>
+      <c r="F379" t="s">
+        <v>30</v>
+      </c>
+      <c r="G379" t="s">
+        <v>16</v>
+      </c>
+      <c r="H379" t="s">
+        <v>16</v>
+      </c>
+      <c r="I379" t="s">
+        <v>16</v>
+      </c>
+      <c r="J379" t="s">
+        <v>249</v>
+      </c>
+      <c r="K379" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>476</v>
+      </c>
+      <c r="B380" t="s">
+        <v>12</v>
+      </c>
+      <c r="C380" t="s">
+        <v>13</v>
+      </c>
+      <c r="D380" t="s">
+        <v>255</v>
+      </c>
+      <c r="E380">
+        <v>304</v>
+      </c>
+      <c r="F380" t="s">
+        <v>30</v>
+      </c>
+      <c r="G380" t="s">
+        <v>16</v>
+      </c>
+      <c r="H380" t="s">
+        <v>16</v>
+      </c>
+      <c r="I380" t="s">
+        <v>16</v>
+      </c>
+      <c r="J380" t="s">
+        <v>16</v>
+      </c>
+      <c r="K380" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>477</v>
+      </c>
+      <c r="B381" t="s">
+        <v>12</v>
+      </c>
+      <c r="C381" t="s">
+        <v>28</v>
+      </c>
+      <c r="D381" t="s">
+        <v>255</v>
+      </c>
+      <c r="E381">
+        <v>401</v>
+      </c>
+      <c r="F381" t="s">
+        <v>15</v>
+      </c>
+      <c r="G381" t="s">
+        <v>16</v>
+      </c>
+      <c r="H381" t="s">
+        <v>16</v>
+      </c>
+      <c r="I381" t="s">
+        <v>16</v>
+      </c>
+      <c r="J381" t="s">
+        <v>16</v>
+      </c>
+      <c r="K381" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>478</v>
+      </c>
+      <c r="B382" t="s">
+        <v>12</v>
+      </c>
+      <c r="C382" t="s">
+        <v>28</v>
+      </c>
+      <c r="D382" t="s">
+        <v>255</v>
+      </c>
+      <c r="E382">
+        <v>200</v>
+      </c>
+      <c r="F382" t="s">
+        <v>30</v>
+      </c>
+      <c r="G382" t="s">
+        <v>16</v>
+      </c>
+      <c r="H382" t="s">
+        <v>16</v>
+      </c>
+      <c r="I382" t="s">
+        <v>16</v>
+      </c>
+      <c r="J382" t="s">
+        <v>16</v>
+      </c>
+      <c r="K382" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Refactor access control project into modular files
Split esp32_access_control_full.ino.ino into hardware_ui.ino, http_backend.ino, and web_ui.ino for better code organization and maintainability. Moved hardware, backend, and web UI logic to dedicated files and updated function prototypes and includes accordingly.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/logs.xlsx
+++ b/Server/rfid-server-DBS-Http/logs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3821" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3981" uniqueCount="501">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1448,6 +1448,72 @@
   </si>
   <si>
     <t>2025-11-28T04:48:07.957Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:40.546Z</t>
+  </si>
+  <si>
+    <t>/user/EA4C7814?roomID=109</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:40.877Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:42.653Z</t>
+  </si>
+  <si>
+    <t>/user/EA4C7814?roomID=110</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:42.729Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:47.872Z</t>
+  </si>
+  <si>
+    <t>/user/EA4C7814?roomID=107</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:48.183Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:48.696Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:49.137Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:51.265Z</t>
+  </si>
+  <si>
+    <t>/user/EA4C7814?roomID=106</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:51.338Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:53.820Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:53.951Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:54.042Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:54.092Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:55.777Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:22:55.829Z</t>
   </si>
 </sst>
 </file>
@@ -1824,7 +1890,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K382"/>
+  <dimension ref="A1:K398"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -15197,6 +15263,566 @@
         <v>250</v>
       </c>
     </row>
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>479</v>
+      </c>
+      <c r="B383" t="s">
+        <v>12</v>
+      </c>
+      <c r="C383" t="s">
+        <v>13</v>
+      </c>
+      <c r="D383" t="s">
+        <v>480</v>
+      </c>
+      <c r="E383">
+        <v>404</v>
+      </c>
+      <c r="F383" t="s">
+        <v>15</v>
+      </c>
+      <c r="G383" t="s">
+        <v>16</v>
+      </c>
+      <c r="H383" t="s">
+        <v>16</v>
+      </c>
+      <c r="I383" t="s">
+        <v>17</v>
+      </c>
+      <c r="J383" t="s">
+        <v>377</v>
+      </c>
+      <c r="K383" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>481</v>
+      </c>
+      <c r="B384" t="s">
+        <v>12</v>
+      </c>
+      <c r="C384" t="s">
+        <v>13</v>
+      </c>
+      <c r="D384" t="s">
+        <v>379</v>
+      </c>
+      <c r="E384">
+        <v>404</v>
+      </c>
+      <c r="F384" t="s">
+        <v>15</v>
+      </c>
+      <c r="G384" t="s">
+        <v>16</v>
+      </c>
+      <c r="H384" t="s">
+        <v>16</v>
+      </c>
+      <c r="I384" t="s">
+        <v>16</v>
+      </c>
+      <c r="J384" t="s">
+        <v>380</v>
+      </c>
+      <c r="K384" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>482</v>
+      </c>
+      <c r="B385" t="s">
+        <v>12</v>
+      </c>
+      <c r="C385" t="s">
+        <v>13</v>
+      </c>
+      <c r="D385" t="s">
+        <v>483</v>
+      </c>
+      <c r="E385">
+        <v>404</v>
+      </c>
+      <c r="F385" t="s">
+        <v>15</v>
+      </c>
+      <c r="G385" t="s">
+        <v>16</v>
+      </c>
+      <c r="H385" t="s">
+        <v>16</v>
+      </c>
+      <c r="I385" t="s">
+        <v>484</v>
+      </c>
+      <c r="J385" t="s">
+        <v>377</v>
+      </c>
+      <c r="K385" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>485</v>
+      </c>
+      <c r="B386" t="s">
+        <v>12</v>
+      </c>
+      <c r="C386" t="s">
+        <v>13</v>
+      </c>
+      <c r="D386" t="s">
+        <v>379</v>
+      </c>
+      <c r="E386">
+        <v>404</v>
+      </c>
+      <c r="F386" t="s">
+        <v>15</v>
+      </c>
+      <c r="G386" t="s">
+        <v>16</v>
+      </c>
+      <c r="H386" t="s">
+        <v>16</v>
+      </c>
+      <c r="I386" t="s">
+        <v>16</v>
+      </c>
+      <c r="J386" t="s">
+        <v>380</v>
+      </c>
+      <c r="K386" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>486</v>
+      </c>
+      <c r="B387" t="s">
+        <v>12</v>
+      </c>
+      <c r="C387" t="s">
+        <v>13</v>
+      </c>
+      <c r="D387" t="s">
+        <v>487</v>
+      </c>
+      <c r="E387">
+        <v>404</v>
+      </c>
+      <c r="F387" t="s">
+        <v>15</v>
+      </c>
+      <c r="G387" t="s">
+        <v>16</v>
+      </c>
+      <c r="H387" t="s">
+        <v>16</v>
+      </c>
+      <c r="I387" t="s">
+        <v>488</v>
+      </c>
+      <c r="J387" t="s">
+        <v>377</v>
+      </c>
+      <c r="K387" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>489</v>
+      </c>
+      <c r="B388" t="s">
+        <v>12</v>
+      </c>
+      <c r="C388" t="s">
+        <v>13</v>
+      </c>
+      <c r="D388" t="s">
+        <v>379</v>
+      </c>
+      <c r="E388">
+        <v>404</v>
+      </c>
+      <c r="F388" t="s">
+        <v>15</v>
+      </c>
+      <c r="G388" t="s">
+        <v>16</v>
+      </c>
+      <c r="H388" t="s">
+        <v>16</v>
+      </c>
+      <c r="I388" t="s">
+        <v>16</v>
+      </c>
+      <c r="J388" t="s">
+        <v>380</v>
+      </c>
+      <c r="K388" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>490</v>
+      </c>
+      <c r="B389" t="s">
+        <v>12</v>
+      </c>
+      <c r="C389" t="s">
+        <v>13</v>
+      </c>
+      <c r="D389" t="s">
+        <v>487</v>
+      </c>
+      <c r="E389">
+        <v>404</v>
+      </c>
+      <c r="F389" t="s">
+        <v>15</v>
+      </c>
+      <c r="G389" t="s">
+        <v>16</v>
+      </c>
+      <c r="H389" t="s">
+        <v>16</v>
+      </c>
+      <c r="I389" t="s">
+        <v>488</v>
+      </c>
+      <c r="J389" t="s">
+        <v>377</v>
+      </c>
+      <c r="K389" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>491</v>
+      </c>
+      <c r="B390" t="s">
+        <v>12</v>
+      </c>
+      <c r="C390" t="s">
+        <v>13</v>
+      </c>
+      <c r="D390" t="s">
+        <v>379</v>
+      </c>
+      <c r="E390">
+        <v>404</v>
+      </c>
+      <c r="F390" t="s">
+        <v>15</v>
+      </c>
+      <c r="G390" t="s">
+        <v>16</v>
+      </c>
+      <c r="H390" t="s">
+        <v>16</v>
+      </c>
+      <c r="I390" t="s">
+        <v>16</v>
+      </c>
+      <c r="J390" t="s">
+        <v>380</v>
+      </c>
+      <c r="K390" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>492</v>
+      </c>
+      <c r="B391" t="s">
+        <v>12</v>
+      </c>
+      <c r="C391" t="s">
+        <v>13</v>
+      </c>
+      <c r="D391" t="s">
+        <v>493</v>
+      </c>
+      <c r="E391">
+        <v>404</v>
+      </c>
+      <c r="F391" t="s">
+        <v>15</v>
+      </c>
+      <c r="G391" t="s">
+        <v>16</v>
+      </c>
+      <c r="H391" t="s">
+        <v>16</v>
+      </c>
+      <c r="I391" t="s">
+        <v>33</v>
+      </c>
+      <c r="J391" t="s">
+        <v>377</v>
+      </c>
+      <c r="K391" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>494</v>
+      </c>
+      <c r="B392" t="s">
+        <v>12</v>
+      </c>
+      <c r="C392" t="s">
+        <v>13</v>
+      </c>
+      <c r="D392" t="s">
+        <v>379</v>
+      </c>
+      <c r="E392">
+        <v>404</v>
+      </c>
+      <c r="F392" t="s">
+        <v>15</v>
+      </c>
+      <c r="G392" t="s">
+        <v>16</v>
+      </c>
+      <c r="H392" t="s">
+        <v>16</v>
+      </c>
+      <c r="I392" t="s">
+        <v>16</v>
+      </c>
+      <c r="J392" t="s">
+        <v>380</v>
+      </c>
+      <c r="K392" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>495</v>
+      </c>
+      <c r="B393" t="s">
+        <v>12</v>
+      </c>
+      <c r="C393" t="s">
+        <v>13</v>
+      </c>
+      <c r="D393" t="s">
+        <v>388</v>
+      </c>
+      <c r="E393">
+        <v>404</v>
+      </c>
+      <c r="F393" t="s">
+        <v>15</v>
+      </c>
+      <c r="G393" t="s">
+        <v>16</v>
+      </c>
+      <c r="H393" t="s">
+        <v>16</v>
+      </c>
+      <c r="I393" t="s">
+        <v>43</v>
+      </c>
+      <c r="J393" t="s">
+        <v>377</v>
+      </c>
+      <c r="K393" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>496</v>
+      </c>
+      <c r="B394" t="s">
+        <v>12</v>
+      </c>
+      <c r="C394" t="s">
+        <v>13</v>
+      </c>
+      <c r="D394" t="s">
+        <v>379</v>
+      </c>
+      <c r="E394">
+        <v>404</v>
+      </c>
+      <c r="F394" t="s">
+        <v>15</v>
+      </c>
+      <c r="G394" t="s">
+        <v>16</v>
+      </c>
+      <c r="H394" t="s">
+        <v>16</v>
+      </c>
+      <c r="I394" t="s">
+        <v>16</v>
+      </c>
+      <c r="J394" t="s">
+        <v>380</v>
+      </c>
+      <c r="K394" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>497</v>
+      </c>
+      <c r="B395" t="s">
+        <v>12</v>
+      </c>
+      <c r="C395" t="s">
+        <v>13</v>
+      </c>
+      <c r="D395" t="s">
+        <v>493</v>
+      </c>
+      <c r="E395">
+        <v>404</v>
+      </c>
+      <c r="F395" t="s">
+        <v>15</v>
+      </c>
+      <c r="G395" t="s">
+        <v>16</v>
+      </c>
+      <c r="H395" t="s">
+        <v>16</v>
+      </c>
+      <c r="I395" t="s">
+        <v>33</v>
+      </c>
+      <c r="J395" t="s">
+        <v>377</v>
+      </c>
+      <c r="K395" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>498</v>
+      </c>
+      <c r="B396" t="s">
+        <v>12</v>
+      </c>
+      <c r="C396" t="s">
+        <v>13</v>
+      </c>
+      <c r="D396" t="s">
+        <v>379</v>
+      </c>
+      <c r="E396">
+        <v>404</v>
+      </c>
+      <c r="F396" t="s">
+        <v>15</v>
+      </c>
+      <c r="G396" t="s">
+        <v>16</v>
+      </c>
+      <c r="H396" t="s">
+        <v>16</v>
+      </c>
+      <c r="I396" t="s">
+        <v>16</v>
+      </c>
+      <c r="J396" t="s">
+        <v>380</v>
+      </c>
+      <c r="K396" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>499</v>
+      </c>
+      <c r="B397" t="s">
+        <v>12</v>
+      </c>
+      <c r="C397" t="s">
+        <v>13</v>
+      </c>
+      <c r="D397" t="s">
+        <v>388</v>
+      </c>
+      <c r="E397">
+        <v>404</v>
+      </c>
+      <c r="F397" t="s">
+        <v>15</v>
+      </c>
+      <c r="G397" t="s">
+        <v>16</v>
+      </c>
+      <c r="H397" t="s">
+        <v>16</v>
+      </c>
+      <c r="I397" t="s">
+        <v>43</v>
+      </c>
+      <c r="J397" t="s">
+        <v>377</v>
+      </c>
+      <c r="K397" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>500</v>
+      </c>
+      <c r="B398" t="s">
+        <v>12</v>
+      </c>
+      <c r="C398" t="s">
+        <v>13</v>
+      </c>
+      <c r="D398" t="s">
+        <v>379</v>
+      </c>
+      <c r="E398">
+        <v>404</v>
+      </c>
+      <c r="F398" t="s">
+        <v>15</v>
+      </c>
+      <c r="G398" t="s">
+        <v>16</v>
+      </c>
+      <c r="H398" t="s">
+        <v>16</v>
+      </c>
+      <c r="I398" t="s">
+        <v>16</v>
+      </c>
+      <c r="J398" t="s">
+        <v>380</v>
+      </c>
+      <c r="K398" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Refactor status handling and UI color logic
Introduced a StatusCode enum and centralized status management for access control events. Updated hardware UI to use named RGB color constants and timing values, improving code clarity and maintainability. Web UI now serves CSS and JS as static resources, reducing inline code duplication. Minor timing and status logic adjustments for consistency.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/logs.xlsx
+++ b/Server/rfid-server-DBS-Http/logs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3981" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4021" uniqueCount="505">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1514,6 +1514,18 @@
   </si>
   <si>
     <t>2025-11-28T20:22:55.829Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:27:22.059Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:27:22.506Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:55:58.652Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T20:55:58.746Z</t>
   </si>
 </sst>
 </file>
@@ -1890,7 +1902,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K398"/>
+  <dimension ref="A1:K402"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -15823,6 +15835,146 @@
         <v>19</v>
       </c>
     </row>
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>501</v>
+      </c>
+      <c r="B399" t="s">
+        <v>12</v>
+      </c>
+      <c r="C399" t="s">
+        <v>13</v>
+      </c>
+      <c r="D399" t="s">
+        <v>388</v>
+      </c>
+      <c r="E399">
+        <v>404</v>
+      </c>
+      <c r="F399" t="s">
+        <v>15</v>
+      </c>
+      <c r="G399" t="s">
+        <v>16</v>
+      </c>
+      <c r="H399" t="s">
+        <v>16</v>
+      </c>
+      <c r="I399" t="s">
+        <v>43</v>
+      </c>
+      <c r="J399" t="s">
+        <v>377</v>
+      </c>
+      <c r="K399" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>502</v>
+      </c>
+      <c r="B400" t="s">
+        <v>12</v>
+      </c>
+      <c r="C400" t="s">
+        <v>13</v>
+      </c>
+      <c r="D400" t="s">
+        <v>379</v>
+      </c>
+      <c r="E400">
+        <v>404</v>
+      </c>
+      <c r="F400" t="s">
+        <v>15</v>
+      </c>
+      <c r="G400" t="s">
+        <v>16</v>
+      </c>
+      <c r="H400" t="s">
+        <v>16</v>
+      </c>
+      <c r="I400" t="s">
+        <v>16</v>
+      </c>
+      <c r="J400" t="s">
+        <v>380</v>
+      </c>
+      <c r="K400" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>503</v>
+      </c>
+      <c r="B401" t="s">
+        <v>12</v>
+      </c>
+      <c r="C401" t="s">
+        <v>13</v>
+      </c>
+      <c r="D401" t="s">
+        <v>388</v>
+      </c>
+      <c r="E401">
+        <v>404</v>
+      </c>
+      <c r="F401" t="s">
+        <v>15</v>
+      </c>
+      <c r="G401" t="s">
+        <v>16</v>
+      </c>
+      <c r="H401" t="s">
+        <v>16</v>
+      </c>
+      <c r="I401" t="s">
+        <v>43</v>
+      </c>
+      <c r="J401" t="s">
+        <v>377</v>
+      </c>
+      <c r="K401" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>504</v>
+      </c>
+      <c r="B402" t="s">
+        <v>12</v>
+      </c>
+      <c r="C402" t="s">
+        <v>13</v>
+      </c>
+      <c r="D402" t="s">
+        <v>379</v>
+      </c>
+      <c r="E402">
+        <v>404</v>
+      </c>
+      <c r="F402" t="s">
+        <v>15</v>
+      </c>
+      <c r="G402" t="s">
+        <v>16</v>
+      </c>
+      <c r="H402" t="s">
+        <v>16</v>
+      </c>
+      <c r="I402" t="s">
+        <v>16</v>
+      </c>
+      <c r="J402" t="s">
+        <v>380</v>
+      </c>
+      <c r="K402" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Revamp web UI with dark theme and improved tables
Updated the web UI CSS for a modern dark theme, enhanced table styling, and improved layout for better readability. Adjusted HTML generation to use new table wrappers and classes. Also updated logs.xlsx and users.xlsx files.

just made sure Esp server side style matches backedn css style
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/logs.xlsx
+++ b/Server/rfid-server-DBS-Http/logs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4021" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4141" uniqueCount="518">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1526,6 +1526,45 @@
   </si>
   <si>
     <t>2025-11-28T20:55:58.746Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:00:37.882Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:00:38.339Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:00:42.719Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:00:43.001Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:00:56.442Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:01:17.110Z</t>
+  </si>
+  <si>
+    <t>hhhhhhhhhhhhhhhhhhhhhhh</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:01:19.295Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:01:19.436Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:01:24.691Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:01:24.744Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:01:31.476Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:01:31.524Z</t>
   </si>
 </sst>
 </file>
@@ -1902,7 +1941,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K402"/>
+  <dimension ref="A1:K414"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -15975,6 +16014,426 @@
         <v>19</v>
       </c>
     </row>
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>505</v>
+      </c>
+      <c r="B403" t="s">
+        <v>12</v>
+      </c>
+      <c r="C403" t="s">
+        <v>13</v>
+      </c>
+      <c r="D403" t="s">
+        <v>388</v>
+      </c>
+      <c r="E403">
+        <v>404</v>
+      </c>
+      <c r="F403" t="s">
+        <v>15</v>
+      </c>
+      <c r="G403" t="s">
+        <v>16</v>
+      </c>
+      <c r="H403" t="s">
+        <v>16</v>
+      </c>
+      <c r="I403" t="s">
+        <v>43</v>
+      </c>
+      <c r="J403" t="s">
+        <v>377</v>
+      </c>
+      <c r="K403" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>506</v>
+      </c>
+      <c r="B404" t="s">
+        <v>12</v>
+      </c>
+      <c r="C404" t="s">
+        <v>13</v>
+      </c>
+      <c r="D404" t="s">
+        <v>379</v>
+      </c>
+      <c r="E404">
+        <v>404</v>
+      </c>
+      <c r="F404" t="s">
+        <v>15</v>
+      </c>
+      <c r="G404" t="s">
+        <v>16</v>
+      </c>
+      <c r="H404" t="s">
+        <v>16</v>
+      </c>
+      <c r="I404" t="s">
+        <v>16</v>
+      </c>
+      <c r="J404" t="s">
+        <v>380</v>
+      </c>
+      <c r="K404" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>507</v>
+      </c>
+      <c r="B405" t="s">
+        <v>12</v>
+      </c>
+      <c r="C405" t="s">
+        <v>13</v>
+      </c>
+      <c r="D405" t="s">
+        <v>388</v>
+      </c>
+      <c r="E405">
+        <v>404</v>
+      </c>
+      <c r="F405" t="s">
+        <v>15</v>
+      </c>
+      <c r="G405" t="s">
+        <v>16</v>
+      </c>
+      <c r="H405" t="s">
+        <v>16</v>
+      </c>
+      <c r="I405" t="s">
+        <v>43</v>
+      </c>
+      <c r="J405" t="s">
+        <v>377</v>
+      </c>
+      <c r="K405" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>508</v>
+      </c>
+      <c r="B406" t="s">
+        <v>12</v>
+      </c>
+      <c r="C406" t="s">
+        <v>13</v>
+      </c>
+      <c r="D406" t="s">
+        <v>379</v>
+      </c>
+      <c r="E406">
+        <v>404</v>
+      </c>
+      <c r="F406" t="s">
+        <v>15</v>
+      </c>
+      <c r="G406" t="s">
+        <v>16</v>
+      </c>
+      <c r="H406" t="s">
+        <v>16</v>
+      </c>
+      <c r="I406" t="s">
+        <v>16</v>
+      </c>
+      <c r="J406" t="s">
+        <v>380</v>
+      </c>
+      <c r="K406" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>509</v>
+      </c>
+      <c r="B407" t="s">
+        <v>12</v>
+      </c>
+      <c r="C407" t="s">
+        <v>13</v>
+      </c>
+      <c r="D407" t="s">
+        <v>50</v>
+      </c>
+      <c r="E407">
+        <v>200</v>
+      </c>
+      <c r="F407" t="s">
+        <v>30</v>
+      </c>
+      <c r="G407" t="s">
+        <v>31</v>
+      </c>
+      <c r="H407" t="s">
+        <v>51</v>
+      </c>
+      <c r="I407" t="s">
+        <v>16</v>
+      </c>
+      <c r="J407" t="s">
+        <v>52</v>
+      </c>
+      <c r="K407" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>510</v>
+      </c>
+      <c r="B408" t="s">
+        <v>12</v>
+      </c>
+      <c r="C408" t="s">
+        <v>28</v>
+      </c>
+      <c r="D408" t="s">
+        <v>29</v>
+      </c>
+      <c r="E408">
+        <v>200</v>
+      </c>
+      <c r="F408" t="s">
+        <v>30</v>
+      </c>
+      <c r="G408" t="s">
+        <v>511</v>
+      </c>
+      <c r="H408" t="s">
+        <v>400</v>
+      </c>
+      <c r="I408" t="s">
+        <v>43</v>
+      </c>
+      <c r="J408" t="s">
+        <v>34</v>
+      </c>
+      <c r="K408" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>512</v>
+      </c>
+      <c r="B409" t="s">
+        <v>12</v>
+      </c>
+      <c r="C409" t="s">
+        <v>13</v>
+      </c>
+      <c r="D409" t="s">
+        <v>393</v>
+      </c>
+      <c r="E409">
+        <v>200</v>
+      </c>
+      <c r="F409" t="s">
+        <v>30</v>
+      </c>
+      <c r="G409" t="s">
+        <v>511</v>
+      </c>
+      <c r="H409" t="s">
+        <v>400</v>
+      </c>
+      <c r="I409" t="s">
+        <v>43</v>
+      </c>
+      <c r="J409" t="s">
+        <v>37</v>
+      </c>
+      <c r="K409" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>513</v>
+      </c>
+      <c r="B410" t="s">
+        <v>12</v>
+      </c>
+      <c r="C410" t="s">
+        <v>13</v>
+      </c>
+      <c r="D410" t="s">
+        <v>396</v>
+      </c>
+      <c r="E410">
+        <v>200</v>
+      </c>
+      <c r="F410" t="s">
+        <v>30</v>
+      </c>
+      <c r="G410" t="s">
+        <v>511</v>
+      </c>
+      <c r="H410" t="s">
+        <v>400</v>
+      </c>
+      <c r="I410" t="s">
+        <v>16</v>
+      </c>
+      <c r="J410" t="s">
+        <v>39</v>
+      </c>
+      <c r="K410" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>514</v>
+      </c>
+      <c r="B411" t="s">
+        <v>12</v>
+      </c>
+      <c r="C411" t="s">
+        <v>13</v>
+      </c>
+      <c r="D411" t="s">
+        <v>393</v>
+      </c>
+      <c r="E411">
+        <v>200</v>
+      </c>
+      <c r="F411" t="s">
+        <v>30</v>
+      </c>
+      <c r="G411" t="s">
+        <v>511</v>
+      </c>
+      <c r="H411" t="s">
+        <v>400</v>
+      </c>
+      <c r="I411" t="s">
+        <v>43</v>
+      </c>
+      <c r="J411" t="s">
+        <v>37</v>
+      </c>
+      <c r="K411" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>515</v>
+      </c>
+      <c r="B412" t="s">
+        <v>12</v>
+      </c>
+      <c r="C412" t="s">
+        <v>13</v>
+      </c>
+      <c r="D412" t="s">
+        <v>396</v>
+      </c>
+      <c r="E412">
+        <v>200</v>
+      </c>
+      <c r="F412" t="s">
+        <v>30</v>
+      </c>
+      <c r="G412" t="s">
+        <v>511</v>
+      </c>
+      <c r="H412" t="s">
+        <v>400</v>
+      </c>
+      <c r="I412" t="s">
+        <v>16</v>
+      </c>
+      <c r="J412" t="s">
+        <v>39</v>
+      </c>
+      <c r="K412" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>516</v>
+      </c>
+      <c r="B413" t="s">
+        <v>12</v>
+      </c>
+      <c r="C413" t="s">
+        <v>13</v>
+      </c>
+      <c r="D413" t="s">
+        <v>393</v>
+      </c>
+      <c r="E413">
+        <v>200</v>
+      </c>
+      <c r="F413" t="s">
+        <v>30</v>
+      </c>
+      <c r="G413" t="s">
+        <v>511</v>
+      </c>
+      <c r="H413" t="s">
+        <v>400</v>
+      </c>
+      <c r="I413" t="s">
+        <v>43</v>
+      </c>
+      <c r="J413" t="s">
+        <v>37</v>
+      </c>
+      <c r="K413" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>517</v>
+      </c>
+      <c r="B414" t="s">
+        <v>12</v>
+      </c>
+      <c r="C414" t="s">
+        <v>13</v>
+      </c>
+      <c r="D414" t="s">
+        <v>396</v>
+      </c>
+      <c r="E414">
+        <v>200</v>
+      </c>
+      <c r="F414" t="s">
+        <v>30</v>
+      </c>
+      <c r="G414" t="s">
+        <v>511</v>
+      </c>
+      <c r="H414" t="s">
+        <v>400</v>
+      </c>
+      <c r="I414" t="s">
+        <v>16</v>
+      </c>
+      <c r="J414" t="s">
+        <v>39</v>
+      </c>
+      <c r="K414" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Refactor ESP32 access control for hardware and backend
Reorganized configuration, pin definitions, and backend URL construction for flexibility. Improved hardware UI logic with relay and buzzer support, added debounce to touch input, and made RFID verification non-blocking. Simplified web UI HTML builders and added input validation for registration. Backend HTTP functions now use dynamic URLs and improved error handling.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/logs.xlsx
+++ b/Server/rfid-server-DBS-Http/logs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4141" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4441" uniqueCount="554">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1565,6 +1565,114 @@
   </si>
   <si>
     <t>2025-11-28T21:01:31.524Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:11:45.314Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:11:45.846Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:11:50.643Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:14:03.198Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:14:03.300Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:14:14.866Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:14:20.639Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:14:20.699Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:14:53.157Z</t>
+  </si>
+  <si>
+    <t>rgggg</t>
+  </si>
+  <si>
+    <t>EA4C7814</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:14:58.817Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:02.108Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:02.387Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:02.934Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:03.032Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:04.563Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:21.526Z</t>
+  </si>
+  <si>
+    <t>/room/EA4C7814/105</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:23.737Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:23.779Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:26.776Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:34.807Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:34.904Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:43.646Z</t>
+  </si>
+  <si>
+    <t>frrr</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:53.486Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:15:57.423Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:16:02.563Z</t>
+  </si>
+  <si>
+    <t>/room/EA4C7814/103</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:16:07.367Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:16:13.522Z</t>
+  </si>
+  <si>
+    <t>/user/EA4C7814</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:16:21.013Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:16:24.234Z</t>
+  </si>
+  <si>
+    <t>2025-11-28T21:16:27.105Z</t>
   </si>
 </sst>
 </file>
@@ -1941,7 +2049,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K414"/>
+  <dimension ref="A1:K444"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -16434,6 +16542,1056 @@
         <v>19</v>
       </c>
     </row>
+    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>518</v>
+      </c>
+      <c r="B415" t="s">
+        <v>12</v>
+      </c>
+      <c r="C415" t="s">
+        <v>13</v>
+      </c>
+      <c r="D415" t="s">
+        <v>255</v>
+      </c>
+      <c r="E415">
+        <v>200</v>
+      </c>
+      <c r="F415" t="s">
+        <v>30</v>
+      </c>
+      <c r="G415" t="s">
+        <v>16</v>
+      </c>
+      <c r="H415" t="s">
+        <v>16</v>
+      </c>
+      <c r="I415" t="s">
+        <v>16</v>
+      </c>
+      <c r="J415" t="s">
+        <v>16</v>
+      </c>
+      <c r="K415" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>519</v>
+      </c>
+      <c r="B416" t="s">
+        <v>12</v>
+      </c>
+      <c r="C416" t="s">
+        <v>13</v>
+      </c>
+      <c r="D416" t="s">
+        <v>252</v>
+      </c>
+      <c r="E416">
+        <v>404</v>
+      </c>
+      <c r="F416" t="s">
+        <v>15</v>
+      </c>
+      <c r="G416" t="s">
+        <v>16</v>
+      </c>
+      <c r="H416" t="s">
+        <v>16</v>
+      </c>
+      <c r="I416" t="s">
+        <v>16</v>
+      </c>
+      <c r="J416" t="s">
+        <v>16</v>
+      </c>
+      <c r="K416" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>520</v>
+      </c>
+      <c r="B417" t="s">
+        <v>12</v>
+      </c>
+      <c r="C417" t="s">
+        <v>28</v>
+      </c>
+      <c r="D417" t="s">
+        <v>255</v>
+      </c>
+      <c r="E417">
+        <v>200</v>
+      </c>
+      <c r="F417" t="s">
+        <v>30</v>
+      </c>
+      <c r="G417" t="s">
+        <v>16</v>
+      </c>
+      <c r="H417" t="s">
+        <v>16</v>
+      </c>
+      <c r="I417" t="s">
+        <v>16</v>
+      </c>
+      <c r="J417" t="s">
+        <v>16</v>
+      </c>
+      <c r="K417" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>521</v>
+      </c>
+      <c r="B418" t="s">
+        <v>12</v>
+      </c>
+      <c r="C418" t="s">
+        <v>13</v>
+      </c>
+      <c r="D418" t="s">
+        <v>388</v>
+      </c>
+      <c r="E418">
+        <v>404</v>
+      </c>
+      <c r="F418" t="s">
+        <v>15</v>
+      </c>
+      <c r="G418" t="s">
+        <v>16</v>
+      </c>
+      <c r="H418" t="s">
+        <v>16</v>
+      </c>
+      <c r="I418" t="s">
+        <v>43</v>
+      </c>
+      <c r="J418" t="s">
+        <v>377</v>
+      </c>
+      <c r="K418" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>522</v>
+      </c>
+      <c r="B419" t="s">
+        <v>12</v>
+      </c>
+      <c r="C419" t="s">
+        <v>13</v>
+      </c>
+      <c r="D419" t="s">
+        <v>379</v>
+      </c>
+      <c r="E419">
+        <v>404</v>
+      </c>
+      <c r="F419" t="s">
+        <v>15</v>
+      </c>
+      <c r="G419" t="s">
+        <v>16</v>
+      </c>
+      <c r="H419" t="s">
+        <v>16</v>
+      </c>
+      <c r="I419" t="s">
+        <v>16</v>
+      </c>
+      <c r="J419" t="s">
+        <v>380</v>
+      </c>
+      <c r="K419" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>523</v>
+      </c>
+      <c r="B420" t="s">
+        <v>12</v>
+      </c>
+      <c r="C420" t="s">
+        <v>28</v>
+      </c>
+      <c r="D420" t="s">
+        <v>255</v>
+      </c>
+      <c r="E420">
+        <v>200</v>
+      </c>
+      <c r="F420" t="s">
+        <v>30</v>
+      </c>
+      <c r="G420" t="s">
+        <v>16</v>
+      </c>
+      <c r="H420" t="s">
+        <v>16</v>
+      </c>
+      <c r="I420" t="s">
+        <v>16</v>
+      </c>
+      <c r="J420" t="s">
+        <v>16</v>
+      </c>
+      <c r="K420" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>524</v>
+      </c>
+      <c r="B421" t="s">
+        <v>12</v>
+      </c>
+      <c r="C421" t="s">
+        <v>13</v>
+      </c>
+      <c r="D421" t="s">
+        <v>388</v>
+      </c>
+      <c r="E421">
+        <v>404</v>
+      </c>
+      <c r="F421" t="s">
+        <v>15</v>
+      </c>
+      <c r="G421" t="s">
+        <v>16</v>
+      </c>
+      <c r="H421" t="s">
+        <v>16</v>
+      </c>
+      <c r="I421" t="s">
+        <v>43</v>
+      </c>
+      <c r="J421" t="s">
+        <v>377</v>
+      </c>
+      <c r="K421" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>525</v>
+      </c>
+      <c r="B422" t="s">
+        <v>12</v>
+      </c>
+      <c r="C422" t="s">
+        <v>13</v>
+      </c>
+      <c r="D422" t="s">
+        <v>379</v>
+      </c>
+      <c r="E422">
+        <v>404</v>
+      </c>
+      <c r="F422" t="s">
+        <v>15</v>
+      </c>
+      <c r="G422" t="s">
+        <v>16</v>
+      </c>
+      <c r="H422" t="s">
+        <v>16</v>
+      </c>
+      <c r="I422" t="s">
+        <v>16</v>
+      </c>
+      <c r="J422" t="s">
+        <v>380</v>
+      </c>
+      <c r="K422" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>526</v>
+      </c>
+      <c r="B423" t="s">
+        <v>12</v>
+      </c>
+      <c r="C423" t="s">
+        <v>28</v>
+      </c>
+      <c r="D423" t="s">
+        <v>29</v>
+      </c>
+      <c r="E423">
+        <v>200</v>
+      </c>
+      <c r="F423" t="s">
+        <v>30</v>
+      </c>
+      <c r="G423" t="s">
+        <v>527</v>
+      </c>
+      <c r="H423" t="s">
+        <v>528</v>
+      </c>
+      <c r="I423" t="s">
+        <v>43</v>
+      </c>
+      <c r="J423" t="s">
+        <v>34</v>
+      </c>
+      <c r="K423" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>529</v>
+      </c>
+      <c r="B424" t="s">
+        <v>12</v>
+      </c>
+      <c r="C424" t="s">
+        <v>28</v>
+      </c>
+      <c r="D424" t="s">
+        <v>255</v>
+      </c>
+      <c r="E424">
+        <v>200</v>
+      </c>
+      <c r="F424" t="s">
+        <v>30</v>
+      </c>
+      <c r="G424" t="s">
+        <v>16</v>
+      </c>
+      <c r="H424" t="s">
+        <v>16</v>
+      </c>
+      <c r="I424" t="s">
+        <v>16</v>
+      </c>
+      <c r="J424" t="s">
+        <v>16</v>
+      </c>
+      <c r="K424" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>530</v>
+      </c>
+      <c r="B425" t="s">
+        <v>12</v>
+      </c>
+      <c r="C425" t="s">
+        <v>13</v>
+      </c>
+      <c r="D425" t="s">
+        <v>388</v>
+      </c>
+      <c r="E425">
+        <v>200</v>
+      </c>
+      <c r="F425" t="s">
+        <v>30</v>
+      </c>
+      <c r="G425" t="s">
+        <v>527</v>
+      </c>
+      <c r="H425" t="s">
+        <v>528</v>
+      </c>
+      <c r="I425" t="s">
+        <v>43</v>
+      </c>
+      <c r="J425" t="s">
+        <v>37</v>
+      </c>
+      <c r="K425" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>531</v>
+      </c>
+      <c r="B426" t="s">
+        <v>12</v>
+      </c>
+      <c r="C426" t="s">
+        <v>13</v>
+      </c>
+      <c r="D426" t="s">
+        <v>379</v>
+      </c>
+      <c r="E426">
+        <v>200</v>
+      </c>
+      <c r="F426" t="s">
+        <v>30</v>
+      </c>
+      <c r="G426" t="s">
+        <v>527</v>
+      </c>
+      <c r="H426" t="s">
+        <v>528</v>
+      </c>
+      <c r="I426" t="s">
+        <v>16</v>
+      </c>
+      <c r="J426" t="s">
+        <v>39</v>
+      </c>
+      <c r="K426" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="427" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>532</v>
+      </c>
+      <c r="B427" t="s">
+        <v>12</v>
+      </c>
+      <c r="C427" t="s">
+        <v>13</v>
+      </c>
+      <c r="D427" t="s">
+        <v>388</v>
+      </c>
+      <c r="E427">
+        <v>200</v>
+      </c>
+      <c r="F427" t="s">
+        <v>30</v>
+      </c>
+      <c r="G427" t="s">
+        <v>527</v>
+      </c>
+      <c r="H427" t="s">
+        <v>528</v>
+      </c>
+      <c r="I427" t="s">
+        <v>43</v>
+      </c>
+      <c r="J427" t="s">
+        <v>37</v>
+      </c>
+      <c r="K427" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>533</v>
+      </c>
+      <c r="B428" t="s">
+        <v>12</v>
+      </c>
+      <c r="C428" t="s">
+        <v>13</v>
+      </c>
+      <c r="D428" t="s">
+        <v>379</v>
+      </c>
+      <c r="E428">
+        <v>200</v>
+      </c>
+      <c r="F428" t="s">
+        <v>30</v>
+      </c>
+      <c r="G428" t="s">
+        <v>527</v>
+      </c>
+      <c r="H428" t="s">
+        <v>528</v>
+      </c>
+      <c r="I428" t="s">
+        <v>16</v>
+      </c>
+      <c r="J428" t="s">
+        <v>39</v>
+      </c>
+      <c r="K428" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>534</v>
+      </c>
+      <c r="B429" t="s">
+        <v>12</v>
+      </c>
+      <c r="C429" t="s">
+        <v>28</v>
+      </c>
+      <c r="D429" t="s">
+        <v>255</v>
+      </c>
+      <c r="E429">
+        <v>200</v>
+      </c>
+      <c r="F429" t="s">
+        <v>30</v>
+      </c>
+      <c r="G429" t="s">
+        <v>16</v>
+      </c>
+      <c r="H429" t="s">
+        <v>16</v>
+      </c>
+      <c r="I429" t="s">
+        <v>16</v>
+      </c>
+      <c r="J429" t="s">
+        <v>16</v>
+      </c>
+      <c r="K429" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>535</v>
+      </c>
+      <c r="B430" t="s">
+        <v>12</v>
+      </c>
+      <c r="C430" t="s">
+        <v>70</v>
+      </c>
+      <c r="D430" t="s">
+        <v>536</v>
+      </c>
+      <c r="E430">
+        <v>200</v>
+      </c>
+      <c r="F430" t="s">
+        <v>30</v>
+      </c>
+      <c r="G430" t="s">
+        <v>527</v>
+      </c>
+      <c r="H430" t="s">
+        <v>528</v>
+      </c>
+      <c r="I430" t="s">
+        <v>43</v>
+      </c>
+      <c r="J430" t="s">
+        <v>289</v>
+      </c>
+      <c r="K430" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>537</v>
+      </c>
+      <c r="B431" t="s">
+        <v>12</v>
+      </c>
+      <c r="C431" t="s">
+        <v>13</v>
+      </c>
+      <c r="D431" t="s">
+        <v>388</v>
+      </c>
+      <c r="E431">
+        <v>404</v>
+      </c>
+      <c r="F431" t="s">
+        <v>15</v>
+      </c>
+      <c r="G431" t="s">
+        <v>16</v>
+      </c>
+      <c r="H431" t="s">
+        <v>16</v>
+      </c>
+      <c r="I431" t="s">
+        <v>43</v>
+      </c>
+      <c r="J431" t="s">
+        <v>377</v>
+      </c>
+      <c r="K431" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>538</v>
+      </c>
+      <c r="B432" t="s">
+        <v>12</v>
+      </c>
+      <c r="C432" t="s">
+        <v>13</v>
+      </c>
+      <c r="D432" t="s">
+        <v>379</v>
+      </c>
+      <c r="E432">
+        <v>404</v>
+      </c>
+      <c r="F432" t="s">
+        <v>15</v>
+      </c>
+      <c r="G432" t="s">
+        <v>16</v>
+      </c>
+      <c r="H432" t="s">
+        <v>16</v>
+      </c>
+      <c r="I432" t="s">
+        <v>16</v>
+      </c>
+      <c r="J432" t="s">
+        <v>380</v>
+      </c>
+      <c r="K432" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="433" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>539</v>
+      </c>
+      <c r="B433" t="s">
+        <v>12</v>
+      </c>
+      <c r="C433" t="s">
+        <v>28</v>
+      </c>
+      <c r="D433" t="s">
+        <v>255</v>
+      </c>
+      <c r="E433">
+        <v>200</v>
+      </c>
+      <c r="F433" t="s">
+        <v>30</v>
+      </c>
+      <c r="G433" t="s">
+        <v>16</v>
+      </c>
+      <c r="H433" t="s">
+        <v>16</v>
+      </c>
+      <c r="I433" t="s">
+        <v>16</v>
+      </c>
+      <c r="J433" t="s">
+        <v>16</v>
+      </c>
+      <c r="K433" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>540</v>
+      </c>
+      <c r="B434" t="s">
+        <v>12</v>
+      </c>
+      <c r="C434" t="s">
+        <v>13</v>
+      </c>
+      <c r="D434" t="s">
+        <v>388</v>
+      </c>
+      <c r="E434">
+        <v>404</v>
+      </c>
+      <c r="F434" t="s">
+        <v>15</v>
+      </c>
+      <c r="G434" t="s">
+        <v>16</v>
+      </c>
+      <c r="H434" t="s">
+        <v>16</v>
+      </c>
+      <c r="I434" t="s">
+        <v>43</v>
+      </c>
+      <c r="J434" t="s">
+        <v>377</v>
+      </c>
+      <c r="K434" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>541</v>
+      </c>
+      <c r="B435" t="s">
+        <v>12</v>
+      </c>
+      <c r="C435" t="s">
+        <v>13</v>
+      </c>
+      <c r="D435" t="s">
+        <v>379</v>
+      </c>
+      <c r="E435">
+        <v>404</v>
+      </c>
+      <c r="F435" t="s">
+        <v>15</v>
+      </c>
+      <c r="G435" t="s">
+        <v>16</v>
+      </c>
+      <c r="H435" t="s">
+        <v>16</v>
+      </c>
+      <c r="I435" t="s">
+        <v>16</v>
+      </c>
+      <c r="J435" t="s">
+        <v>380</v>
+      </c>
+      <c r="K435" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="436" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>542</v>
+      </c>
+      <c r="B436" t="s">
+        <v>12</v>
+      </c>
+      <c r="C436" t="s">
+        <v>28</v>
+      </c>
+      <c r="D436" t="s">
+        <v>29</v>
+      </c>
+      <c r="E436">
+        <v>200</v>
+      </c>
+      <c r="F436" t="s">
+        <v>30</v>
+      </c>
+      <c r="G436" t="s">
+        <v>543</v>
+      </c>
+      <c r="H436" t="s">
+        <v>528</v>
+      </c>
+      <c r="I436" t="s">
+        <v>43</v>
+      </c>
+      <c r="J436" t="s">
+        <v>34</v>
+      </c>
+      <c r="K436" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="437" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>544</v>
+      </c>
+      <c r="B437" t="s">
+        <v>12</v>
+      </c>
+      <c r="C437" t="s">
+        <v>28</v>
+      </c>
+      <c r="D437" t="s">
+        <v>29</v>
+      </c>
+      <c r="E437">
+        <v>200</v>
+      </c>
+      <c r="F437" t="s">
+        <v>30</v>
+      </c>
+      <c r="G437" t="s">
+        <v>543</v>
+      </c>
+      <c r="H437" t="s">
+        <v>528</v>
+      </c>
+      <c r="I437" t="s">
+        <v>79</v>
+      </c>
+      <c r="J437" t="s">
+        <v>41</v>
+      </c>
+      <c r="K437" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>545</v>
+      </c>
+      <c r="B438" t="s">
+        <v>12</v>
+      </c>
+      <c r="C438" t="s">
+        <v>28</v>
+      </c>
+      <c r="D438" t="s">
+        <v>255</v>
+      </c>
+      <c r="E438">
+        <v>200</v>
+      </c>
+      <c r="F438" t="s">
+        <v>30</v>
+      </c>
+      <c r="G438" t="s">
+        <v>16</v>
+      </c>
+      <c r="H438" t="s">
+        <v>16</v>
+      </c>
+      <c r="I438" t="s">
+        <v>16</v>
+      </c>
+      <c r="J438" t="s">
+        <v>16</v>
+      </c>
+      <c r="K438" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="439" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>546</v>
+      </c>
+      <c r="B439" t="s">
+        <v>12</v>
+      </c>
+      <c r="C439" t="s">
+        <v>70</v>
+      </c>
+      <c r="D439" t="s">
+        <v>547</v>
+      </c>
+      <c r="E439">
+        <v>200</v>
+      </c>
+      <c r="F439" t="s">
+        <v>30</v>
+      </c>
+      <c r="G439" t="s">
+        <v>543</v>
+      </c>
+      <c r="H439" t="s">
+        <v>528</v>
+      </c>
+      <c r="I439" t="s">
+        <v>79</v>
+      </c>
+      <c r="J439" t="s">
+        <v>72</v>
+      </c>
+      <c r="K439" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="440" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>548</v>
+      </c>
+      <c r="B440" t="s">
+        <v>12</v>
+      </c>
+      <c r="C440" t="s">
+        <v>28</v>
+      </c>
+      <c r="D440" t="s">
+        <v>255</v>
+      </c>
+      <c r="E440">
+        <v>200</v>
+      </c>
+      <c r="F440" t="s">
+        <v>30</v>
+      </c>
+      <c r="G440" t="s">
+        <v>16</v>
+      </c>
+      <c r="H440" t="s">
+        <v>16</v>
+      </c>
+      <c r="I440" t="s">
+        <v>16</v>
+      </c>
+      <c r="J440" t="s">
+        <v>16</v>
+      </c>
+      <c r="K440" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="441" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>549</v>
+      </c>
+      <c r="B441" t="s">
+        <v>12</v>
+      </c>
+      <c r="C441" t="s">
+        <v>70</v>
+      </c>
+      <c r="D441" t="s">
+        <v>550</v>
+      </c>
+      <c r="E441">
+        <v>200</v>
+      </c>
+      <c r="F441" t="s">
+        <v>30</v>
+      </c>
+      <c r="G441" t="s">
+        <v>543</v>
+      </c>
+      <c r="H441" t="s">
+        <v>528</v>
+      </c>
+      <c r="I441" t="s">
+        <v>16</v>
+      </c>
+      <c r="J441" t="s">
+        <v>77</v>
+      </c>
+      <c r="K441" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="442" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>551</v>
+      </c>
+      <c r="B442" t="s">
+        <v>12</v>
+      </c>
+      <c r="C442" t="s">
+        <v>28</v>
+      </c>
+      <c r="D442" t="s">
+        <v>255</v>
+      </c>
+      <c r="E442">
+        <v>200</v>
+      </c>
+      <c r="F442" t="s">
+        <v>30</v>
+      </c>
+      <c r="G442" t="s">
+        <v>16</v>
+      </c>
+      <c r="H442" t="s">
+        <v>16</v>
+      </c>
+      <c r="I442" t="s">
+        <v>16</v>
+      </c>
+      <c r="J442" t="s">
+        <v>16</v>
+      </c>
+      <c r="K442" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="443" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>552</v>
+      </c>
+      <c r="B443" t="s">
+        <v>12</v>
+      </c>
+      <c r="C443" t="s">
+        <v>70</v>
+      </c>
+      <c r="D443" t="s">
+        <v>408</v>
+      </c>
+      <c r="E443">
+        <v>200</v>
+      </c>
+      <c r="F443" t="s">
+        <v>30</v>
+      </c>
+      <c r="G443" t="s">
+        <v>511</v>
+      </c>
+      <c r="H443" t="s">
+        <v>400</v>
+      </c>
+      <c r="I443" t="s">
+        <v>16</v>
+      </c>
+      <c r="J443" t="s">
+        <v>77</v>
+      </c>
+      <c r="K443" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="444" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>553</v>
+      </c>
+      <c r="B444" t="s">
+        <v>12</v>
+      </c>
+      <c r="C444" t="s">
+        <v>28</v>
+      </c>
+      <c r="D444" t="s">
+        <v>255</v>
+      </c>
+      <c r="E444">
+        <v>200</v>
+      </c>
+      <c r="F444" t="s">
+        <v>30</v>
+      </c>
+      <c r="G444" t="s">
+        <v>16</v>
+      </c>
+      <c r="H444" t="s">
+        <v>16</v>
+      </c>
+      <c r="I444" t="s">
+        <v>16</v>
+      </c>
+      <c r="J444" t="s">
+        <v>16</v>
+      </c>
+      <c r="K444" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Remove servo lock logic from access control example
Eliminated all code related to servo-based door control from both main and hardware UI files, including setup, helpers, and status handling. This refactor simplifies the project to use only buzzer and LED indicators, removing unused servo dependencies and logic.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/logs.xlsx
+++ b/Server/rfid-server-DBS-Http/logs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13851" uniqueCount="1520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14111" uniqueCount="1547">
   <si>
     <t>Timestamp</t>
   </si>
@@ -4571,6 +4571,87 @@
   </si>
   <si>
     <t>2025-11-29T23:42:07.152Z</t>
+  </si>
+  <si>
+    <t>2025-11-29T23:42:12.152Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:31.838Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:32.004Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:42.002Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:45.608Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:47.226Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:50.060Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:50.151Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:50.557Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:52.604Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:55.935Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:56.012Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:56.750Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:59.482Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:11:59.589Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:00.828Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:00.897Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:01.743Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:01.961Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:02.064Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:06.750Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:07.739Z</t>
+  </si>
+  <si>
+    <t>/room/6BF02F00/106</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:11.741Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:16.764Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:21.753Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:26.751Z</t>
   </si>
 </sst>
 </file>
@@ -4947,7 +5028,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1385"/>
+  <dimension ref="A1:K1411"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -53425,6 +53506,916 @@
         <v>250</v>
       </c>
     </row>
+    <row r="1386" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1386" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B1386" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1386" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1386" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1386">
+        <v>200</v>
+      </c>
+      <c r="F1386" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1386" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1386" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1386" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1386" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1386" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1387" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B1387" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1387" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1387" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1387">
+        <v>404</v>
+      </c>
+      <c r="F1387" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1387" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1387" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1387" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1387" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1387" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1388" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B1388" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1388" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1388" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1388">
+        <v>404</v>
+      </c>
+      <c r="F1388" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1388" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1388" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1388" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1388" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1388" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1389" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B1389" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1389" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1389" t="s">
+        <v>252</v>
+      </c>
+      <c r="E1389">
+        <v>404</v>
+      </c>
+      <c r="F1389" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1389" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1389" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1389" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1389" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1389" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1390" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B1390" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1390" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1390" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1390">
+        <v>200</v>
+      </c>
+      <c r="F1390" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1390" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1390" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1390" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1390" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1390" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1391" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B1391" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1391" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1391" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1391">
+        <v>200</v>
+      </c>
+      <c r="F1391" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1391" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1391" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1391" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1391" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1391" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1392" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B1392" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1392" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1392" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1392">
+        <v>200</v>
+      </c>
+      <c r="F1392" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1392" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1392" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1392" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1392" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1392" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1393" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B1393" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1393" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1393" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1393">
+        <v>200</v>
+      </c>
+      <c r="F1393" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1393" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1393" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1393" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1393" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1393" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1394" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B1394" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1394" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1394" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1394">
+        <v>200</v>
+      </c>
+      <c r="F1394" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1394" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1394" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1394" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1394" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1394" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1395" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B1395" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1395" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1395" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1395">
+        <v>200</v>
+      </c>
+      <c r="F1395" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1395" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1395" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1395" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1395" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1395" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1396" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B1396" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1396" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1396" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1396">
+        <v>200</v>
+      </c>
+      <c r="F1396" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1396" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1396" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1396" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1396" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1396" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1397" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B1397" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1397" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1397" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1397">
+        <v>200</v>
+      </c>
+      <c r="F1397" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1397" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1397" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1397" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1397" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1397" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1398" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B1398" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1398" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1398" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1398">
+        <v>200</v>
+      </c>
+      <c r="F1398" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1398" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1398" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1398" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1398" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1398" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1399" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B1399" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1399" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1399" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1399">
+        <v>200</v>
+      </c>
+      <c r="F1399" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1399" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1399" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1399" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1399" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1399" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1400" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B1400" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1400" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1400" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1400">
+        <v>200</v>
+      </c>
+      <c r="F1400" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1400" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1400" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1400" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1400" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1400" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1401" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B1401" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1401" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1401" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1401">
+        <v>200</v>
+      </c>
+      <c r="F1401" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1401" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1401" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1401" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1401" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1401" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1402" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B1402" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1402" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1402" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1402">
+        <v>200</v>
+      </c>
+      <c r="F1402" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1402" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1402" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1402" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1402" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1402" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1403" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B1403" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1403" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1403" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1403">
+        <v>200</v>
+      </c>
+      <c r="F1403" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1403" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1403" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1403" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1403" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1403" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1404" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B1404" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1404" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1404" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1404">
+        <v>200</v>
+      </c>
+      <c r="F1404" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1404" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1404" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1404" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1404" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1404" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1405" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B1405" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1405" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1405" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1405">
+        <v>200</v>
+      </c>
+      <c r="F1405" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1405" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1405" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1405" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1405" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1405" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1406" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B1406" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1406" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1406" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1406">
+        <v>200</v>
+      </c>
+      <c r="F1406" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1406" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1406" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1406" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1406" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1406" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1407" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B1407" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1407" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1407" t="s">
+        <v>1542</v>
+      </c>
+      <c r="E1407">
+        <v>200</v>
+      </c>
+      <c r="F1407" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1407" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1407" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1407" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1407" t="s">
+        <v>289</v>
+      </c>
+      <c r="K1407" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1408" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B1408" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1408" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1408" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1408">
+        <v>200</v>
+      </c>
+      <c r="F1408" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1408" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1408" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1408" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1408" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1408" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1409" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B1409" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1409" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1409" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1409">
+        <v>200</v>
+      </c>
+      <c r="F1409" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1409" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1409" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1409" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1409" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1409" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1410" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B1410" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1410" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1410" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1410">
+        <v>200</v>
+      </c>
+      <c r="F1410" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1410" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1410" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1410" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1410" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1410" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1411" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B1411" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1411" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1411" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1411">
+        <v>200</v>
+      </c>
+      <c r="F1411" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1411" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1411" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1411" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1411" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1411" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update logs.xlsx with latest log data
The logs.xlsx file has been updated to include new or modified log entries. No changes to code or logic were made.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/logs.xlsx
+++ b/Server/rfid-server-DBS-Http/logs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14111" uniqueCount="1547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14221" uniqueCount="1558">
   <si>
     <t>Timestamp</t>
   </si>
@@ -4652,6 +4652,39 @@
   </si>
   <si>
     <t>2025-11-30T02:12:26.751Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:31.770Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:41.669Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:42.571Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:46.805Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:52.602Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:12:57.787Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:15:10.742Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:21:29.510Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:23:08.488Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:23:13.595Z</t>
+  </si>
+  <si>
+    <t>2025-11-30T02:28:43.927Z</t>
   </si>
 </sst>
 </file>
@@ -5028,7 +5061,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1411"/>
+  <dimension ref="A1:K1422"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -54416,6 +54449,391 @@
         <v>250</v>
       </c>
     </row>
+    <row r="1412" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1412" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B1412" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1412" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1412" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1412">
+        <v>200</v>
+      </c>
+      <c r="F1412" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1412" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1412" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1412" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1412" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1412" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1413" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B1413" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1413" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1413" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1413">
+        <v>200</v>
+      </c>
+      <c r="F1413" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1413" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1413" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1413" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1413" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1413" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1414" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B1414" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1414" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1414" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1414">
+        <v>200</v>
+      </c>
+      <c r="F1414" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1414" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1414" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1414" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1414" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1414" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1415" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B1415" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1415" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1415" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1415">
+        <v>200</v>
+      </c>
+      <c r="F1415" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1415" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1415" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1415" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1415" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1415" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1416" t="s">
+        <v>1551</v>
+      </c>
+      <c r="B1416" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1416" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1416" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1416">
+        <v>200</v>
+      </c>
+      <c r="F1416" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1416" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1416" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1416" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1416" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1416" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1417" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B1417" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1417" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1417" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1417">
+        <v>200</v>
+      </c>
+      <c r="F1417" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1417" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1417" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1417" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1417" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1417" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1418" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B1418" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1418" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1418" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1418">
+        <v>200</v>
+      </c>
+      <c r="F1418" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1418" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1418" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1418" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1418" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1418" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1419" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B1419" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1419" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1419" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1419">
+        <v>200</v>
+      </c>
+      <c r="F1419" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1419" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1419" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1419" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1419" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1419" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1420" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B1420" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1420" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1420" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1420">
+        <v>200</v>
+      </c>
+      <c r="F1420" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1420" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1420" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1420" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1420" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1420" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1421" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B1421" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1421" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1421" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1421">
+        <v>200</v>
+      </c>
+      <c r="F1421" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1421" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1421" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1421" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1421" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1421" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1422" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B1422" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1422" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1422" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1422">
+        <v>200</v>
+      </c>
+      <c r="F1422" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1422" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1422" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1422" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1422" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1422" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Add ESP32 access control project files and diagrams
Added project documentation, architecture diagrams, firmware module diagrams, backend interaction flows, indicator state machines, registration and access flows, risk map, and tech stack files for the ESP32 RFID access control system. Also included presentation assets, example source code, and updated hardware UI and instruction files.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS-Http/logs.xlsx
+++ b/Server/rfid-server-DBS-Http/logs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14221" uniqueCount="1558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14961" uniqueCount="1633">
   <si>
     <t>Timestamp</t>
   </si>
@@ -4685,6 +4685,231 @@
   </si>
   <si>
     <t>2025-11-30T02:28:43.927Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:04:21.580Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:04:21.880Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:04:46.629Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:04:46.714Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:05:05.511Z</t>
+  </si>
+  <si>
+    <t>/user/EA4C7814?roomID=102</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:05:05.562Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:05:23.060Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:05:23.532Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:05:32.738Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:05:34.858Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:05:34.964Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:05:35.985Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:05:36.182Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:07.980Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:29.529Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:33.397Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:33.586Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:35.058Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:36.564Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:36.639Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:39.616Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:39.696Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:40.058Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:42.274Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:42.448Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:45.055Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:50.053Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:12:55.053Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:13:00.047Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:13:05.053Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:13:10.050Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:13:15.984Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:13:20.992Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:13:25.986Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:15:47.928Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:19:30.213Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:23:44.436Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:27:35.437Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:29:14.587Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:29:15.051Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:29:20.993Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:32:10.443Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:32:15.994Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:36:29.406Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:41:08.385Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:46:02.602Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:50:08.134Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:53:56.452Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T18:57:36.611Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:01:47.003Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:05:36.487Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:09:45.603Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:14:04.732Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:17:51.921Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:22:32.907Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:26:36.294Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:32:01.554Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:35:51.632Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:39:54.382Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:44:05.255Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:48:04.292Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:51:49.829Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T19:56:13.290Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T20:00:57.579Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T20:06:28.587Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T20:10:34.420Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T20:14:43.863Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T20:18:59.413Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T20:23:10.686Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T20:28:56.805Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T20:32:42.597Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T20:37:14.527Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T20:41:35.775Z</t>
+  </si>
+  <si>
+    <t>2025-12-01T20:42:47.968Z</t>
   </si>
 </sst>
 </file>
@@ -5061,7 +5286,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1422"/>
+  <dimension ref="A1:K1496"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -54834,6 +55059,2596 @@
         <v>250</v>
       </c>
     </row>
+    <row r="1423" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1423" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B1423" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1423" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1423" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1423">
+        <v>404</v>
+      </c>
+      <c r="F1423" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1423" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1423" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1423" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1423" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1423" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1424" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B1424" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1424" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1424" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1424">
+        <v>404</v>
+      </c>
+      <c r="F1424" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1424" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1424" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1424" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1424" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1424" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1425" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B1425" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1425" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1425" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1425">
+        <v>404</v>
+      </c>
+      <c r="F1425" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1425" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1425" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1425" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1425" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1425" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1426" t="s">
+        <v>1561</v>
+      </c>
+      <c r="B1426" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1426" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1426" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1426">
+        <v>404</v>
+      </c>
+      <c r="F1426" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1426" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1426" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1426" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1426" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1426" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1427" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B1427" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1427" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1427" t="s">
+        <v>1563</v>
+      </c>
+      <c r="E1427">
+        <v>404</v>
+      </c>
+      <c r="F1427" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1427" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1427" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1427" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1427" t="s">
+        <v>377</v>
+      </c>
+      <c r="K1427" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1428" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B1428" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1428" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1428" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1428">
+        <v>404</v>
+      </c>
+      <c r="F1428" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1428" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1428" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1428" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1428" t="s">
+        <v>380</v>
+      </c>
+      <c r="K1428" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1429" t="s">
+        <v>1565</v>
+      </c>
+      <c r="B1429" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1429" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1429" t="s">
+        <v>255</v>
+      </c>
+      <c r="E1429">
+        <v>200</v>
+      </c>
+      <c r="F1429" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1429" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1429" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1429" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1429" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1429" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1430" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B1430" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1430" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1430" t="s">
+        <v>252</v>
+      </c>
+      <c r="E1430">
+        <v>404</v>
+      </c>
+      <c r="F1430" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1430" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1430" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1430" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1430" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1430" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1431" t="s">
+        <v>1567</v>
+      </c>
+      <c r="B1431" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1431" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1431" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1431">
+        <v>200</v>
+      </c>
+      <c r="F1431" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1431" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1431" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1431" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1431" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1431" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1432" t="s">
+        <v>1568</v>
+      </c>
+      <c r="B1432" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1432" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1432" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1432">
+        <v>200</v>
+      </c>
+      <c r="F1432" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1432" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1432" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1432" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1432" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1432" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1433" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B1433" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1433" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1433" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1433">
+        <v>200</v>
+      </c>
+      <c r="F1433" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1433" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1433" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1433" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1433" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1433" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1434" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B1434" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1434" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1434" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1434">
+        <v>200</v>
+      </c>
+      <c r="F1434" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1434" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1434" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1434" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1434" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1434" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1435" t="s">
+        <v>1571</v>
+      </c>
+      <c r="B1435" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1435" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1435" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1435">
+        <v>200</v>
+      </c>
+      <c r="F1435" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1435" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1435" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1435" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1435" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1435" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1436" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B1436" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1436" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1436" t="s">
+        <v>255</v>
+      </c>
+      <c r="E1436">
+        <v>401</v>
+      </c>
+      <c r="F1436" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1436" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1436" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1436" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1436" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1436" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1437" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B1437" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1437" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1437" t="s">
+        <v>255</v>
+      </c>
+      <c r="E1437">
+        <v>200</v>
+      </c>
+      <c r="F1437" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1437" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1437" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1437" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1437" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1437" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1438" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B1438" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1438" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1438" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1438">
+        <v>200</v>
+      </c>
+      <c r="F1438" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1438" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1438" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1438" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1438" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1438" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1439" t="s">
+        <v>1575</v>
+      </c>
+      <c r="B1439" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1439" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1439" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1439">
+        <v>200</v>
+      </c>
+      <c r="F1439" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1439" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1439" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1439" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1439" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1439" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1440" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B1440" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1440" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1440" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1440">
+        <v>200</v>
+      </c>
+      <c r="F1440" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1440" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1440" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1440" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1440" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1440" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1441" t="s">
+        <v>1577</v>
+      </c>
+      <c r="B1441" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1441" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1441" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1441">
+        <v>200</v>
+      </c>
+      <c r="F1441" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1441" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1441" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1441" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1441" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1441" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1442" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B1442" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1442" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1442" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1442">
+        <v>200</v>
+      </c>
+      <c r="F1442" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1442" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1442" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1442" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1442" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1442" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1443" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B1443" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1443" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1443" t="s">
+        <v>1563</v>
+      </c>
+      <c r="E1443">
+        <v>404</v>
+      </c>
+      <c r="F1443" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1443" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1443" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1443" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1443" t="s">
+        <v>377</v>
+      </c>
+      <c r="K1443" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1444" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B1444" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1444" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1444" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1444">
+        <v>404</v>
+      </c>
+      <c r="F1444" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1444" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1444" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1444" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1444" t="s">
+        <v>380</v>
+      </c>
+      <c r="K1444" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1445" t="s">
+        <v>1581</v>
+      </c>
+      <c r="B1445" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1445" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1445" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1445">
+        <v>200</v>
+      </c>
+      <c r="F1445" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1445" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1445" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1445" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1445" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1445" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1446" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B1446" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1446" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1446" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1446">
+        <v>200</v>
+      </c>
+      <c r="F1446" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1446" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1446" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1446" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1446" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1446" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1447" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B1447" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1447" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1447" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1447">
+        <v>200</v>
+      </c>
+      <c r="F1447" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1447" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1447" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1447" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1447" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1447" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1448" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B1448" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1448" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1448" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1448">
+        <v>200</v>
+      </c>
+      <c r="F1448" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1448" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1448" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1448" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1448" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1448" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1449" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B1449" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1449" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1449" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1449">
+        <v>200</v>
+      </c>
+      <c r="F1449" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1449" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1449" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1449" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1449" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1449" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1450" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B1450" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1450" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1450" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1450">
+        <v>200</v>
+      </c>
+      <c r="F1450" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1450" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1450" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1450" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1450" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1450" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1451" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B1451" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1451" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1451" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1451">
+        <v>200</v>
+      </c>
+      <c r="F1451" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1451" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1451" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1451" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1451" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1451" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1452" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B1452" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1452" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1452" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1452">
+        <v>200</v>
+      </c>
+      <c r="F1452" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1452" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1452" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1452" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1452" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1452" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1453" t="s">
+        <v>1589</v>
+      </c>
+      <c r="B1453" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1453" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1453" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1453">
+        <v>200</v>
+      </c>
+      <c r="F1453" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1453" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1453" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1453" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1453" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1453" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1454" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B1454" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1454" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1454" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1454">
+        <v>200</v>
+      </c>
+      <c r="F1454" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1454" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1454" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1454" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1454" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1454" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1455" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B1455" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1455" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1455" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1455">
+        <v>200</v>
+      </c>
+      <c r="F1455" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1455" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1455" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1455" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1455" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1455" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1456" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B1456" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1456" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1456" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1456">
+        <v>200</v>
+      </c>
+      <c r="F1456" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1456" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1456" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1456" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1456" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1456" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1457" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B1457" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1457" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1457" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1457">
+        <v>200</v>
+      </c>
+      <c r="F1457" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1457" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1457" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1457" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1457" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1457" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1458" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B1458" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1458" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1458" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1458">
+        <v>200</v>
+      </c>
+      <c r="F1458" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1458" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1458" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1458" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1458" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1458" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1459" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B1459" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1459" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1459" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1459">
+        <v>200</v>
+      </c>
+      <c r="F1459" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1459" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1459" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1459" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1459" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1459" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1460" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B1460" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1460" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1460" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1460">
+        <v>200</v>
+      </c>
+      <c r="F1460" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1460" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1460" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1460" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1460" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1460" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1461" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B1461" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1461" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1461" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1461">
+        <v>200</v>
+      </c>
+      <c r="F1461" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1461" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1461" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1461" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1461" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1461" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1462" t="s">
+        <v>1598</v>
+      </c>
+      <c r="B1462" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1462" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1462" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1462">
+        <v>200</v>
+      </c>
+      <c r="F1462" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1462" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1462" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1462" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1462" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1462" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1463" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B1463" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1463" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1463" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1463">
+        <v>200</v>
+      </c>
+      <c r="F1463" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1463" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1463" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1463" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1463" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1463" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1464" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B1464" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1464" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1464" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1464">
+        <v>200</v>
+      </c>
+      <c r="F1464" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1464" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1464" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1464" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1464" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1464" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1465" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B1465" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1465" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1465" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1465">
+        <v>200</v>
+      </c>
+      <c r="F1465" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1465" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1465" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1465" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1465" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1465" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1466" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B1466" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1466" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1466" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1466">
+        <v>200</v>
+      </c>
+      <c r="F1466" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1466" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1466" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1466" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1466" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1466" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1467" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B1467" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1467" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1467" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1467">
+        <v>200</v>
+      </c>
+      <c r="F1467" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1467" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1467" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1467" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1467" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1467" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1468" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B1468" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1468" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1468" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1468">
+        <v>200</v>
+      </c>
+      <c r="F1468" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1468" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1468" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1468" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1468" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1468" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1469" t="s">
+        <v>1605</v>
+      </c>
+      <c r="B1469" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1469" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1469" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1469">
+        <v>200</v>
+      </c>
+      <c r="F1469" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1469" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1469" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1469" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1469" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1469" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1470" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B1470" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1470" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1470" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1470">
+        <v>200</v>
+      </c>
+      <c r="F1470" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1470" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1470" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1470" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1470" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1470" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1471" t="s">
+        <v>1607</v>
+      </c>
+      <c r="B1471" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1471" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1471" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1471">
+        <v>200</v>
+      </c>
+      <c r="F1471" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1471" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1471" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1471" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1471" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1471" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1472" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B1472" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1472" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1472" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1472">
+        <v>200</v>
+      </c>
+      <c r="F1472" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1472" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1472" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1472" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1472" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1472" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1473" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B1473" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1473" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1473" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1473">
+        <v>200</v>
+      </c>
+      <c r="F1473" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1473" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1473" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1473" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1473" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1473" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1474" t="s">
+        <v>1610</v>
+      </c>
+      <c r="B1474" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1474" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1474" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1474">
+        <v>200</v>
+      </c>
+      <c r="F1474" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1474" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1474" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1474" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1474" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1474" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1475" t="s">
+        <v>1611</v>
+      </c>
+      <c r="B1475" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1475" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1475" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1475">
+        <v>200</v>
+      </c>
+      <c r="F1475" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1475" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1475" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1475" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1475" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1475" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1476" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B1476" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1476" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1476" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1476">
+        <v>200</v>
+      </c>
+      <c r="F1476" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1476" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1476" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1476" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1476" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1476" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1477" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B1477" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1477" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1477" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1477">
+        <v>200</v>
+      </c>
+      <c r="F1477" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1477" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1477" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1477" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1477" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1477" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1478" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B1478" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1478" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1478" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1478">
+        <v>200</v>
+      </c>
+      <c r="F1478" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1478" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1478" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1478" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1478" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1478" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1479" t="s">
+        <v>1615</v>
+      </c>
+      <c r="B1479" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1479" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1479" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1479">
+        <v>200</v>
+      </c>
+      <c r="F1479" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1479" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1479" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1479" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1479" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1479" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1480" t="s">
+        <v>1616</v>
+      </c>
+      <c r="B1480" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1480" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1480" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1480">
+        <v>200</v>
+      </c>
+      <c r="F1480" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1480" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1480" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1480" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1480" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1480" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1481" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B1481" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1481" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1481" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1481">
+        <v>200</v>
+      </c>
+      <c r="F1481" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1481" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1481" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1481" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1481" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1481" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1482" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B1482" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1482" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1482" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1482">
+        <v>200</v>
+      </c>
+      <c r="F1482" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1482" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1482" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1482" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1482" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1482" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1483" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B1483" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1483" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1483" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1483">
+        <v>200</v>
+      </c>
+      <c r="F1483" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1483" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1483" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1483" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1483" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1483" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1484" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B1484" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1484" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1484" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1484">
+        <v>200</v>
+      </c>
+      <c r="F1484" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1484" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1484" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1484" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1484" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1484" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1485" t="s">
+        <v>1621</v>
+      </c>
+      <c r="B1485" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1485" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1485" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1485">
+        <v>200</v>
+      </c>
+      <c r="F1485" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1485" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1485" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1485" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1485" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1485" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1486" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B1486" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1486" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1486" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1486">
+        <v>200</v>
+      </c>
+      <c r="F1486" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1486" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1486" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1486" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1486" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1486" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1487" t="s">
+        <v>1623</v>
+      </c>
+      <c r="B1487" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1487" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1487" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1487">
+        <v>200</v>
+      </c>
+      <c r="F1487" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1487" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1487" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1487" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1487" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1487" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1488" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B1488" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1488" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1488" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1488">
+        <v>200</v>
+      </c>
+      <c r="F1488" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1488" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1488" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1488" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1488" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1488" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1489" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B1489" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1489" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1489" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1489">
+        <v>200</v>
+      </c>
+      <c r="F1489" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1489" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1489" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1489" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1489" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1489" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1490" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B1490" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1490" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1490" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1490">
+        <v>200</v>
+      </c>
+      <c r="F1490" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1490" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1490" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1490" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1490" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1490" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1491" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B1491" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1491" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1491" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1491">
+        <v>200</v>
+      </c>
+      <c r="F1491" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1491" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1491" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1491" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1491" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1491" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1492" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B1492" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1492" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1492" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1492">
+        <v>200</v>
+      </c>
+      <c r="F1492" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1492" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1492" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1492" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1492" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1492" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1493" t="s">
+        <v>1629</v>
+      </c>
+      <c r="B1493" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1493" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1493" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1493">
+        <v>200</v>
+      </c>
+      <c r="F1493" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1493" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1493" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1493" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1493" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1493" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1494" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B1494" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1494" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1494" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1494">
+        <v>200</v>
+      </c>
+      <c r="F1494" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1494" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1494" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1494" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1494" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1494" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1495" t="s">
+        <v>1631</v>
+      </c>
+      <c r="B1495" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1495" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1495" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1495">
+        <v>200</v>
+      </c>
+      <c r="F1495" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1495" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1495" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1495" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1495" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1495" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1496" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B1496" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1496" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1496" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1496">
+        <v>200</v>
+      </c>
+      <c r="F1496" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1496" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1496" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1496" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1496" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1496" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>